<commit_message>
Updated RSI formula .
</commit_message>
<xml_diff>
--- a/buy_low.xlsx
+++ b/buy_low.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="V20" sheetId="1" state="visible" r:id="rId1"/>
@@ -847,8 +847,8 @@
   </sheetPr>
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -923,31 +923,31 @@
         </is>
       </c>
       <c r="B2" s="5" t="n">
-        <v>2410.699951171875</v>
+        <v>2428.699951171875</v>
       </c>
       <c r="C2" s="5" t="n">
-        <v>-0.08082196965174537</v>
+        <v>0.210424711591517</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>2479.385506591797</v>
+        <v>2477.690006103516</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>-2.770265262796433</v>
+        <v>-1.977247145968995</v>
       </c>
       <c r="F2" s="5" t="n">
-        <v>2559.169995117188</v>
+        <v>2556.009995117187</v>
       </c>
       <c r="G2" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="5" t="n">
-        <v>12.32752498561443</v>
+        <v>37.50138741285078</v>
       </c>
       <c r="I2" s="5" t="n">
         <v>1</v>
       </c>
       <c r="J2" s="6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -957,31 +957,31 @@
         </is>
       </c>
       <c r="B3" s="5" t="n">
-        <v>3418.5</v>
+        <v>3429.89990234375</v>
       </c>
       <c r="C3" s="5" t="n">
-        <v>1.16299862085687</v>
+        <v>0.01603232892073425</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>3319.634499511719</v>
+        <v>3320.408999023437</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>2.978204392767434</v>
+        <v>3.297512545969934</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>3379.307998046875</v>
+        <v>3388.372998046875</v>
       </c>
       <c r="G3" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H3" s="5" t="n">
-        <v>44.84287247304366</v>
+        <v>55.40127060757342</v>
       </c>
       <c r="I3" s="5" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="J3" s="6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
@@ -991,31 +991,31 @@
         </is>
       </c>
       <c r="B4" s="5" t="n">
-        <v>1465.099975585938</v>
+        <v>1477.449951171875</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>1.471759556693297</v>
+        <v>-0.09805079574340958</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>1425.449003295898</v>
+        <v>1424.279752807617</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>2.781647901703873</v>
+        <v>3.733128850525743</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>1376.887993164062</v>
+        <v>1385.307993164063</v>
       </c>
       <c r="G4" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H4" s="5" t="n">
-        <v>73.82618430327139</v>
+        <v>71.23688122189265</v>
       </c>
       <c r="I4" s="5" t="n">
         <v>19</v>
       </c>
       <c r="J4" s="6" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -1025,31 +1025,31 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>1584.550048828125</v>
+        <v>1595.5</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>0.6255221922703225</v>
+        <v>1.308017986322763</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>1629.381003417969</v>
+        <v>1628.977753295899</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>-2.751410167161724</v>
+        <v>-2.055138765901698</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>1639.787998046875</v>
+        <v>1637.614997558594</v>
       </c>
       <c r="G5" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H5" s="5" t="n">
-        <v>38.83005312295278</v>
+        <v>47.24302965236613</v>
       </c>
       <c r="I5" s="5" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J5" s="6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -1059,31 +1059,31 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>967.3499755859375</v>
+        <v>957.5</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>-0.139365810269565</v>
+        <v>-1.125570439824974</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>912.8255029296874</v>
+        <v>913.2880032348633</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>5.973153957821655</v>
+        <v>4.840969837393899</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>964.5270031738281</v>
+        <v>966.0260034179687</v>
       </c>
       <c r="G6" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H6" s="5" t="n">
-        <v>56.68952780973778</v>
+        <v>44.49949446185531</v>
       </c>
       <c r="I6" s="5" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="J6" s="6" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
@@ -1093,31 +1093,31 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>575.5499877929688</v>
+        <v>570.5</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>1.053463283047429</v>
+        <v>-0.4363001745200656</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>573.32724899292</v>
+        <v>573.0507490539551</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.3876911142725439</v>
+        <v>-0.4451174801125552</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>584.3449963378906</v>
+        <v>584.9819970703124</v>
       </c>
       <c r="G7" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>61.40757496511604</v>
+        <v>45.58455772357443</v>
       </c>
       <c r="I7" s="5" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="J7" s="6" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -1127,28 +1127,28 @@
         </is>
       </c>
       <c r="B8" s="5" t="n">
-        <v>2501.39990234375</v>
+        <v>2523.5</v>
       </c>
       <c r="C8" s="5" t="n">
-        <v>-0.135745225890016</v>
+        <v>0.6561476975525116</v>
       </c>
       <c r="D8" s="5" t="n">
-        <v>2584.489011230469</v>
+        <v>2584.952510986328</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>-3.214914380586214</v>
+        <v>-2.377316825943539</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>2602.45001953125</v>
+        <v>2597.187016601562</v>
       </c>
       <c r="G8" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>39.98732260124183</v>
+        <v>42.47878738357827</v>
       </c>
       <c r="I8" s="5" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J8" s="6" t="n">
         <v>1</v>
@@ -1161,31 +1161,31 @@
         </is>
       </c>
       <c r="B9" s="5" t="n">
-        <v>7270.25</v>
+        <v>7387.7998046875</v>
       </c>
       <c r="C9" s="5" t="n">
-        <v>-0.6877864790397425</v>
+        <v>0.5813359445554056</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>6596.480024414062</v>
+        <v>6601.194025878906</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>10.21408346712587</v>
+        <v>11.91611359588635</v>
       </c>
       <c r="F9" s="5" t="n">
-        <v>7290.614072265625</v>
+        <v>7305.505068359375</v>
       </c>
       <c r="G9" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H9" s="5" t="n">
-        <v>63.62507808279309</v>
+        <v>59.65708261190853</v>
       </c>
       <c r="I9" s="5" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J9" s="6" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
@@ -1195,31 +1195,31 @@
         </is>
       </c>
       <c r="B10" s="5" t="n">
-        <v>3235.550048828125</v>
+        <v>3225.300048828125</v>
       </c>
       <c r="C10" s="5" t="n">
-        <v>-0.736297944209463</v>
+        <v>0.06204821052036014</v>
       </c>
       <c r="D10" s="5" t="n">
-        <v>3067.115498046875</v>
+        <v>3068.585247802735</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>5.49162725983121</v>
+        <v>5.107070143728492</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>3331.57798828125</v>
+        <v>3328.432993164062</v>
       </c>
       <c r="G10" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H10" s="5" t="n">
-        <v>56.25830612155943</v>
+        <v>42.66167300117723</v>
       </c>
       <c r="I10" s="5" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="J10" s="6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -1229,28 +1229,28 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>3100.300048828125</v>
+        <v>3176.050048828125</v>
       </c>
       <c r="C11" s="5" t="n">
-        <v>-0.5293891087496561</v>
+        <v>1.272265284722396</v>
       </c>
       <c r="D11" s="5" t="n">
-        <v>2692.329250488281</v>
+        <v>2697.75875</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>15.15307974557177</v>
+        <v>17.72920943461401</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>3026.916997070312</v>
+        <v>3034.92599609375</v>
       </c>
       <c r="G11" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H11" s="5" t="n">
-        <v>68.93348554080572</v>
+        <v>71.58520014277879</v>
       </c>
       <c r="I11" s="5" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J11" s="6" t="n">
         <v>19</v>
@@ -1263,28 +1263,28 @@
         </is>
       </c>
       <c r="B12" s="5" t="n">
-        <v>8582.5498046875</v>
+        <v>8537.400390625</v>
       </c>
       <c r="C12" s="5" t="n">
-        <v>3.874774870820352</v>
+        <v>0.9763719647770674</v>
       </c>
       <c r="D12" s="5" t="n">
-        <v>7588.910017089844</v>
+        <v>7604.952016601563</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>13.09331360313971</v>
+        <v>12.26106847206804</v>
       </c>
       <c r="F12" s="5" t="n">
-        <v>8242.30103515625</v>
+        <v>8257.200029296875</v>
       </c>
       <c r="G12" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H12" s="5" t="n">
-        <v>74.40739881764028</v>
+        <v>63.20615526987179</v>
       </c>
       <c r="I12" s="5" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J12" s="6" t="n">
         <v>18</v>
@@ -1297,31 +1297,31 @@
         </is>
       </c>
       <c r="B13" s="5" t="n">
-        <v>21738.19921875</v>
+        <v>22004.099609375</v>
       </c>
       <c r="C13" s="5" t="n">
-        <v>-0.809249853084848</v>
+        <v>0.226151838883748</v>
       </c>
       <c r="D13" s="5" t="n">
-        <v>20737.28521484375</v>
+        <v>20756.63345703125</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>4.826639521694947</v>
+        <v>6.009963778211704</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>22475.699140625</v>
+        <v>22451.517109375</v>
       </c>
       <c r="G13" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>45.41213357509822</v>
+        <v>46.06191533780506</v>
       </c>
       <c r="I13" s="5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J13" s="6" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14">
@@ -1331,31 +1331,31 @@
         </is>
       </c>
       <c r="B14" s="5" t="n">
-        <v>2474.85009765625</v>
+        <v>2502.39990234375</v>
       </c>
       <c r="C14" s="5" t="n">
-        <v>-0.9366517499749816</v>
+        <v>0.4455446272257024</v>
       </c>
       <c r="D14" s="5" t="n">
-        <v>2511.651251220703</v>
+        <v>2509.741501464844</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>-1.465217495723869</v>
+        <v>-0.2925241152050361</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>2587.741020507813</v>
+        <v>2581.831020507812</v>
       </c>
       <c r="G14" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>39.69012923756437</v>
+        <v>43.19846830812461</v>
       </c>
       <c r="I14" s="5" t="n">
         <v>4</v>
       </c>
       <c r="J14" s="6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
@@ -1365,28 +1365,28 @@
         </is>
       </c>
       <c r="B15" s="5" t="n">
-        <v>4507.2001953125</v>
+        <v>4569.14990234375</v>
       </c>
       <c r="C15" s="5" t="n">
-        <v>0.5095520456396274</v>
+        <v>1.200449721184538</v>
       </c>
       <c r="D15" s="5" t="n">
-        <v>4540.049499511719</v>
+        <v>4544.186499023437</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>-0.7235450671353183</v>
+        <v>0.5493481248112856</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>4805.62900390625</v>
+        <v>4787.711005859375</v>
       </c>
       <c r="G15" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>51.31626793853752</v>
+        <v>45.73089296211879</v>
       </c>
       <c r="I15" s="5" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="J15" s="6" t="n">
         <v>6</v>
@@ -1399,31 +1399,31 @@
         </is>
       </c>
       <c r="B16" s="5" t="n">
-        <v>557.9000244140625</v>
+        <v>561.5499877929688</v>
       </c>
       <c r="C16" s="5" t="n">
-        <v>0.8222732500000607</v>
+        <v>0.303654957786148</v>
       </c>
       <c r="D16" s="5" t="n">
-        <v>553.4117510986329</v>
+        <v>553.5090008544922</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>0.8110187950507951</v>
+        <v>1.452729210557202</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>569.8330017089844</v>
+        <v>569.6030017089844</v>
       </c>
       <c r="G16" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>43.58268879185387</v>
+        <v>49.18326502465255</v>
       </c>
       <c r="I16" s="5" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J16" s="6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
@@ -1433,28 +1433,28 @@
         </is>
       </c>
       <c r="B17" s="5" t="n">
-        <v>1359.199951171875</v>
+        <v>1353</v>
       </c>
       <c r="C17" s="5" t="n">
-        <v>-1.346401656913443</v>
+        <v>-0.4707977268737396</v>
       </c>
       <c r="D17" s="5" t="n">
-        <v>1242.189751586914</v>
+        <v>1243.471001586914</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>9.419671949110738</v>
+        <v>8.808327518157263</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>1309.827006835937</v>
+        <v>1312.5680078125</v>
       </c>
       <c r="G17" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>68.21551676388256</v>
+        <v>56.37810244304083</v>
       </c>
       <c r="I17" s="5" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J17" s="6" t="n">
         <v>15</v>
@@ -1467,31 +1467,31 @@
         </is>
       </c>
       <c r="B18" s="5" t="n">
-        <v>4824.85009765625</v>
+        <v>5033.10009765625</v>
       </c>
       <c r="C18" s="5" t="n">
-        <v>-0.3202247706732053</v>
+        <v>0.9750245291654025</v>
       </c>
       <c r="D18" s="5" t="n">
-        <v>4656.698493652344</v>
+        <v>4662.388745117188</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>3.610961805517737</v>
+        <v>7.951103453724226</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>5049.8730078125</v>
+        <v>5048.577001953125</v>
       </c>
       <c r="G18" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>50.33840947546531</v>
+        <v>56.4876927606853</v>
       </c>
       <c r="I18" s="5" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J18" s="6" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19">
@@ -1501,31 +1501,31 @@
         </is>
       </c>
       <c r="B19" s="5" t="n">
-        <v>1358</v>
+        <v>1345.050048828125</v>
       </c>
       <c r="C19" s="5" t="n">
-        <v>1.241288606039559</v>
+        <v>-0.09284705895153955</v>
       </c>
       <c r="D19" s="5" t="n">
-        <v>1202.402996826172</v>
+        <v>1204.566747436523</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>12.9405036069053</v>
+        <v>11.66255848341892</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>1350.136999511719</v>
+        <v>1352.846000976562</v>
       </c>
       <c r="G19" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H19" s="5" t="n">
-        <v>52.87486455763445</v>
+        <v>51.11827984905831</v>
       </c>
       <c r="I19" s="5" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J19" s="6" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20">
@@ -1535,28 +1535,28 @@
         </is>
       </c>
       <c r="B20" s="5" t="n">
-        <v>1940.949951171875</v>
+        <v>2018.900024414062</v>
       </c>
       <c r="C20" s="5" t="n">
-        <v>0.07991784770038368</v>
+        <v>1.505823373008508</v>
       </c>
       <c r="D20" s="5" t="n">
-        <v>1633.268748779297</v>
+        <v>1637.651498413086</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>18.83836953486918</v>
+        <v>23.28019889276891</v>
       </c>
       <c r="F20" s="5" t="n">
-        <v>1887.055998535156</v>
+        <v>1901.235998535156</v>
       </c>
       <c r="G20" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H20" s="5" t="n">
-        <v>45.1830681028455</v>
+        <v>64.94308930507873</v>
       </c>
       <c r="I20" s="5" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="J20" s="6" t="n">
         <v>20</v>
@@ -1569,31 +1569,31 @@
         </is>
       </c>
       <c r="B21" s="8" t="n">
-        <v>39618.44921875</v>
+        <v>40806.3984375</v>
       </c>
       <c r="C21" s="8" t="n">
-        <v>-0.5111515776455189</v>
+        <v>3.294783495953668</v>
       </c>
       <c r="D21" s="8" t="n">
-        <v>40130.59447265625</v>
+        <v>40067.63470703125</v>
       </c>
       <c r="E21" s="8" t="n">
-        <v>-1.27619652944641</v>
+        <v>1.843791718354442</v>
       </c>
       <c r="F21" s="8" t="n">
-        <v>38381.880859375</v>
+        <v>38475.395859375</v>
       </c>
       <c r="G21" s="8" t="n">
         <v>0</v>
       </c>
       <c r="H21" s="8" t="n">
-        <v>34.90389278314157</v>
+        <v>62.36917373827774</v>
       </c>
       <c r="I21" s="8" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="J21" s="9" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1687,31 +1687,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>22345.25</v>
+        <v>23106.599609375</v>
       </c>
       <c r="C2" t="n">
-        <v>-1.582937347378843</v>
+        <v>1.374747389578057</v>
       </c>
       <c r="D2" t="n">
-        <v>21856.24674804688</v>
+        <v>21889.8275</v>
       </c>
       <c r="E2" t="n">
-        <v>2.237361508543646</v>
+        <v>5.558618994941831</v>
       </c>
       <c r="F2" t="n">
-        <v>23429.0809375</v>
+        <v>23442.794921875</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>23.97666107757306</v>
+        <v>47.1239382763026</v>
       </c>
       <c r="I2" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="J2" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -1721,31 +1721,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2767.89990234375</v>
+        <v>2700.949951171875</v>
       </c>
       <c r="C3" t="n">
-        <v>1.145597666998643</v>
+        <v>-1.216077850698116</v>
       </c>
       <c r="D3" t="n">
-        <v>2402.034997558594</v>
+        <v>2406.197746582031</v>
       </c>
       <c r="E3" t="n">
-        <v>15.23145604277282</v>
+        <v>12.24970827973448</v>
       </c>
       <c r="F3" t="n">
-        <v>2701.75201171875</v>
+        <v>2712.342006835937</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>44.1903615338814</v>
+        <v>43.43984872357683</v>
       </c>
       <c r="I3" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J3" t="n">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4">
@@ -1755,31 +1755,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3235.550048828125</v>
+        <v>3225.300048828125</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.736297944209463</v>
+        <v>0.06204821052036014</v>
       </c>
       <c r="D4" t="n">
-        <v>3067.115498046875</v>
+        <v>3068.585247802735</v>
       </c>
       <c r="E4" t="n">
-        <v>5.49162725983121</v>
+        <v>5.107070143728492</v>
       </c>
       <c r="F4" t="n">
-        <v>3331.57798828125</v>
+        <v>3328.432993164062</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>56.25830612155943</v>
+        <v>42.66167300117723</v>
       </c>
       <c r="I4" t="n">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="J4" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
@@ -1789,31 +1789,31 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1510.099975585938</v>
+        <v>1518.199951171875</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.2905265377393551</v>
+        <v>0.5130921414501222</v>
       </c>
       <c r="D5" t="n">
-        <v>1458.9725</v>
+        <v>1457.364499511719</v>
       </c>
       <c r="E5" t="n">
-        <v>3.504348134453351</v>
+        <v>4.174347027153382</v>
       </c>
       <c r="F5" t="n">
-        <v>1548.508000488281</v>
+        <v>1548.890998535156</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>59.00479895415247</v>
+        <v>52.23780854765826</v>
       </c>
       <c r="I5" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="J5" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
@@ -1823,31 +1823,31 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7226.64990234375</v>
+        <v>7191</v>
       </c>
       <c r="C6" t="n">
-        <v>-1.55500633964788</v>
+        <v>0.1978624971986198</v>
       </c>
       <c r="D6" t="n">
-        <v>6533.129262695313</v>
+        <v>6538.398010253906</v>
       </c>
       <c r="E6" t="n">
-        <v>10.61544340793156</v>
+        <v>9.981068584730455</v>
       </c>
       <c r="F6" t="n">
-        <v>7286.187998046875</v>
+        <v>7299.203994140625</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>47.01482644533632</v>
+        <v>45.35963087780068</v>
       </c>
       <c r="I6" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="J6" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
@@ -1857,31 +1857,31 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>7270.25</v>
+        <v>7387.7998046875</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.6877864790397425</v>
+        <v>0.5813359445554056</v>
       </c>
       <c r="D7" t="n">
-        <v>6596.480024414062</v>
+        <v>6601.194025878906</v>
       </c>
       <c r="E7" t="n">
-        <v>10.21408346712587</v>
+        <v>11.91611359588635</v>
       </c>
       <c r="F7" t="n">
-        <v>7290.614072265625</v>
+        <v>7305.505068359375</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>63.62507808279309</v>
+        <v>59.65708261190853</v>
       </c>
       <c r="I7" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J7" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8">
@@ -1891,31 +1891,31 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1655.050048828125</v>
+        <v>1686.550048828125</v>
       </c>
       <c r="C8" t="n">
-        <v>-1.730786319253086</v>
+        <v>0.2764744840099809</v>
       </c>
       <c r="D8" t="n">
-        <v>1580.699503173828</v>
+        <v>1580.628753662109</v>
       </c>
       <c r="E8" t="n">
-        <v>4.703648321835438</v>
+        <v>6.701212724405393</v>
       </c>
       <c r="F8" t="n">
-        <v>1693.130004882812</v>
+        <v>1695.123005371094</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>51.88964143088013</v>
+        <v>47.93740912066044</v>
       </c>
       <c r="I8" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J8" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
@@ -1925,31 +1925,31 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>707.7999877929688</v>
+        <v>715.75</v>
       </c>
       <c r="C9" t="n">
-        <v>-1.673958213745907</v>
+        <v>0.888010104245418</v>
       </c>
       <c r="D9" t="n">
-        <v>621.6609991455078</v>
+        <v>622.6952493286133</v>
       </c>
       <c r="E9" t="n">
-        <v>13.85626390683372</v>
+        <v>14.94386712789569</v>
       </c>
       <c r="F9" t="n">
-        <v>690.7709985351562</v>
+        <v>692.2219982910157</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>56.16340536772084</v>
+        <v>58.258534774193</v>
       </c>
       <c r="I9" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J9" t="n">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10">
@@ -1959,31 +1959,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1940.949951171875</v>
+        <v>2018.900024414062</v>
       </c>
       <c r="C10" t="n">
-        <v>0.07991784770038368</v>
+        <v>1.505823373008508</v>
       </c>
       <c r="D10" t="n">
-        <v>1633.268748779297</v>
+        <v>1637.651498413086</v>
       </c>
       <c r="E10" t="n">
-        <v>18.83836953486918</v>
+        <v>23.28019889276891</v>
       </c>
       <c r="F10" t="n">
-        <v>1887.055998535156</v>
+        <v>1901.235998535156</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>45.1830681028455</v>
+        <v>64.94308930507873</v>
       </c>
       <c r="I10" t="n">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="J10" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11">
@@ -1993,31 +1993,31 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>557.9000244140625</v>
+        <v>561.5499877929688</v>
       </c>
       <c r="C11" t="n">
-        <v>0.8222732500000607</v>
+        <v>0.303654957786148</v>
       </c>
       <c r="D11" t="n">
-        <v>553.4117510986329</v>
+        <v>553.5090008544922</v>
       </c>
       <c r="E11" t="n">
-        <v>0.8110187950507951</v>
+        <v>1.452729210557202</v>
       </c>
       <c r="F11" t="n">
-        <v>569.8330017089844</v>
+        <v>569.6030017089844</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>43.58268879185387</v>
+        <v>49.18326502465255</v>
       </c>
       <c r="I11" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="J11" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12">
@@ -2027,31 +2027,31 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>5579.10009765625</v>
+        <v>5875.7001953125</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7566983469230681</v>
+        <v>6.279230591911489</v>
       </c>
       <c r="D12" t="n">
-        <v>4899.026752929687</v>
+        <v>4904.92275390625</v>
       </c>
       <c r="E12" t="n">
-        <v>13.88180508138416</v>
+        <v>19.79190071103828</v>
       </c>
       <c r="F12" t="n">
-        <v>5458.37001953125</v>
+        <v>5498.05501953125</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>58.35402625044343</v>
+        <v>68.17996295103906</v>
       </c>
       <c r="I12" t="n">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="J12" t="n">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
@@ -2061,31 +2061,31 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1426.099975585938</v>
+        <v>1446.900024414062</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.8482286607810141</v>
+        <v>-0.7272710522084003</v>
       </c>
       <c r="D13" t="n">
-        <v>1330.669997558594</v>
+        <v>1331.905997314453</v>
       </c>
       <c r="E13" t="n">
-        <v>7.171573583415205</v>
+        <v>8.6337945269016</v>
       </c>
       <c r="F13" t="n">
-        <v>1411.126997070312</v>
+        <v>1412.310998535156</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>55.33979316834522</v>
+        <v>60.6477009939208</v>
       </c>
       <c r="I13" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="J13" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14">
@@ -2095,31 +2095,31 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1359.199951171875</v>
+        <v>1353</v>
       </c>
       <c r="C14" t="n">
-        <v>-1.346401656913443</v>
+        <v>-0.4707977268737396</v>
       </c>
       <c r="D14" t="n">
-        <v>1242.189751586914</v>
+        <v>1243.471001586914</v>
       </c>
       <c r="E14" t="n">
-        <v>9.419671949110738</v>
+        <v>8.808327518157263</v>
       </c>
       <c r="F14" t="n">
-        <v>1309.827006835937</v>
+        <v>1312.5680078125</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>68.21551676388256</v>
+        <v>56.37810244304083</v>
       </c>
       <c r="I14" t="n">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="J14" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15">
@@ -2129,31 +2129,31 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1232.5</v>
+        <v>1235.849975585938</v>
       </c>
       <c r="C15" t="n">
-        <v>3.938265242780736</v>
+        <v>0.0242747558544476</v>
       </c>
       <c r="D15" t="n">
-        <v>1109.51674621582</v>
+        <v>1110.884996337891</v>
       </c>
       <c r="E15" t="n">
-        <v>11.08439815835436</v>
+        <v>11.24913736885479</v>
       </c>
       <c r="F15" t="n">
-        <v>1154.502001953125</v>
+        <v>1157.277001953125</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>71.88608296596459</v>
+        <v>72.37065527793652</v>
       </c>
       <c r="I15" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J15" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16">
@@ -2163,31 +2163,31 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2452.800048828125</v>
+        <v>2457.10009765625</v>
       </c>
       <c r="C16" t="n">
-        <v>0.8863773296915234</v>
+        <v>-0.5866644856402869</v>
       </c>
       <c r="D16" t="n">
-        <v>2057.964499511719</v>
+        <v>2062.005250244141</v>
       </c>
       <c r="E16" t="n">
-        <v>19.18573179518338</v>
+        <v>19.16071005955635</v>
       </c>
       <c r="F16" t="n">
-        <v>2410.940007324219</v>
+        <v>2429.06201171875</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>45.65353269816185</v>
+        <v>48.8015931421949</v>
       </c>
       <c r="I16" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J16" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17">
@@ -2197,28 +2197,28 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1584.550048828125</v>
+        <v>1595.5</v>
       </c>
       <c r="C17" t="n">
-        <v>0.6255221922703225</v>
+        <v>1.308017986322763</v>
       </c>
       <c r="D17" t="n">
-        <v>1629.381003417969</v>
+        <v>1628.977753295899</v>
       </c>
       <c r="E17" t="n">
-        <v>-2.751410167161724</v>
+        <v>-2.055138765901698</v>
       </c>
       <c r="F17" t="n">
-        <v>1639.787998046875</v>
+        <v>1637.614997558594</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>38.83005312295278</v>
+        <v>47.24302965236613</v>
       </c>
       <c r="I17" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="J17" t="n">
         <v>4</v>
@@ -2231,31 +2231,31 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>640.0499877929688</v>
+        <v>647.5499877929688</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.2026955394800023</v>
+        <v>1.029717678483433</v>
       </c>
       <c r="D18" t="n">
-        <v>574.0722492980957</v>
+        <v>575.2182493591308</v>
       </c>
       <c r="E18" t="n">
-        <v>11.49293291489746</v>
+        <v>12.57465988160581</v>
       </c>
       <c r="F18" t="n">
-        <v>647.6909985351563</v>
+        <v>648.317998046875</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>56.58844099141432</v>
+        <v>57.63628034553414</v>
       </c>
       <c r="I18" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J18" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19">
@@ -2265,28 +2265,28 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2501.39990234375</v>
+        <v>2523.5</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.135745225890016</v>
+        <v>0.6561476975525116</v>
       </c>
       <c r="D19" t="n">
-        <v>2584.489011230469</v>
+        <v>2584.952510986328</v>
       </c>
       <c r="E19" t="n">
-        <v>-3.214914380586214</v>
+        <v>-2.377316825943539</v>
       </c>
       <c r="F19" t="n">
-        <v>2602.45001953125</v>
+        <v>2597.187016601562</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>39.98732260124183</v>
+        <v>42.47878738357827</v>
       </c>
       <c r="I19" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J19" t="n">
         <v>2</v>
@@ -2299,31 +2299,31 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>967.3499755859375</v>
+        <v>957.5</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.139365810269565</v>
+        <v>-1.125570439824974</v>
       </c>
       <c r="D20" t="n">
-        <v>912.8255029296874</v>
+        <v>913.2880032348633</v>
       </c>
       <c r="E20" t="n">
-        <v>5.973153957821655</v>
+        <v>4.840969837393899</v>
       </c>
       <c r="F20" t="n">
-        <v>964.5270031738281</v>
+        <v>966.0260034179687</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>56.68952780973778</v>
+        <v>44.49949446185531</v>
       </c>
       <c r="I20" t="n">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="J20" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21">
@@ -2333,31 +2333,31 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1358</v>
+        <v>1345.050048828125</v>
       </c>
       <c r="C21" t="n">
-        <v>1.241288606039559</v>
+        <v>-0.09284705895153955</v>
       </c>
       <c r="D21" t="n">
-        <v>1202.402996826172</v>
+        <v>1204.566747436523</v>
       </c>
       <c r="E21" t="n">
-        <v>12.9405036069053</v>
+        <v>11.66255848341892</v>
       </c>
       <c r="F21" t="n">
-        <v>1350.136999511719</v>
+        <v>1352.846000976562</v>
       </c>
       <c r="G21" t="n">
         <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>52.87486455763445</v>
+        <v>51.11827984905831</v>
       </c>
       <c r="I21" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J21" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22">
@@ -2367,31 +2367,31 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>553.5499877929688</v>
+        <v>539.6500244140625</v>
       </c>
       <c r="C22" t="n">
-        <v>-1.468494157931566</v>
+        <v>0.5215700764573894</v>
       </c>
       <c r="D22" t="n">
-        <v>479.2915000915527</v>
+        <v>479.9142500305176</v>
       </c>
       <c r="E22" t="n">
-        <v>15.49338715316908</v>
+        <v>12.44717663202257</v>
       </c>
       <c r="F22" t="n">
-        <v>567.6319982910156</v>
+        <v>566.7579980468749</v>
       </c>
       <c r="G22" t="n">
         <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>48.85374639699929</v>
+        <v>39.71893208924943</v>
       </c>
       <c r="I22" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="J22" t="n">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23">
@@ -2401,28 +2401,28 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1465.099975585938</v>
+        <v>1477.449951171875</v>
       </c>
       <c r="C23" t="n">
-        <v>1.471759556693297</v>
+        <v>-0.09805079574340958</v>
       </c>
       <c r="D23" t="n">
-        <v>1425.449003295898</v>
+        <v>1424.279752807617</v>
       </c>
       <c r="E23" t="n">
-        <v>2.781647901703873</v>
+        <v>3.733128850525743</v>
       </c>
       <c r="F23" t="n">
-        <v>1376.887993164062</v>
+        <v>1385.307993164063</v>
       </c>
       <c r="G23" t="n">
         <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>73.82618430327139</v>
+        <v>71.23688122189265</v>
       </c>
       <c r="I23" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J23" t="n">
         <v>10</v>
@@ -2435,31 +2435,31 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>437.5</v>
+        <v>447.4500122070312</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.8048946584791938</v>
+        <v>0.9817210660338915</v>
       </c>
       <c r="D24" t="n">
-        <v>400.6475001525879</v>
+        <v>401.6612501525879</v>
       </c>
       <c r="E24" t="n">
-        <v>9.198235314928137</v>
+        <v>11.39984552581275</v>
       </c>
       <c r="F24" t="n">
-        <v>458.4110003662109</v>
+        <v>458.4130004882812</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
       </c>
       <c r="H24" t="n">
-        <v>38.13382953936283</v>
+        <v>48.6774637909874</v>
       </c>
       <c r="I24" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="J24" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25">
@@ -2469,28 +2469,28 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1762.199951171875</v>
+        <v>1770.300048828125</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.5025139482099594</v>
+        <v>-0.0423477586359744</v>
       </c>
       <c r="D25" t="n">
-        <v>1834.256001586914</v>
+        <v>1832.380501708984</v>
       </c>
       <c r="E25" t="n">
-        <v>-3.928352986317034</v>
+        <v>-3.387967336639938</v>
       </c>
       <c r="F25" t="n">
-        <v>1835.102990722656</v>
+        <v>1832.899992675781</v>
       </c>
       <c r="G25" t="n">
         <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>38.59897265324037</v>
+        <v>40.87691544225076</v>
       </c>
       <c r="I25" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J25" t="n">
         <v>1</v>
@@ -2503,31 +2503,31 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>577.5499877929688</v>
+        <v>588.25</v>
       </c>
       <c r="C26" t="n">
-        <v>1.440241074673332</v>
+        <v>1.835016902611497</v>
       </c>
       <c r="D26" t="n">
-        <v>517.7055009460449</v>
+        <v>518.626501159668</v>
       </c>
       <c r="E26" t="n">
-        <v>11.55956170787546</v>
+        <v>13.42459336047257</v>
       </c>
       <c r="F26" t="n">
-        <v>550.5059985351562</v>
+        <v>552.6799987792969</v>
       </c>
       <c r="G26" t="n">
         <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>56.83298424559536</v>
+        <v>66.98881621913912</v>
       </c>
       <c r="I26" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="J26" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27">
@@ -2537,28 +2537,28 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>317</v>
+        <v>326.7000122070312</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.07880220646178104</v>
+        <v>1.302329366521326</v>
       </c>
       <c r="D27" t="n">
-        <v>255.8182492828369</v>
+        <v>256.4544994354248</v>
       </c>
       <c r="E27" t="n">
-        <v>23.91610093833436</v>
+        <v>27.39102372009436</v>
       </c>
       <c r="F27" t="n">
-        <v>303.1049993896484</v>
+        <v>305.9589996337891</v>
       </c>
       <c r="G27" t="n">
         <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>52.82113205777596</v>
+        <v>66.96843068263155</v>
       </c>
       <c r="I27" t="n">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="J27" t="n">
         <v>37</v>
@@ -2571,31 +2571,31 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>21738.19921875</v>
+        <v>22004.099609375</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.809249853084848</v>
+        <v>0.226151838883748</v>
       </c>
       <c r="D28" t="n">
-        <v>20737.28521484375</v>
+        <v>20756.63345703125</v>
       </c>
       <c r="E28" t="n">
-        <v>4.826639521694947</v>
+        <v>6.009963778211704</v>
       </c>
       <c r="F28" t="n">
-        <v>22475.699140625</v>
+        <v>22451.517109375</v>
       </c>
       <c r="G28" t="n">
         <v>0</v>
       </c>
       <c r="H28" t="n">
-        <v>45.41213357509822</v>
+        <v>46.06191533780506</v>
       </c>
       <c r="I28" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J28" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29">
@@ -2605,31 +2605,31 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>982.25</v>
+        <v>965.0499877929688</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.8979492705278314</v>
+        <v>-1.670999461010048</v>
       </c>
       <c r="D29" t="n">
-        <v>913.4177499389648</v>
+        <v>914.5822497558594</v>
       </c>
       <c r="E29" t="n">
-        <v>7.535681243947212</v>
+        <v>5.518119124942709</v>
       </c>
       <c r="F29" t="n">
-        <v>963.1630017089843</v>
+        <v>963.7140014648437</v>
       </c>
       <c r="G29" t="n">
         <v>0</v>
       </c>
       <c r="H29" t="n">
-        <v>68.78329220056601</v>
+        <v>48.91237797108527</v>
       </c>
       <c r="I29" t="n">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="J29" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30">
@@ -2639,31 +2639,31 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>39618.44921875</v>
+        <v>40806.3984375</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.5111515776455189</v>
+        <v>3.294783495953668</v>
       </c>
       <c r="D30" t="n">
-        <v>40130.59447265625</v>
+        <v>40067.63470703125</v>
       </c>
       <c r="E30" t="n">
-        <v>-1.27619652944641</v>
+        <v>1.843791718354442</v>
       </c>
       <c r="F30" t="n">
-        <v>38381.880859375</v>
+        <v>38475.395859375</v>
       </c>
       <c r="G30" t="n">
         <v>0</v>
       </c>
       <c r="H30" t="n">
-        <v>34.90389278314157</v>
+        <v>62.36917373827774</v>
       </c>
       <c r="I30" t="n">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="J30" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31">
@@ -2673,31 +2673,31 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>3857.85009765625</v>
+        <v>3849.699951171875</v>
       </c>
       <c r="C31" t="n">
-        <v>1.108622565208295</v>
+        <v>-0.4525237955357642</v>
       </c>
       <c r="D31" t="n">
-        <v>3949.484495849609</v>
+        <v>3943.426495361328</v>
       </c>
       <c r="E31" t="n">
-        <v>-2.32016098024071</v>
+        <v>-2.376779288258683</v>
       </c>
       <c r="F31" t="n">
-        <v>3867.689995117188</v>
+        <v>3871.917993164062</v>
       </c>
       <c r="G31" t="n">
         <v>1</v>
       </c>
       <c r="H31" t="n">
-        <v>52.39507439342001</v>
+        <v>46.01127715592742</v>
       </c>
       <c r="I31" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="J31" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32">
@@ -2707,28 +2707,28 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>16310.7998046875</v>
+        <v>16395.5</v>
       </c>
       <c r="C32" t="n">
-        <v>1.188329510910857</v>
+        <v>1.496556527122195</v>
       </c>
       <c r="D32" t="n">
-        <v>14258.58748046875</v>
+        <v>14281.30697753906</v>
       </c>
       <c r="E32" t="n">
-        <v>14.39281644854266</v>
+        <v>14.8039183373485</v>
       </c>
       <c r="F32" t="n">
-        <v>15384.9279296875</v>
+        <v>15461.78494140625</v>
       </c>
       <c r="G32" t="n">
         <v>0</v>
       </c>
       <c r="H32" t="n">
-        <v>63.76058630154503</v>
+        <v>61.78215744463773</v>
       </c>
       <c r="I32" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J32" t="n">
         <v>29</v>
@@ -2741,28 +2741,28 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>2474.85009765625</v>
+        <v>2502.39990234375</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.9366517499749816</v>
+        <v>0.4455446272257024</v>
       </c>
       <c r="D33" t="n">
-        <v>2511.651251220703</v>
+        <v>2509.741501464844</v>
       </c>
       <c r="E33" t="n">
-        <v>-1.465217495723869</v>
+        <v>-0.2925241152050361</v>
       </c>
       <c r="F33" t="n">
-        <v>2587.741020507813</v>
+        <v>2581.831020507812</v>
       </c>
       <c r="G33" t="n">
         <v>0</v>
       </c>
       <c r="H33" t="n">
-        <v>39.69012923756437</v>
+        <v>43.19846830812461</v>
       </c>
       <c r="I33" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J33" t="n">
         <v>6</v>
@@ -2775,28 +2775,28 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>7109.0498046875</v>
+        <v>7113.89990234375</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.09626467137338057</v>
+        <v>0.3172857307421673</v>
       </c>
       <c r="D34" t="n">
-        <v>6180.053000488281</v>
+        <v>6195.587749023438</v>
       </c>
       <c r="E34" t="n">
-        <v>15.03218182960275</v>
+        <v>14.82203449487191</v>
       </c>
       <c r="F34" t="n">
-        <v>7024.430986328125</v>
+        <v>7034.59798828125</v>
       </c>
       <c r="G34" t="n">
         <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>50.165644866465</v>
+        <v>51.58917485578689</v>
       </c>
       <c r="I34" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J34" t="n">
         <v>30</v>
@@ -2809,31 +2809,31 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>3418.5</v>
+        <v>3429.89990234375</v>
       </c>
       <c r="C35" t="n">
-        <v>1.16299862085687</v>
+        <v>0.01603232892073425</v>
       </c>
       <c r="D35" t="n">
-        <v>3319.634499511719</v>
+        <v>3320.408999023437</v>
       </c>
       <c r="E35" t="n">
-        <v>2.978204392767434</v>
+        <v>3.297512545969934</v>
       </c>
       <c r="F35" t="n">
-        <v>3379.307998046875</v>
+        <v>3388.372998046875</v>
       </c>
       <c r="G35" t="n">
         <v>0</v>
       </c>
       <c r="H35" t="n">
-        <v>44.84287247304366</v>
+        <v>55.40127060757342</v>
       </c>
       <c r="I35" t="n">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="J35" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36">
@@ -2843,31 +2843,31 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>3100.300048828125</v>
+        <v>3176.050048828125</v>
       </c>
       <c r="C36" t="n">
-        <v>-0.5293891087496561</v>
+        <v>1.272265284722396</v>
       </c>
       <c r="D36" t="n">
-        <v>2692.329250488281</v>
+        <v>2697.75875</v>
       </c>
       <c r="E36" t="n">
-        <v>15.15307974557177</v>
+        <v>17.72920943461401</v>
       </c>
       <c r="F36" t="n">
-        <v>3026.916997070312</v>
+        <v>3034.92599609375</v>
       </c>
       <c r="G36" t="n">
         <v>0</v>
       </c>
       <c r="H36" t="n">
-        <v>68.93348554080572</v>
+        <v>71.58520014277879</v>
       </c>
       <c r="I36" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J36" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37">
@@ -2877,31 +2877,31 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>1650.050048828125</v>
+        <v>1666.400024414062</v>
       </c>
       <c r="C37" t="n">
-        <v>1.13389105122994</v>
+        <v>0.1171602210576772</v>
       </c>
       <c r="D37" t="n">
-        <v>1425.736500854492</v>
+        <v>1427.146000976562</v>
       </c>
       <c r="E37" t="n">
-        <v>15.73317003802556</v>
+        <v>16.76450925650103</v>
       </c>
       <c r="F37" t="n">
-        <v>1505.818005371094</v>
+        <v>1514.316005859375</v>
       </c>
       <c r="G37" t="n">
         <v>0</v>
       </c>
       <c r="H37" t="n">
-        <v>81.85002724553229</v>
+        <v>80.68174210994169</v>
       </c>
       <c r="I37" t="n">
         <v>37</v>
       </c>
       <c r="J37" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38">
@@ -2911,31 +2911,31 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>2410.699951171875</v>
+        <v>2428.699951171875</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.08082196965174537</v>
+        <v>0.210424711591517</v>
       </c>
       <c r="D38" t="n">
-        <v>2479.385506591797</v>
+        <v>2477.690006103516</v>
       </c>
       <c r="E38" t="n">
-        <v>-2.770265262796433</v>
+        <v>-1.977247145968995</v>
       </c>
       <c r="F38" t="n">
-        <v>2559.169995117188</v>
+        <v>2556.009995117187</v>
       </c>
       <c r="G38" t="n">
         <v>0</v>
       </c>
       <c r="H38" t="n">
-        <v>12.32752498561443</v>
+        <v>37.50138741285078</v>
       </c>
       <c r="I38" t="n">
         <v>1</v>
       </c>
       <c r="J38" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2951,8 +2951,8 @@
   </sheetPr>
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -3019,31 +3019,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>50.56000137329102</v>
+        <v>50.61000061035156</v>
       </c>
       <c r="C2" t="n">
-        <v>2.327467171484199</v>
+        <v>-0.2562102164265445</v>
       </c>
       <c r="D2" t="n">
-        <v>41.46304992675781</v>
+        <v>41.58494993209839</v>
       </c>
       <c r="E2" t="n">
-        <v>21.93989941068606</v>
+        <v>21.70268496893623</v>
       </c>
       <c r="F2" t="n">
-        <v>46.14840003967285</v>
+        <v>46.44540008544922</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>75.11452835748922</v>
+        <v>75.64477569142045</v>
       </c>
       <c r="I2" t="n">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="J2" t="n">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3">
@@ -3053,28 +3053,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>52.02999877929688</v>
+        <v>51.91999816894531</v>
       </c>
       <c r="C3" t="n">
-        <v>0.01922014887585366</v>
+        <v>0.03852917625914998</v>
       </c>
       <c r="D3" t="n">
-        <v>50.76030004501343</v>
+        <v>50.81385004043579</v>
       </c>
       <c r="E3" t="n">
-        <v>2.501361759401532</v>
+        <v>2.176863448900825</v>
       </c>
       <c r="F3" t="n">
-        <v>51.69400009155274</v>
+        <v>51.72060005187988</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>64.41702141601743</v>
+        <v>55.64451995339876</v>
       </c>
       <c r="I3" t="n">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="J3" t="n">
         <v>3</v>
@@ -3087,31 +3087,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>50.7400016784668</v>
+        <v>50.56999969482422</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1579191300743243</v>
+        <v>-0.2170493482422708</v>
       </c>
       <c r="D4" t="n">
-        <v>49.03609992980957</v>
+        <v>49.10699993133545</v>
       </c>
       <c r="E4" t="n">
-        <v>3.474790513715801</v>
+        <v>2.979208189330294</v>
       </c>
       <c r="F4" t="n">
-        <v>50.47799980163574</v>
+        <v>50.4497998046875</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>62.36569063572244</v>
+        <v>53.78116984937952</v>
       </c>
       <c r="I4" t="n">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="J4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -3121,28 +3121,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>270.6600036621094</v>
+        <v>271.6600036621094</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7631951239131185</v>
+        <v>-0.01839748060094015</v>
       </c>
       <c r="D5" t="n">
-        <v>283.1208999633789</v>
+        <v>283.2248999023437</v>
       </c>
       <c r="E5" t="n">
-        <v>-4.401263312910256</v>
+        <v>-4.083290785598989</v>
       </c>
       <c r="F5" t="n">
-        <v>275.7575994873047</v>
+        <v>275.7075994873047</v>
       </c>
       <c r="G5" t="n">
         <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>38.00057657913176</v>
+        <v>48.30488960376013</v>
       </c>
       <c r="I5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J5" t="n">
         <v>1</v>
@@ -3155,25 +3155,25 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>14.92000007629395</v>
+        <v>14.89000034332275</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6068789821368936</v>
+        <v>-0.3346669241289457</v>
       </c>
       <c r="D6" t="n">
-        <v>14.5175</v>
+        <v>14.53610000133514</v>
       </c>
       <c r="E6" t="n">
-        <v>2.772516454582023</v>
+        <v>2.434630622760599</v>
       </c>
       <c r="F6" t="n">
-        <v>14.71140003204346</v>
+        <v>14.75540002822876</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>46.56861576378399</v>
+        <v>51.3825050781397</v>
       </c>
       <c r="I6" t="n">
         <v>7</v>
@@ -3189,28 +3189,28 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>53.54000091552734</v>
+        <v>53.25</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4691311610151461</v>
+        <v>-0.3928153536643997</v>
       </c>
       <c r="D7" t="n">
-        <v>53.2846000289917</v>
+        <v>53.29370002746582</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4793146357421939</v>
+        <v>-0.08199848658152073</v>
       </c>
       <c r="F7" t="n">
-        <v>53.51980033874511</v>
+        <v>53.54100036621094</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>53.41365123452771</v>
+        <v>48.37289604677409</v>
       </c>
       <c r="I7" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="J7" t="n">
         <v>2</v>
@@ -3223,31 +3223,31 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>124.75</v>
+        <v>124.4300003051758</v>
       </c>
       <c r="C8" t="n">
-        <v>0.120386458840982</v>
+        <v>-0.08030071075350032</v>
       </c>
       <c r="D8" t="n">
-        <v>108.9263589477539</v>
+        <v>109.1492989730835</v>
       </c>
       <c r="E8" t="n">
-        <v>14.52691635441136</v>
+        <v>13.99981628453753</v>
       </c>
       <c r="F8" t="n">
-        <v>122.2571998596191</v>
+        <v>122.4927998352051</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>63.3093473845985</v>
+        <v>59.01436568707613</v>
       </c>
       <c r="I8" t="n">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="J8" t="n">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9">
@@ -3257,31 +3257,31 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>213.8300018310547</v>
+        <v>214.7700042724609</v>
       </c>
       <c r="C9" t="n">
-        <v>0.5927433144009564</v>
+        <v>0.294202337073024</v>
       </c>
       <c r="D9" t="n">
-        <v>200.3224001312256</v>
+        <v>200.4370501708984</v>
       </c>
       <c r="E9" t="n">
-        <v>6.742931240330916</v>
+        <v>7.150850648291727</v>
       </c>
       <c r="F9" t="n">
-        <v>212.0074005126953</v>
+        <v>212.4416006469727</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>57.83007021840172</v>
+        <v>61.60485576568603</v>
       </c>
       <c r="I9" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J9" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
@@ -3291,31 +3291,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>15.27000045776367</v>
+        <v>15.35000038146973</v>
       </c>
       <c r="C10" t="n">
-        <v>0.7255977009151593</v>
+        <v>-0.06509944942071355</v>
       </c>
       <c r="D10" t="n">
-        <v>13.98889999389649</v>
+        <v>14.00714999198914</v>
       </c>
       <c r="E10" t="n">
-        <v>9.157978571768655</v>
+        <v>9.586892338902512</v>
       </c>
       <c r="F10" t="n">
-        <v>15.16180004119873</v>
+        <v>15.19680004119873</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>53.103455986909</v>
+        <v>54.85329857972254</v>
       </c>
       <c r="I10" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="J10" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11">
@@ -3325,31 +3325,31 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>162.1399993896484</v>
+        <v>163.1900024414062</v>
       </c>
       <c r="C11" t="n">
-        <v>0.7080741550611336</v>
+        <v>0.2950007422611423</v>
       </c>
       <c r="D11" t="n">
-        <v>148.35744972229</v>
+        <v>148.5488997650147</v>
       </c>
       <c r="E11" t="n">
-        <v>9.290096111221873</v>
+        <v>9.856082878804182</v>
       </c>
       <c r="F11" t="n">
-        <v>160.3509997558594</v>
+        <v>160.7167999267578</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>53.14592465795397</v>
+        <v>61.99420212562164</v>
       </c>
       <c r="I11" t="n">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="J11" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12">
@@ -3359,31 +3359,31 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>22.72999954223633</v>
+        <v>22.84000015258789</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6643030072501999</v>
+        <v>0.04380301758761806</v>
       </c>
       <c r="D12" t="n">
-        <v>20.13704998016357</v>
+        <v>20.16349998474121</v>
       </c>
       <c r="E12" t="n">
-        <v>12.8765115278901</v>
+        <v>13.27398601369866</v>
       </c>
       <c r="F12" t="n">
-        <v>21.98019996643066</v>
+        <v>22.04799995422363</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>70.1219072518649</v>
+        <v>68.74875689375517</v>
       </c>
       <c r="I12" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J12" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13">
@@ -3393,28 +3393,28 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>45.04999923706055</v>
+        <v>45.38999938964844</v>
       </c>
       <c r="C13" t="n">
-        <v>0.4235368348727508</v>
+        <v>0.1544565209522952</v>
       </c>
       <c r="D13" t="n">
-        <v>39.81960004806518</v>
+        <v>39.87950004577637</v>
       </c>
       <c r="E13" t="n">
-        <v>13.13523787954145</v>
+        <v>13.81787469137464</v>
       </c>
       <c r="F13" t="n">
-        <v>43.40899993896485</v>
+        <v>43.5423999786377</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>60.41663171335399</v>
+        <v>66.66260118998133</v>
       </c>
       <c r="I13" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="J13" t="n">
         <v>35</v>
@@ -3427,31 +3427,31 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>16.21999931335449</v>
+        <v>16.43000030517578</v>
       </c>
       <c r="C14" t="n">
-        <v>0.5579674970275228</v>
+        <v>0.4892961580399868</v>
       </c>
       <c r="D14" t="n">
-        <v>14.91184996604919</v>
+        <v>14.92949996948242</v>
       </c>
       <c r="E14" t="n">
-        <v>8.772549014935429</v>
+        <v>10.05057328618207</v>
       </c>
       <c r="F14" t="n">
-        <v>16.01319993972778</v>
+        <v>16.05019994735718</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>57.14274036653751</v>
+        <v>66.53205604699011</v>
       </c>
       <c r="I14" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="J14" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15">
@@ -3461,31 +3461,31 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>214.4199981689453</v>
+        <v>214.9600067138672</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6147048729960636</v>
+        <v>0.1117760300855197</v>
       </c>
       <c r="D15" t="n">
-        <v>200.3859498596191</v>
+        <v>200.5389999389648</v>
       </c>
       <c r="E15" t="n">
-        <v>7.003509137820176</v>
+        <v>7.191123312319025</v>
       </c>
       <c r="F15" t="n">
-        <v>212.7855993652344</v>
+        <v>213.2151995849609</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>57.65359356778985</v>
+        <v>60.31212928036703</v>
       </c>
       <c r="I15" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J15" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16">
@@ -3495,31 +3495,31 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>203.7100067138672</v>
+        <v>204.2700042724609</v>
       </c>
       <c r="C16" t="n">
-        <v>0.6074728428892451</v>
+        <v>0.05387960833582728</v>
       </c>
       <c r="D16" t="n">
-        <v>190.5334002685547</v>
+        <v>190.6795503234863</v>
       </c>
       <c r="E16" t="n">
-        <v>6.915641261185819</v>
+        <v>7.127378854165807</v>
       </c>
       <c r="F16" t="n">
-        <v>202.2512005615234</v>
+        <v>202.6640008544922</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>55.14546999969277</v>
+        <v>60.16398949385513</v>
       </c>
       <c r="I16" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="J16" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17">
@@ -3529,31 +3529,31 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>215.5899963378906</v>
+        <v>216.2200012207031</v>
       </c>
       <c r="C17" t="n">
-        <v>0.6160414612916165</v>
+        <v>0.1760586032523825</v>
       </c>
       <c r="D17" t="n">
-        <v>201.5434494781494</v>
+        <v>201.6983995056152</v>
       </c>
       <c r="E17" t="n">
-        <v>6.96948816551047</v>
+        <v>7.199661351147014</v>
       </c>
       <c r="F17" t="n">
-        <v>214.0269995117187</v>
+        <v>214.4651995849609</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>55.92105593377158</v>
+        <v>60.39064883485165</v>
       </c>
       <c r="I17" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="J17" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18">
@@ -3563,31 +3563,16 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>236.9199981689453</v>
-      </c>
-      <c r="C18" t="n">
-        <v/>
-      </c>
-      <c r="D18" t="n">
-        <v/>
-      </c>
-      <c r="E18" t="n">
-        <v/>
-      </c>
-      <c r="F18" t="n">
-        <v/>
+        <v>236.9499969482422</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
       </c>
-      <c r="H18" t="n">
-        <v/>
-      </c>
       <c r="I18" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J18" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19">
@@ -3597,28 +3582,28 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>34.27999877929688</v>
+        <v>34.54000091552734</v>
       </c>
       <c r="C19" t="n">
-        <v>1.15078016132264</v>
+        <v>-0.2022527985835465</v>
       </c>
       <c r="D19" t="n">
-        <v>28.51575001716614</v>
+        <v>28.56580001831055</v>
       </c>
       <c r="E19" t="n">
-        <v>20.21426320072496</v>
+        <v>20.91382315001632</v>
       </c>
       <c r="F19" t="n">
-        <v>31.95559986114502</v>
+        <v>32.16479988098145</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>84.39718902393659</v>
+        <v>78.05838353608104</v>
       </c>
       <c r="I19" t="n">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J19" t="n">
         <v>45</v>
@@ -3631,31 +3616,31 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>198.6300048828125</v>
+        <v>199.7400054931641</v>
       </c>
       <c r="C20" t="n">
-        <v>0.4094618990010401</v>
+        <v>0.1052506967132771</v>
       </c>
       <c r="D20" t="n">
-        <v>181.9523007202149</v>
+        <v>182.1817507171631</v>
       </c>
       <c r="E20" t="n">
-        <v>9.165975970945643</v>
+        <v>9.637768166615187</v>
       </c>
       <c r="F20" t="n">
-        <v>197.8132009887695</v>
+        <v>198.1710009765625</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>56.18200697890631</v>
+        <v>56.88535287810716</v>
       </c>
       <c r="I20" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J20" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21">
@@ -3665,31 +3650,31 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>162.2299957275391</v>
+        <v>161.5500030517578</v>
       </c>
       <c r="C21" t="n">
-        <v>0.2471691849215585</v>
+        <v>-0.3823118481765087</v>
       </c>
       <c r="D21" t="n">
-        <v>137.1264998245239</v>
+        <v>137.4429998397827</v>
       </c>
       <c r="E21" t="n">
-        <v>18.30681592189636</v>
+        <v>17.53963696956311</v>
       </c>
       <c r="F21" t="n">
-        <v>154.3326000976562</v>
+        <v>154.8394000244141</v>
       </c>
       <c r="G21" t="n">
         <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>82.88028028335664</v>
+        <v>70.52450472252418</v>
       </c>
       <c r="I21" t="n">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="J21" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22">
@@ -3699,31 +3684,31 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>454.25</v>
+        <v>453.5499877929688</v>
       </c>
       <c r="C22" t="n">
-        <v>0.3202323865110657</v>
+        <v>-0.2463381357221683</v>
       </c>
       <c r="D22" t="n">
-        <v>435.2630500793457</v>
+        <v>435.5070501708984</v>
       </c>
       <c r="E22" t="n">
-        <v>4.362178208601235</v>
+        <v>4.142972568409639</v>
       </c>
       <c r="F22" t="n">
-        <v>456.1260003662109</v>
+        <v>456.5518005371094</v>
       </c>
       <c r="G22" t="n">
         <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>59.2158434894163</v>
+        <v>50.31361443162904</v>
       </c>
       <c r="I22" t="n">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="J22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23">
@@ -3733,31 +3718,31 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>450.4100036621094</v>
+        <v>450.1400146484375</v>
       </c>
       <c r="C23" t="n">
-        <v>0.3117956985447146</v>
+        <v>-0.1486175803075862</v>
       </c>
       <c r="D23" t="n">
-        <v>431.7311000061035</v>
+        <v>431.9731001281738</v>
       </c>
       <c r="E23" t="n">
-        <v>4.326513344936645</v>
+        <v>4.205566160224616</v>
       </c>
       <c r="F23" t="n">
-        <v>452.2988012695312</v>
+        <v>452.7192010498047</v>
       </c>
       <c r="G23" t="n">
         <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>59.11312740785437</v>
+        <v>51.04990691555505</v>
       </c>
       <c r="I23" t="n">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="J23" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24">
@@ -3767,28 +3752,28 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>44.97999954223633</v>
+        <v>44.95000076293945</v>
       </c>
       <c r="C24" t="n">
-        <v>0.3569831514983024</v>
+        <v>-0.06669359626984006</v>
       </c>
       <c r="D24" t="n">
-        <v>42.82649999618531</v>
+        <v>42.86385000228882</v>
       </c>
       <c r="E24" t="n">
-        <v>5.028427600300847</v>
+        <v>4.866923434407401</v>
       </c>
       <c r="F24" t="n">
-        <v>44.81679992675781</v>
+        <v>44.83379997253418</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
       </c>
       <c r="H24" t="n">
-        <v>58.06451612903226</v>
+        <v>52.50259525583105</v>
       </c>
       <c r="I24" t="n">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J24" t="n">
         <v>10</v>
@@ -3807,25 +3792,25 @@
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>19.27180002212524</v>
+        <v>19.282350025177</v>
       </c>
       <c r="E25" t="n">
-        <v>3.467244944246185</v>
+        <v>3.410634637489304</v>
       </c>
       <c r="F25" t="n">
-        <v>20.28320007324219</v>
+        <v>20.29240009307861</v>
       </c>
       <c r="G25" t="n">
         <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>44.11763880902627</v>
+        <v>42.34592928411659</v>
       </c>
       <c r="I25" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J25" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26">
@@ -3835,31 +3820,31 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>528.3200073242188</v>
+        <v>536.3900146484375</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.1209948997753507</v>
+        <v>0.825190723390512</v>
       </c>
       <c r="D26" t="n">
-        <v>492.3493017578125</v>
+        <v>493.2011018371582</v>
       </c>
       <c r="E26" t="n">
-        <v>7.305932076674358</v>
+        <v>8.756856513580766</v>
       </c>
       <c r="F26" t="n">
-        <v>539.6692028808594</v>
+        <v>539.8012036132812</v>
       </c>
       <c r="G26" t="n">
         <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>42.97062229043811</v>
+        <v>52.98750937841459</v>
       </c>
       <c r="I26" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="J26" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27">
@@ -3869,31 +3854,31 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>96.05000305175781</v>
+        <v>98.06999969482422</v>
       </c>
       <c r="C27" t="n">
-        <v>0.3972038152874724</v>
+        <v>0.7602978011384653</v>
       </c>
       <c r="D27" t="n">
-        <v>83.96624977111816</v>
+        <v>84.11289978027344</v>
       </c>
       <c r="E27" t="n">
-        <v>14.39120279109583</v>
+        <v>16.59329300382064</v>
       </c>
       <c r="F27" t="n">
-        <v>94.33259994506835</v>
+        <v>94.74999984741211</v>
       </c>
       <c r="G27" t="n">
         <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>44.99278585562632</v>
+        <v>61.46965590545945</v>
       </c>
       <c r="I27" t="n">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="J27" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28">
@@ -3903,31 +3888,31 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>9.590000152587891</v>
+        <v>9.779999732971191</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>0.6172784392394215</v>
       </c>
       <c r="D28" t="n">
-        <v>8.385249993801118</v>
+        <v>8.399899990558625</v>
       </c>
       <c r="E28" t="n">
-        <v>14.36749243823854</v>
+        <v>16.42995445140752</v>
       </c>
       <c r="F28" t="n">
-        <v>9.426600036621094</v>
+        <v>9.467600021362305</v>
       </c>
       <c r="G28" t="n">
         <v>0</v>
       </c>
       <c r="H28" t="n">
-        <v>43.66195291260571</v>
+        <v>60.54885315426946</v>
       </c>
       <c r="I28" t="n">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="J28" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29">
@@ -3937,31 +3922,31 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>91.55999755859375</v>
+        <v>92.44000244140625</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.02184349427928334</v>
+        <v>0.5001077056798975</v>
       </c>
       <c r="D29" t="n">
-        <v>84.3671000289917</v>
+        <v>84.43450004577636</v>
       </c>
       <c r="E29" t="n">
-        <v>8.525713847139821</v>
+        <v>9.481316750012954</v>
       </c>
       <c r="F29" t="n">
-        <v>90.61580017089844</v>
+        <v>90.75980026245117</v>
       </c>
       <c r="G29" t="n">
         <v>0</v>
       </c>
       <c r="H29" t="n">
-        <v>69.35917815671807</v>
+        <v>65.85917127209967</v>
       </c>
       <c r="I29" t="n">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="J29" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30">
@@ -3971,31 +3956,31 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>65.73999786376953</v>
+        <v>66.41000366210938</v>
       </c>
       <c r="C30" t="n">
-        <v>1.670266224084727</v>
+        <v>0.3475420910743043</v>
       </c>
       <c r="D30" t="n">
-        <v>57.1796000289917</v>
+        <v>57.26380004882812</v>
       </c>
       <c r="E30" t="n">
-        <v>14.9710698053807</v>
+        <v>15.97205146267345</v>
       </c>
       <c r="F30" t="n">
-        <v>62.24019996643067</v>
+        <v>62.51900001525879</v>
       </c>
       <c r="G30" t="n">
         <v>0</v>
       </c>
       <c r="H30" t="n">
-        <v>74.08087861475965</v>
+        <v>75.80606199792771</v>
       </c>
       <c r="I30" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J30" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31">
@@ -4011,25 +3996,25 @@
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>87.00280010223389</v>
+        <v>87.20820007324218</v>
       </c>
       <c r="E31" t="n">
-        <v>13.08831356465982</v>
+        <v>12.82195860826754</v>
       </c>
       <c r="F31" t="n">
-        <v>95.64780029296875</v>
+        <v>96.09060028076172</v>
       </c>
       <c r="G31" t="n">
         <v>0</v>
       </c>
       <c r="H31" t="n">
-        <v>61.93025158519125</v>
+        <v>67.83070521020178</v>
       </c>
       <c r="I31" t="n">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="J31" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32">
@@ -4039,31 +4024,31 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>33.58000183105469</v>
+        <v>33.70999908447266</v>
       </c>
       <c r="C32" t="n">
-        <v>2.503063344122625</v>
+        <v>-0.0296623246393235</v>
       </c>
       <c r="D32" t="n">
-        <v>30.50405003547668</v>
+        <v>30.53270003318787</v>
       </c>
       <c r="E32" t="n">
-        <v>10.0837488530232</v>
+        <v>10.40621709783671</v>
       </c>
       <c r="F32" t="n">
-        <v>31.6092000579834</v>
+        <v>31.76600006103516</v>
       </c>
       <c r="G32" t="n">
         <v>0</v>
       </c>
       <c r="H32" t="n">
-        <v>74.13130825154062</v>
+        <v>76.19586391253554</v>
       </c>
       <c r="I32" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J32" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33">
@@ -4073,28 +4058,28 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>33.68000030517578</v>
+        <v>33.88999938964844</v>
       </c>
       <c r="C33" t="n">
-        <v>1.998788123144712</v>
+        <v>-0.08843980222953407</v>
       </c>
       <c r="D33" t="n">
-        <v>30.64610004425049</v>
+        <v>30.67505003929138</v>
       </c>
       <c r="E33" t="n">
-        <v>9.89979232771735</v>
+        <v>10.48066538192785</v>
       </c>
       <c r="F33" t="n">
-        <v>31.77360008239746</v>
+        <v>31.93240001678467</v>
       </c>
       <c r="G33" t="n">
         <v>0</v>
       </c>
       <c r="H33" t="n">
-        <v>69.03227235475225</v>
+        <v>73.82300995510549</v>
       </c>
       <c r="I33" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="J33" t="n">
         <v>29</v>
@@ -4107,25 +4092,25 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>33.81999969482422</v>
+        <v>33.95000076293945</v>
       </c>
       <c r="C34" t="n">
-        <v>2.267916561600036</v>
+        <v>-0.05887682380029124</v>
       </c>
       <c r="D34" t="n">
-        <v>30.63205002784729</v>
+        <v>30.6749000453949</v>
       </c>
       <c r="E34" t="n">
-        <v>10.40723576802335</v>
+        <v>10.67680974574597</v>
       </c>
       <c r="F34" t="n">
-        <v>31.51379989624023</v>
+        <v>31.66479991912842</v>
       </c>
       <c r="G34" t="n">
         <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>70.819684843391</v>
+        <v>74.04197412281607</v>
       </c>
       <c r="I34" t="n">
         <v>41</v>
@@ -4141,31 +4126,31 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>42.5</v>
+        <v>42.93000030517578</v>
       </c>
       <c r="C35" t="n">
-        <v>1.214570852934105</v>
+        <v>0.06992722198104762</v>
       </c>
       <c r="D35" t="n">
-        <v>35.07094997406006</v>
+        <v>35.16979997634888</v>
       </c>
       <c r="E35" t="n">
-        <v>21.18291643492628</v>
+        <v>22.06495440419199</v>
       </c>
       <c r="F35" t="n">
-        <v>39.59440002441406</v>
+        <v>39.82780006408692</v>
       </c>
       <c r="G35" t="n">
         <v>0</v>
       </c>
       <c r="H35" t="n">
-        <v>89.00334407825484</v>
+        <v>82.66793927854721</v>
       </c>
       <c r="I35" t="n">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J35" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36">
@@ -4175,31 +4160,31 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>152.8200073242188</v>
+        <v>154.8899993896484</v>
       </c>
       <c r="C36" t="n">
-        <v>1.138319755940165</v>
+        <v>0.4344431096109824</v>
       </c>
       <c r="D36" t="n">
-        <v>126.8969500732422</v>
+        <v>127.2423500823975</v>
       </c>
       <c r="E36" t="n">
-        <v>20.42843207501389</v>
+        <v>21.72833910199503</v>
       </c>
       <c r="F36" t="n">
-        <v>142.5377996826172</v>
+        <v>143.3645999145508</v>
       </c>
       <c r="G36" t="n">
         <v>0</v>
       </c>
       <c r="H36" t="n">
-        <v>88.62168357696586</v>
+        <v>85.90081861285971</v>
       </c>
       <c r="I36" t="n">
         <v>50</v>
       </c>
       <c r="J36" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37">
@@ -4209,31 +4194,31 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>152.6999969482422</v>
+        <v>154.5200042724609</v>
       </c>
       <c r="C37" t="n">
-        <v>0.998739653715619</v>
+        <v>-0.1228119922182302</v>
       </c>
       <c r="D37" t="n">
-        <v>125.8199496841431</v>
+        <v>126.1638497161865</v>
       </c>
       <c r="E37" t="n">
-        <v>21.36389923186146</v>
+        <v>22.47565734563694</v>
       </c>
       <c r="F37" t="n">
-        <v>140.9469998168945</v>
+        <v>141.8932000732422</v>
       </c>
       <c r="G37" t="n">
         <v>0</v>
       </c>
       <c r="H37" t="n">
-        <v>90.01984244822005</v>
+        <v>88.04991241743183</v>
       </c>
       <c r="I37" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J37" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38">
@@ -4249,25 +4234,25 @@
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>12.48590000629425</v>
+        <v>12.53000000476837</v>
       </c>
       <c r="E38" t="n">
-        <v>18.69388420020445</v>
+        <v>18.27613478997904</v>
       </c>
       <c r="F38" t="n">
-        <v>14.01739999771118</v>
+        <v>14.11099998474121</v>
       </c>
       <c r="G38" t="n">
         <v>0</v>
       </c>
       <c r="H38" t="n">
-        <v>79.06987575573426</v>
+        <v>78.7802685683757</v>
       </c>
       <c r="I38" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J38" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39">
@@ -4277,10 +4262,10 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>193.7299957275391</v>
+        <v>195.0599975585938</v>
       </c>
       <c r="C39" t="n">
-        <v>0.7698287269384041</v>
+        <v>0.8635390528031195</v>
       </c>
       <c r="D39" t="n">
         <v/>
@@ -4289,19 +4274,19 @@
         <v/>
       </c>
       <c r="F39" t="n">
-        <v>180.2637997436524</v>
+        <v>181.152399597168</v>
       </c>
       <c r="G39" t="n">
         <v>0</v>
       </c>
       <c r="H39" t="n">
-        <v>83.84620531076908</v>
+        <v>82.32131497545089</v>
       </c>
       <c r="I39" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J39" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40">
@@ -4311,31 +4296,31 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>47.68999862670898</v>
+        <v>47.97999954223633</v>
       </c>
       <c r="C40" t="n">
-        <v>1.836422724809728</v>
+        <v>0.4396045268166393</v>
       </c>
       <c r="D40" t="n">
-        <v>43.87349996566773</v>
+        <v>43.89934995651245</v>
       </c>
       <c r="E40" t="n">
-        <v>8.698869850884424</v>
+        <v>9.295466993853546</v>
       </c>
       <c r="F40" t="n">
-        <v>46.72920021057129</v>
+        <v>46.83380020141602</v>
       </c>
       <c r="G40" t="n">
         <v>0</v>
       </c>
       <c r="H40" t="n">
-        <v>70.35722070844687</v>
+        <v>67.18983562467321</v>
       </c>
       <c r="I40" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J40" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41">
@@ -4345,31 +4330,31 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>46.70000076293945</v>
+        <v>46.97999954223633</v>
       </c>
       <c r="C41" t="n">
-        <v>0.6682504362355957</v>
+        <v>0.3846160429704426</v>
       </c>
       <c r="D41" t="n">
-        <v>42.87709997177124</v>
+        <v>42.90299997329712</v>
       </c>
       <c r="E41" t="n">
-        <v>8.915949991219271</v>
+        <v>9.502830970973445</v>
       </c>
       <c r="F41" t="n">
-        <v>45.74879989624024</v>
+        <v>45.85219985961914</v>
       </c>
       <c r="G41" t="n">
         <v>0</v>
       </c>
       <c r="H41" t="n">
-        <v>67.27274198507874</v>
+        <v>65.58614331161073</v>
       </c>
       <c r="I41" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J41" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42">
@@ -4379,28 +4364,28 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>480.1499938964844</v>
+        <v>483.489990234375</v>
       </c>
       <c r="C42" t="n">
-        <v>0.8676116503783859</v>
+        <v>0.5218468939904186</v>
       </c>
       <c r="D42" t="n">
-        <v>439.7825991821289</v>
+        <v>440.0515492248535</v>
       </c>
       <c r="E42" t="n">
-        <v>9.178943139048103</v>
+        <v>9.871216471351572</v>
       </c>
       <c r="F42" t="n">
-        <v>469.5069995117187</v>
+        <v>470.6327996826172</v>
       </c>
       <c r="G42" t="n">
         <v>0</v>
       </c>
       <c r="H42" t="n">
-        <v>68.6473482777474</v>
+        <v>66.55612275231057</v>
       </c>
       <c r="I42" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J42" t="n">
         <v>26</v>
@@ -4413,31 +4398,31 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>15.27999973297119</v>
+        <v>15.60000038146973</v>
       </c>
       <c r="C43" t="n">
-        <v>0.1967195604668293</v>
+        <v>0.8403368597089678</v>
       </c>
       <c r="D43" t="n">
-        <v>13.11404999732971</v>
+        <v>13.13619999885559</v>
       </c>
       <c r="E43" t="n">
-        <v>16.51625345398646</v>
+        <v>18.75580748487978</v>
       </c>
       <c r="F43" t="n">
-        <v>14.50360000610352</v>
+        <v>14.59700002670288</v>
       </c>
       <c r="G43" t="n">
         <v>0</v>
       </c>
       <c r="H43" t="n">
-        <v>35.71424400839233</v>
+        <v>65.57961163313863</v>
       </c>
       <c r="I43" t="n">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="J43" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44">
@@ -4447,31 +4432,31 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>231.2599945068359</v>
+        <v>230.7899932861328</v>
       </c>
       <c r="C44" t="n">
-        <v>0.1819434134501252</v>
+        <v>-0.2937779975738297</v>
       </c>
       <c r="D44" t="n">
-        <v>217.4183000946045</v>
+        <v>217.5883000946045</v>
       </c>
       <c r="E44" t="n">
-        <v>6.366388848688706</v>
+        <v>6.06728081693197</v>
       </c>
       <c r="F44" t="n">
-        <v>229.5769998168945</v>
+        <v>229.9391998291016</v>
       </c>
       <c r="G44" t="n">
         <v>0</v>
       </c>
       <c r="H44" t="n">
-        <v>61.39860408488171</v>
+        <v>53.49778608280701</v>
       </c>
       <c r="I44" t="n">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="J44" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45">
@@ -4481,28 +4466,28 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>462.3500061035156</v>
+        <v>462.7999877929688</v>
       </c>
       <c r="C45" t="n">
-        <v>2.634965997980254</v>
+        <v>-0.6333896311392917</v>
       </c>
       <c r="D45" t="n">
-        <v>409.0212509155273</v>
+        <v>409.9015507507324</v>
       </c>
       <c r="E45" t="n">
-        <v>13.03813801082965</v>
+        <v>12.90515660293383</v>
       </c>
       <c r="F45" t="n">
-        <v>444.7418023681641</v>
+        <v>447.3554016113281</v>
       </c>
       <c r="G45" t="n">
         <v>0</v>
       </c>
       <c r="H45" t="n">
-        <v>57.45586037335945</v>
+        <v>58.39839557388669</v>
       </c>
       <c r="I45" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J45" t="n">
         <v>33</v>
@@ -4515,10 +4500,10 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>121.9700012207031</v>
+        <v>122.8099975585938</v>
       </c>
       <c r="C46" t="n">
-        <v>1.035453932538255</v>
+        <v>0.1712879992547434</v>
       </c>
       <c r="D46" t="n">
         <v/>
@@ -4533,13 +4518,13 @@
         <v>0</v>
       </c>
       <c r="H46" t="n">
-        <v>89.63590422708988</v>
+        <v>86.04274048896559</v>
       </c>
       <c r="I46" t="n">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J46" t="n">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47">
@@ -4555,25 +4540,25 @@
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>29.99665002822876</v>
+        <v>30.0096000289917</v>
       </c>
       <c r="E47" t="n">
-        <v>5.011726210615156</v>
+        <v>4.966410647154426</v>
       </c>
       <c r="F47" t="n">
-        <v>31.3242000579834</v>
+        <v>31.39880004882813</v>
       </c>
       <c r="G47" t="n">
         <v>0</v>
       </c>
       <c r="H47" t="n">
-        <v>57.03707471315523</v>
+        <v>52.18545559943068</v>
       </c>
       <c r="I47" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="J47" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48">
@@ -4583,31 +4568,31 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>114.7699966430664</v>
+        <v>115.1900024414062</v>
       </c>
       <c r="C48" t="n">
-        <v>0.5783857936943804</v>
+        <v>-0.181974940811036</v>
       </c>
       <c r="D48" t="n">
-        <v>105.9788501739502</v>
+        <v>106.1119002151489</v>
       </c>
       <c r="E48" t="n">
-        <v>8.295189516291899</v>
+        <v>8.555215963384761</v>
       </c>
       <c r="F48" t="n">
-        <v>112.3807998657227</v>
+        <v>112.672799987793</v>
       </c>
       <c r="G48" t="n">
         <v>0</v>
       </c>
       <c r="H48" t="n">
-        <v>60.91015273074307</v>
+        <v>63.48549162790322</v>
       </c>
       <c r="I48" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J48" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49">
@@ -4617,31 +4602,31 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>112.7399978637695</v>
+        <v>113.1999969482422</v>
       </c>
       <c r="C49" t="n">
-        <v>1.175623759316191</v>
+        <v>-0.2467451536908083</v>
       </c>
       <c r="D49" t="n">
-        <v>103.9900496673584</v>
+        <v>104.1235496520996</v>
       </c>
       <c r="E49" t="n">
-        <v>8.414216768239198</v>
+        <v>8.716997573045717</v>
       </c>
       <c r="F49" t="n">
-        <v>110.1071997070313</v>
+        <v>110.4209997558594</v>
       </c>
       <c r="G49" t="n">
         <v>0</v>
       </c>
       <c r="H49" t="n">
-        <v>63.06875154403965</v>
+        <v>63.48228939603072</v>
       </c>
       <c r="I49" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J49" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50">
@@ -4651,31 +4636,31 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>64.40000152587891</v>
+        <v>64.69999694824219</v>
       </c>
       <c r="C50" t="n">
-        <v>0.2490717114416618</v>
+        <v>0.09281800612666036</v>
       </c>
       <c r="D50" t="n">
-        <v>50.71569993972778</v>
+        <v>50.97804992675781</v>
       </c>
       <c r="E50" t="n">
-        <v>26.98237745395213</v>
+        <v>26.91736353430396</v>
       </c>
       <c r="F50" t="n">
-        <v>63.6215998840332</v>
+        <v>63.73439979553223</v>
       </c>
       <c r="G50" t="n">
         <v>0</v>
       </c>
       <c r="H50" t="n">
-        <v>57.82123758268736</v>
+        <v>58.43550719237708</v>
       </c>
       <c r="I50" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J50" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51">
@@ -4685,31 +4670,31 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>33.02999877929688</v>
+        <v>33.04000091552734</v>
       </c>
       <c r="C51" t="n">
-        <v>0.3951284115160769</v>
+        <v>-0.8700897077573488</v>
       </c>
       <c r="D51" t="n">
-        <v>28.91210006713867</v>
+        <v>28.98035007476807</v>
       </c>
       <c r="E51" t="n">
-        <v>14.24282118073666</v>
+        <v>14.00828778909003</v>
       </c>
       <c r="F51" t="n">
-        <v>32.33759998321533</v>
+        <v>32.41600002288818</v>
       </c>
       <c r="G51" t="n">
         <v>0</v>
       </c>
       <c r="H51" t="n">
-        <v>54.50980304159075</v>
+        <v>59.35323206596963</v>
       </c>
       <c r="I51" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="J51" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52">
@@ -4719,31 +4704,31 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>28.79000091552734</v>
+        <v>29.03000068664551</v>
       </c>
       <c r="C52" t="n">
-        <v>0.4185589079667373</v>
+        <v>0.0689433216334745</v>
       </c>
       <c r="D52" t="n">
-        <v>26.21260004043579</v>
+        <v>26.24180004119873</v>
       </c>
       <c r="E52" t="n">
-        <v>9.832679211965353</v>
+        <v>10.62503578668155</v>
       </c>
       <c r="F52" t="n">
-        <v>28.16540004730225</v>
+        <v>28.2492000579834</v>
       </c>
       <c r="G52" t="n">
         <v>0</v>
       </c>
       <c r="H52" t="n">
-        <v>68.24327981586347</v>
+        <v>69.93303165138573</v>
       </c>
       <c r="I52" t="n">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="J52" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="53">
@@ -4753,31 +4738,31 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>119.6900024414062</v>
+        <v>121.2900009155273</v>
       </c>
       <c r="C53" t="n">
-        <v>-0.05010234538099789</v>
+        <v>0.2811111830210766</v>
       </c>
       <c r="D53" t="n">
-        <v>102.8579500579834</v>
+        <v>103.039700050354</v>
       </c>
       <c r="E53" t="n">
-        <v>16.3643669487232</v>
+        <v>17.7119118711086</v>
       </c>
       <c r="F53" t="n">
-        <v>113.6134001159668</v>
+        <v>114.1330001831055</v>
       </c>
       <c r="G53" t="n">
         <v>0</v>
       </c>
       <c r="H53" t="n">
-        <v>84.11918162731746</v>
+        <v>81.88762238939523</v>
       </c>
       <c r="I53" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J53" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54">
@@ -4787,31 +4772,31 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>75.19999694824219</v>
+        <v>73.68000030517578</v>
       </c>
       <c r="C54" t="n">
-        <v>-1.221595085679616</v>
+        <v>-0.2977012397301304</v>
       </c>
       <c r="D54" t="n">
-        <v>70.3679497718811</v>
+        <v>70.51599979400635</v>
       </c>
       <c r="E54" t="n">
-        <v>6.866829560937362</v>
+        <v>4.486925691207975</v>
       </c>
       <c r="F54" t="n">
-        <v>73.71279968261719</v>
+        <v>73.73739974975587</v>
       </c>
       <c r="G54" t="n">
         <v>0</v>
       </c>
       <c r="H54" t="n">
-        <v>75.19027059416449</v>
+        <v>46.49418986361129</v>
       </c>
       <c r="I54" t="n">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="J54" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55">
@@ -4821,25 +4806,10 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>72.26000213623047</v>
-      </c>
-      <c r="C55" t="n">
-        <v/>
-      </c>
-      <c r="D55" t="n">
-        <v/>
-      </c>
-      <c r="E55" t="n">
-        <v/>
-      </c>
-      <c r="F55" t="n">
-        <v/>
+        <v>71.18000030517578</v>
       </c>
       <c r="G55" t="n">
         <v>0</v>
-      </c>
-      <c r="H55" t="n">
-        <v/>
       </c>
       <c r="I55" t="n">
         <v>54</v>

</xml_diff>

<commit_message>
Commit for fixing the issues.
</commit_message>
<xml_diff>
--- a/buy_low.xlsx
+++ b/buy_low.xlsx
@@ -1547,31 +1547,31 @@
         </is>
       </c>
       <c r="B2" s="5" t="n">
-        <v>2438.85009765625</v>
+        <v>2453.300048828125</v>
       </c>
       <c r="C2" s="5" t="n">
-        <v>-1.444677870733924</v>
+        <v>0.09179739112532559</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>2475.305007324219</v>
+        <v>2473.843256835938</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>-1.472744149108973</v>
+        <v>-0.8304167190482193</v>
       </c>
       <c r="F2" s="5" t="n">
-        <v>2548.706000976562</v>
+        <v>2543.328002929688</v>
       </c>
       <c r="G2" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="5" t="n">
-        <v>42.20490372005197</v>
+        <v>45.48869274494449</v>
       </c>
       <c r="I2" s="5" t="n">
         <v>3</v>
       </c>
       <c r="J2" s="6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" hidden="1">
@@ -1581,31 +1581,31 @@
         </is>
       </c>
       <c r="B3" s="5" t="n">
-        <v>3580.800048828125</v>
+        <v>3560.050048828125</v>
       </c>
       <c r="C3" s="5" t="n">
-        <v>2.877340419010177</v>
+        <v>-0.2186204188693086</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>3323.950998535156</v>
+        <v>3325.741500244141</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>7.727221322039968</v>
+        <v>7.045302485679773</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>3408.159990234375</v>
+        <v>3418.1419921875</v>
       </c>
       <c r="G3" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H3" s="5" t="n">
-        <v>71.8845173562848</v>
+        <v>67.82911466459805</v>
       </c>
       <c r="I3" s="5" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J3" s="6" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" hidden="1">
@@ -1615,31 +1615,31 @@
         </is>
       </c>
       <c r="B4" s="5" t="n">
-        <v>1501.099975585938</v>
+        <v>1506.949951171875</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>1.669546901640495</v>
+        <v>0.5739630744529212</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>1422.197501831055</v>
+        <v>1420.896751098633</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>5.54792661731561</v>
+        <v>6.056259894091958</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>1399.024990234375</v>
+        <v>1405.281987304687</v>
       </c>
       <c r="G4" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H4" s="5" t="n">
-        <v>73.32280324092426</v>
+        <v>73.60504057556201</v>
       </c>
       <c r="I4" s="5" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J4" s="6" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" hidden="1">
@@ -1649,31 +1649,31 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>1636.900024414062</v>
+        <v>1642.900024414062</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>0.3125367957673486</v>
+        <v>-0.06083094988433846</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>1629.465503540039</v>
+        <v>1629.685503540039</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>0.4562551866162191</v>
+        <v>0.8108632521623723</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>1632.905998535156</v>
+        <v>1630.611999511719</v>
       </c>
       <c r="G5" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H5" s="5" t="n">
-        <v>60.26475981085756</v>
+        <v>61.75024002971947</v>
       </c>
       <c r="I5" s="5" t="n">
         <v>13</v>
       </c>
       <c r="J5" s="6" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" hidden="1">
@@ -1683,31 +1683,31 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>990.5</v>
+        <v>987.7000122070312</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>1.252236135957063</v>
+        <v>-0.2121616096015466</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>914.3482531738281</v>
+        <v>914.8900033569336</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>8.328527621925099</v>
+        <v>7.958334726900686</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>969.1380053710938</v>
+        <v>970.6340051269531</v>
       </c>
       <c r="G6" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H6" s="5" t="n">
-        <v>64.22582268704463</v>
+        <v>61.89860050554522</v>
       </c>
       <c r="I6" s="5" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J6" s="6" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" hidden="1">
@@ -1717,28 +1717,28 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>588.3499755859375</v>
+        <v>597.2999877929688</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>-0.5661714639143223</v>
+        <v>0.1425057538002816</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>572.725749053955</v>
+        <v>572.610749053955</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>2.728046810849872</v>
+        <v>4.311696694448071</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>586.022998046875</v>
+        <v>586.3009985351563</v>
       </c>
       <c r="G7" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>57.27135858784958</v>
+        <v>62.33971807151516</v>
       </c>
       <c r="I7" s="5" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J7" s="6" t="n">
         <v>8</v>
@@ -1751,25 +1751,25 @@
         </is>
       </c>
       <c r="B8" s="5" t="n">
-        <v>2498.85009765625</v>
+        <v>2500.800048828125</v>
       </c>
       <c r="C8" s="5" t="n">
-        <v>-1.47461418802366</v>
+        <v>-0.2293989702175758</v>
       </c>
       <c r="D8" s="5" t="n">
-        <v>2585.193511962891</v>
+        <v>2584.797263183594</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>-3.33992074121684</v>
+        <v>-3.249663544289452</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>2584.676015625</v>
+        <v>2575.706015625</v>
       </c>
       <c r="G8" s="5" t="n">
         <v>1</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>39.68087930681767</v>
+        <v>40.67590602793034</v>
       </c>
       <c r="I8" s="5" t="n">
         <v>1</v>
@@ -1785,28 +1785,28 @@
         </is>
       </c>
       <c r="B9" s="5" t="n">
-        <v>7431.2998046875</v>
+        <v>7494.2998046875</v>
       </c>
       <c r="C9" s="5" t="n">
-        <v>0.5364147770469785</v>
+        <v>0.246122909403601</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>6614.499526367187</v>
+        <v>6621.756274414062</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>12.34863310616813</v>
+        <v>13.17692005132953</v>
       </c>
       <c r="F9" s="5" t="n">
-        <v>7326.7990625</v>
+        <v>7312.219052734375</v>
       </c>
       <c r="G9" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H9" s="5" t="n">
-        <v>60.92912672236771</v>
+        <v>64.03270622155677</v>
       </c>
       <c r="I9" s="5" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J9" s="6" t="n">
         <v>17</v>
@@ -1819,31 +1819,31 @@
         </is>
       </c>
       <c r="B10" s="5" t="n">
-        <v>3256.85009765625</v>
+        <v>3240.25</v>
       </c>
       <c r="C10" s="5" t="n">
-        <v>-0.07822926808295216</v>
+        <v>-1.144077492182138</v>
       </c>
       <c r="D10" s="5" t="n">
-        <v>3071.611247558594</v>
+        <v>3073.083997802734</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>6.030673648720668</v>
+        <v>5.43968216673511</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>3320.99099609375</v>
+        <v>3316.908999023437</v>
       </c>
       <c r="G10" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H10" s="5" t="n">
-        <v>49.20269279104048</v>
+        <v>46.12894854570784</v>
       </c>
       <c r="I10" s="5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J10" s="6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" hidden="1">
@@ -1853,31 +1853,31 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>3185.800048828125</v>
+        <v>3261.35009765625</v>
       </c>
       <c r="C11" s="5" t="n">
-        <v>-0.8558179934061605</v>
+        <v>-0.05668832873574337</v>
       </c>
       <c r="D11" s="5" t="n">
-        <v>2709.878250732422</v>
+        <v>2716.473001708984</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>17.56247897731464</v>
+        <v>20.05825552488368</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>3049.59900390625</v>
+        <v>3056.600004882812</v>
       </c>
       <c r="G11" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H11" s="5" t="n">
-        <v>67.57715800267991</v>
+        <v>74.51039025442756</v>
       </c>
       <c r="I11" s="5" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J11" s="6" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" hidden="1">
@@ -1887,31 +1887,31 @@
         </is>
       </c>
       <c r="B12" s="5" t="n">
-        <v>8571.650390625</v>
+        <v>8687.9501953125</v>
       </c>
       <c r="C12" s="5" t="n">
-        <v>1.299386562684046</v>
+        <v>0.5974814391659811</v>
       </c>
       <c r="D12" s="5" t="n">
-        <v>7638.565270996094</v>
+        <v>7656.515769042969</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>12.21544997686756</v>
+        <v>13.47132896192619</v>
       </c>
       <c r="F12" s="5" t="n">
-        <v>8272.870048828125</v>
+        <v>8283.578037109375</v>
       </c>
       <c r="G12" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H12" s="5" t="n">
-        <v>62.68093139777933</v>
+        <v>66.7951377946066</v>
       </c>
       <c r="I12" s="5" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J12" s="6" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13">
@@ -1921,28 +1921,28 @@
         </is>
       </c>
       <c r="B13" s="5" t="n">
-        <v>22317.75</v>
+        <v>22477.69921875</v>
       </c>
       <c r="C13" s="5" t="n">
-        <v>0.8618374885802416</v>
+        <v>1.343106912627601</v>
       </c>
       <c r="D13" s="5" t="n">
-        <v>20803.42822265625</v>
+        <v>20830.39172851562</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>7.279193415316796</v>
+        <v>7.90819256643794</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>22399.977109375</v>
+        <v>22382.6480859375</v>
       </c>
       <c r="G13" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>55.60147301249906</v>
+        <v>58.57435559117977</v>
       </c>
       <c r="I13" s="5" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J13" s="6" t="n">
         <v>12</v>
@@ -1955,31 +1955,31 @@
         </is>
       </c>
       <c r="B14" s="5" t="n">
-        <v>2487.25</v>
+        <v>2483.199951171875</v>
       </c>
       <c r="C14" s="5" t="n">
-        <v>-1.446260525012377</v>
+        <v>-0.2149885496082082</v>
       </c>
       <c r="D14" s="5" t="n">
-        <v>2506.085501708984</v>
+        <v>2504.114251708984</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>-0.7515905461381813</v>
+        <v>-0.8351975363279007</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>2574.075014648437</v>
+        <v>2569.924013671875</v>
       </c>
       <c r="G14" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>41.60982471634887</v>
+        <v>41.00398208361345</v>
       </c>
       <c r="I14" s="5" t="n">
         <v>2</v>
       </c>
       <c r="J14" s="6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -1989,31 +1989,31 @@
         </is>
       </c>
       <c r="B15" s="5" t="n">
-        <v>4567.14990234375</v>
+        <v>4574.35009765625</v>
       </c>
       <c r="C15" s="5" t="n">
-        <v>-0.03064216006387621</v>
+        <v>-0.7356350533011424</v>
       </c>
       <c r="D15" s="5" t="n">
-        <v>4552.526750488281</v>
+        <v>4556.565249023438</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.3212095756252343</v>
+        <v>0.3903126074321825</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>4753.02201171875</v>
+        <v>4734.549013671875</v>
       </c>
       <c r="G15" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>46.77443884311108</v>
+        <v>47.88098736632688</v>
       </c>
       <c r="I15" s="5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J15" s="6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
@@ -2023,31 +2023,31 @@
         </is>
       </c>
       <c r="B16" s="5" t="n">
-        <v>565.7000122070312</v>
+        <v>567.4500122070312</v>
       </c>
       <c r="C16" s="5" t="n">
-        <v>-0.702123909828245</v>
+        <v>0.3448297448331195</v>
       </c>
       <c r="D16" s="5" t="n">
-        <v>553.8657507324219</v>
+        <v>553.9797509765625</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>2.136666052912626</v>
+        <v>2.431543970104176</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>569.0450024414063</v>
+        <v>568.262001953125</v>
       </c>
       <c r="G16" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>52.09770543139894</v>
+        <v>53.84018881107965</v>
       </c>
       <c r="I16" s="5" t="n">
         <v>8</v>
       </c>
       <c r="J16" s="6" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" hidden="1">
@@ -2057,31 +2057,31 @@
         </is>
       </c>
       <c r="B17" s="5" t="n">
-        <v>1416.599975585938</v>
+        <v>1391.900024414062</v>
       </c>
       <c r="C17" s="5" t="n">
-        <v>-2.036587410377233</v>
+        <v>-0.4719324694985705</v>
       </c>
       <c r="D17" s="5" t="n">
-        <v>1247.199501342773</v>
+        <v>1248.704001464844</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>13.58246808636328</v>
+        <v>11.46757140052701</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>1323.330007324219</v>
+        <v>1327.845007324219</v>
       </c>
       <c r="G17" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>62.99814629034363</v>
+        <v>57.07248217399005</v>
       </c>
       <c r="I17" s="5" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="J17" s="6" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18">
@@ -2091,31 +2091,31 @@
         </is>
       </c>
       <c r="B18" s="5" t="n">
-        <v>4979.2001953125</v>
+        <v>5084.5498046875</v>
       </c>
       <c r="C18" s="5" t="n">
-        <v>-2.291034949819415</v>
+        <v>1.467767006336063</v>
       </c>
       <c r="D18" s="5" t="n">
-        <v>4673.370495605469</v>
+        <v>4675.825744628906</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>6.54409274836252</v>
+        <v>8.741216683023158</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>5041.3180078125</v>
+        <v>5039.477001953125</v>
       </c>
       <c r="G18" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>50.86312366304616</v>
+        <v>57.3263561752374</v>
       </c>
       <c r="I18" s="5" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J18" s="6" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19">
@@ -2125,31 +2125,31 @@
         </is>
       </c>
       <c r="B19" s="5" t="n">
-        <v>1350.5</v>
+        <v>1368.900024414062</v>
       </c>
       <c r="C19" s="5" t="n">
-        <v>-1.181723493619857</v>
+        <v>0.9476033422986196</v>
       </c>
       <c r="D19" s="5" t="n">
-        <v>1209.013247680664</v>
+        <v>1210.991748046875</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>11.70266352256768</v>
+        <v>13.03958318641451</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>1354.388002929687</v>
+        <v>1356.04400390625</v>
       </c>
       <c r="G19" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H19" s="5" t="n">
-        <v>51.88662703493427</v>
+        <v>57.38893887184976</v>
       </c>
       <c r="I19" s="5" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="J19" s="6" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" hidden="1">
@@ -2159,31 +2159,31 @@
         </is>
       </c>
       <c r="B20" s="5" t="n">
-        <v>1990.300048828125</v>
+        <v>1949.300048828125</v>
       </c>
       <c r="C20" s="5" t="n">
-        <v>-1.019494703709956</v>
+        <v>-0.7206652930116575</v>
       </c>
       <c r="D20" s="5" t="n">
-        <v>1646.151999511719</v>
+        <v>1649.907499389648</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>20.90621336416609</v>
+        <v>18.14602027987819</v>
       </c>
       <c r="F20" s="5" t="n">
-        <v>1926.626000976562</v>
+        <v>1934.899001464844</v>
       </c>
       <c r="G20" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H20" s="5" t="n">
-        <v>56.65375823098906</v>
+        <v>46.83202484057886</v>
       </c>
       <c r="I20" s="5" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="J20" s="6" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21">
@@ -2193,31 +2193,31 @@
         </is>
       </c>
       <c r="B21" s="8" t="n">
-        <v>40847.19921875</v>
+        <v>40036.3515625</v>
       </c>
       <c r="C21" s="8" t="n">
-        <v>-2.027584176692232</v>
+        <v>-0.4473277282193155</v>
       </c>
       <c r="D21" s="8" t="n">
-        <v>39973.39896484375</v>
+        <v>39906.5512109375</v>
       </c>
       <c r="E21" s="8" t="n">
-        <v>2.185954350979136</v>
+        <v>0.3252607595088972</v>
       </c>
       <c r="F21" s="8" t="n">
-        <v>38798.1759375</v>
+        <v>38926.349921875</v>
       </c>
       <c r="G21" s="8" t="n">
         <v>0</v>
       </c>
       <c r="H21" s="8" t="n">
-        <v>55.83949325016842</v>
+        <v>49.38908192089843</v>
       </c>
       <c r="I21" s="8" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J21" s="9" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2314,25 +2314,25 @@
         </is>
       </c>
       <c r="B2" s="5" t="n">
-        <v>22897.25</v>
+        <v>22910.599609375</v>
       </c>
       <c r="C2" s="5" t="n">
-        <v>-0.3822024305657923</v>
+        <v>-0.4066691430087532</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>21956.60350585937</v>
+        <v>21985.02025390625</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>4.284116593395714</v>
+        <v>4.210045498158214</v>
       </c>
       <c r="F2" s="5" t="n">
-        <v>23436.7129296875</v>
+        <v>23424.7039453125</v>
       </c>
       <c r="G2" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="5" t="n">
-        <v>43.53609332739748</v>
+        <v>44.1927780961856</v>
       </c>
       <c r="I2" s="5" t="n">
         <v>6</v>
@@ -2348,31 +2348,31 @@
         </is>
       </c>
       <c r="B3" s="5" t="n">
-        <v>2674.199951171875</v>
+        <v>2641.300048828125</v>
       </c>
       <c r="C3" s="5" t="n">
-        <v>-2.832329412925227</v>
+        <v>-0.6936723816853063</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>2413.395994873047</v>
+        <v>2416.477995605469</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>10.80651318113037</v>
+        <v>9.303707860427895</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>2733.612001953125</v>
+        <v>2741.355</v>
       </c>
       <c r="G3" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H3" s="5" t="n">
-        <v>42.40650058538354</v>
+        <v>39.23515199231478</v>
       </c>
       <c r="I3" s="5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J3" s="6" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
@@ -2382,31 +2382,31 @@
         </is>
       </c>
       <c r="B4" s="5" t="n">
-        <v>3256.85009765625</v>
+        <v>3240.25</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>-0.07822926808295216</v>
+        <v>-1.144077492182138</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>3071.611247558594</v>
+        <v>3073.083997802734</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>6.030673648720668</v>
+        <v>5.43968216673511</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>3320.99099609375</v>
+        <v>3316.908999023437</v>
       </c>
       <c r="G4" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H4" s="5" t="n">
-        <v>49.20269279104048</v>
+        <v>46.12894854570784</v>
       </c>
       <c r="I4" s="5" t="n">
         <v>8</v>
       </c>
       <c r="J4" s="6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" hidden="1">
@@ -2416,31 +2416,31 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>1542.449951171875</v>
+        <v>1550.900024414062</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>-0.4678324984470406</v>
+        <v>-0.1223611768621735</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>1455.278999633789</v>
+        <v>1454.459000244141</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>5.989982096905265</v>
+        <v>6.630714523663678</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>1549.665</v>
+        <v>1546.875002441406</v>
       </c>
       <c r="G5" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H5" s="5" t="n">
-        <v>58.34025335345209</v>
+        <v>60.3421920789576</v>
       </c>
       <c r="I5" s="5" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="J5" s="6" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
@@ -2450,25 +2450,25 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>7133</v>
+        <v>7125.0498046875</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>-0.7264960459494874</v>
+        <v>0.4490160787516961</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>6549.869260253906</v>
+        <v>6555.981760253906</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>8.902937090434214</v>
+        <v>8.680134650215296</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>7314.073994140625</v>
+        <v>7312.2169921875</v>
       </c>
       <c r="G6" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H6" s="5" t="n">
-        <v>42.88660900096254</v>
+        <v>43.18170575629154</v>
       </c>
       <c r="I6" s="5" t="n">
         <v>5</v>
@@ -2484,31 +2484,31 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>7431.2998046875</v>
+        <v>7494.2998046875</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>0.5364147770469785</v>
+        <v>0.246122909403601</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>6614.499526367187</v>
+        <v>6621.756274414062</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>12.34863310616813</v>
+        <v>13.17692005132953</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>7326.7990625</v>
+        <v>7312.219052734375</v>
       </c>
       <c r="G7" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>60.92912672236771</v>
+        <v>64.03270622155677</v>
       </c>
       <c r="I7" s="5" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J7" s="6" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">
@@ -2518,31 +2518,31 @@
         </is>
       </c>
       <c r="B8" s="5" t="n">
-        <v>1700.849975585938</v>
+        <v>1659.949951171875</v>
       </c>
       <c r="C8" s="5" t="n">
-        <v>-0.9809615220889967</v>
+        <v>-0.7414730525958202</v>
       </c>
       <c r="D8" s="5" t="n">
-        <v>1581.345003051758</v>
+        <v>1581.007752685547</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>7.557172679178358</v>
+        <v>4.993156950194241</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>1699.598002929687</v>
+        <v>1700.422001953125</v>
       </c>
       <c r="G8" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>50.10379760662235</v>
+        <v>41.59262572908468</v>
       </c>
       <c r="I8" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="J8" s="6" t="n">
         <v>10</v>
-      </c>
-      <c r="J8" s="6" t="n">
-        <v>14</v>
       </c>
     </row>
     <row r="9" hidden="1">
@@ -2552,31 +2552,31 @@
         </is>
       </c>
       <c r="B9" s="5" t="n">
-        <v>719.2000122070312</v>
+        <v>729</v>
       </c>
       <c r="C9" s="5" t="n">
-        <v>-0.3533062407992671</v>
+        <v>0.6906077348066253</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>624.880249633789</v>
+        <v>625.9874996948242</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>15.09405404131724</v>
+        <v>16.45599957753078</v>
       </c>
       <c r="F9" s="5" t="n">
-        <v>695.4030004882812</v>
+        <v>697.5140002441407</v>
       </c>
       <c r="G9" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H9" s="5" t="n">
-        <v>58.74461316229715</v>
+        <v>64.27016848122179</v>
       </c>
       <c r="I9" s="5" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="J9" s="6" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" hidden="1">
@@ -2586,31 +2586,31 @@
         </is>
       </c>
       <c r="B10" s="5" t="n">
-        <v>1990.300048828125</v>
+        <v>1949.300048828125</v>
       </c>
       <c r="C10" s="5" t="n">
-        <v>-1.019494703709956</v>
+        <v>-0.7206652930116575</v>
       </c>
       <c r="D10" s="5" t="n">
-        <v>1646.151999511719</v>
+        <v>1649.907499389648</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>20.90621336416609</v>
+        <v>18.14602027987819</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>1926.626000976562</v>
+        <v>1934.899001464844</v>
       </c>
       <c r="G10" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H10" s="5" t="n">
-        <v>56.65375823098906</v>
+        <v>46.83202484057886</v>
       </c>
       <c r="I10" s="5" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="J10" s="6" t="n">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" hidden="1">
@@ -2620,31 +2620,31 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>565.7000122070312</v>
+        <v>567.4500122070312</v>
       </c>
       <c r="C11" s="5" t="n">
-        <v>-0.702123909828245</v>
+        <v>0.3448297448331195</v>
       </c>
       <c r="D11" s="5" t="n">
-        <v>553.8657507324219</v>
+        <v>553.9797509765625</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>2.136666052912626</v>
+        <v>2.431543970104176</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>569.0450024414063</v>
+        <v>568.262001953125</v>
       </c>
       <c r="G11" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H11" s="5" t="n">
-        <v>52.09770543139894</v>
+        <v>53.84018881107965</v>
       </c>
       <c r="I11" s="5" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J11" s="6" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" hidden="1">
@@ -2654,31 +2654,31 @@
         </is>
       </c>
       <c r="B12" s="5" t="n">
-        <v>5863.5</v>
+        <v>6104.75</v>
       </c>
       <c r="C12" s="5" t="n">
-        <v>-2.860265320394251</v>
+        <v>4.250448665743156</v>
       </c>
       <c r="D12" s="5" t="n">
-        <v>4921.753251953125</v>
+        <v>4931.174252929687</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>19.13437549257791</v>
+        <v>23.79911329178995</v>
       </c>
       <c r="F12" s="5" t="n">
-        <v>5564.24400390625</v>
+        <v>5598.35900390625</v>
       </c>
       <c r="G12" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H12" s="5" t="n">
-        <v>61.4923623824867</v>
+        <v>69.29575723069195</v>
       </c>
       <c r="I12" s="5" t="n">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="J12" s="6" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" hidden="1">
@@ -2688,31 +2688,31 @@
         </is>
       </c>
       <c r="B13" s="5" t="n">
-        <v>1461.75</v>
+        <v>1538.550048828125</v>
       </c>
       <c r="C13" s="5" t="n">
-        <v>0.0890170065110274</v>
+        <v>-0.3562060701448266</v>
       </c>
       <c r="D13" s="5" t="n">
-        <v>1334.859247436523</v>
+        <v>1337.100997924805</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>9.50592752061004</v>
+        <v>15.06610579275398</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>1414.72099609375</v>
+        <v>1419.532998046875</v>
       </c>
       <c r="G13" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>64.32932551248233</v>
+        <v>77.01492755840997</v>
       </c>
       <c r="I13" s="5" t="n">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J13" s="6" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" hidden="1">
@@ -2722,31 +2722,31 @@
         </is>
       </c>
       <c r="B14" s="5" t="n">
-        <v>1416.599975585938</v>
+        <v>1391.900024414062</v>
       </c>
       <c r="C14" s="5" t="n">
-        <v>-2.036587410377233</v>
+        <v>-0.4719324694985705</v>
       </c>
       <c r="D14" s="5" t="n">
-        <v>1247.199501342773</v>
+        <v>1248.704001464844</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>13.58246808636328</v>
+        <v>11.46757140052701</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>1323.330007324219</v>
+        <v>1327.845007324219</v>
       </c>
       <c r="G14" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>62.99814629034363</v>
+        <v>57.07248217399005</v>
       </c>
       <c r="I14" s="5" t="n">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="J14" s="6" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" hidden="1">
@@ -2756,31 +2756,31 @@
         </is>
       </c>
       <c r="B15" s="5" t="n">
-        <v>1282.400024414062</v>
+        <v>1283.599975585938</v>
       </c>
       <c r="C15" s="5" t="n">
-        <v>0.06632402587123387</v>
+        <v>0.6547716593560127</v>
       </c>
       <c r="D15" s="5" t="n">
-        <v>1114.257746582031</v>
+        <v>1115.762996826172</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>15.09007034932492</v>
+        <v>15.0423503232482</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>1164.686005859375</v>
+        <v>1168.155004882813</v>
       </c>
       <c r="G15" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>79.80539785772331</v>
+        <v>77.30624507569753</v>
       </c>
       <c r="I15" s="5" t="n">
         <v>37</v>
       </c>
       <c r="J15" s="6" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" hidden="1">
@@ -2790,28 +2790,28 @@
         </is>
       </c>
       <c r="B16" s="5" t="n">
-        <v>2630.89990234375</v>
+        <v>2665.550048828125</v>
       </c>
       <c r="C16" s="5" t="n">
-        <v>-1.238785285098964</v>
+        <v>1.57958727294345</v>
       </c>
       <c r="D16" s="5" t="n">
-        <v>2071.979250488281</v>
+        <v>2076.990001220703</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>26.97520507137096</v>
+        <v>28.33716326325641</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>2462.384013671875</v>
+        <v>2476.454013671875</v>
       </c>
       <c r="G16" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>62.33950149865779</v>
+        <v>64.49653848393541</v>
       </c>
       <c r="I16" s="5" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J16" s="6" t="n">
         <v>36</v>
@@ -2824,31 +2824,31 @@
         </is>
       </c>
       <c r="B17" s="5" t="n">
-        <v>1636.900024414062</v>
+        <v>1642.900024414062</v>
       </c>
       <c r="C17" s="5" t="n">
-        <v>0.3125367957673486</v>
+        <v>-0.06083094988433846</v>
       </c>
       <c r="D17" s="5" t="n">
-        <v>1629.465503540039</v>
+        <v>1629.685503540039</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>0.4562551866162191</v>
+        <v>0.8108632521623723</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>1632.905998535156</v>
+        <v>1630.611999511719</v>
       </c>
       <c r="G17" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>60.26475981085756</v>
+        <v>61.75024002971947</v>
       </c>
       <c r="I17" s="5" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J17" s="6" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" hidden="1">
@@ -2858,31 +2858,31 @@
         </is>
       </c>
       <c r="B18" s="5" t="n">
-        <v>660.9500122070312</v>
+        <v>645.4500122070312</v>
       </c>
       <c r="C18" s="5" t="n">
-        <v>-1.151575850726805</v>
+        <v>-0.7305444341467515</v>
       </c>
       <c r="D18" s="5" t="n">
-        <v>577.6797496032715</v>
+        <v>578.3622499084472</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>14.41460647719547</v>
+        <v>11.59960946780392</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>648.467998046875</v>
+        <v>647.9689990234375</v>
       </c>
       <c r="G18" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>62.24856356578118</v>
+        <v>50.37696903960684</v>
       </c>
       <c r="I18" s="5" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="J18" s="6" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19">
@@ -2892,28 +2892,28 @@
         </is>
       </c>
       <c r="B19" s="5" t="n">
-        <v>2498.85009765625</v>
+        <v>2500.800048828125</v>
       </c>
       <c r="C19" s="5" t="n">
-        <v>-1.47461418802366</v>
+        <v>-0.2293989702175758</v>
       </c>
       <c r="D19" s="5" t="n">
-        <v>2585.193511962891</v>
+        <v>2584.797263183594</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>-3.33992074121684</v>
+        <v>-3.249663544289452</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>2584.676015625</v>
+        <v>2575.706015625</v>
       </c>
       <c r="G19" s="5" t="n">
         <v>1</v>
       </c>
       <c r="H19" s="5" t="n">
-        <v>39.68087930681767</v>
+        <v>40.67590602793034</v>
       </c>
       <c r="I19" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J19" s="6" t="n">
         <v>1</v>
@@ -2926,28 +2926,28 @@
         </is>
       </c>
       <c r="B20" s="5" t="n">
-        <v>990.5</v>
+        <v>987.7000122070312</v>
       </c>
       <c r="C20" s="5" t="n">
-        <v>1.252236135957063</v>
+        <v>-0.2121616096015466</v>
       </c>
       <c r="D20" s="5" t="n">
-        <v>914.3482531738281</v>
+        <v>914.8900033569336</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>8.328527621925099</v>
+        <v>7.958334726900686</v>
       </c>
       <c r="F20" s="5" t="n">
-        <v>969.1380053710938</v>
+        <v>970.6340051269531</v>
       </c>
       <c r="G20" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H20" s="5" t="n">
-        <v>64.22582268704463</v>
+        <v>61.89860050554522</v>
       </c>
       <c r="I20" s="5" t="n">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="J20" s="6" t="n">
         <v>16</v>
@@ -2960,31 +2960,31 @@
         </is>
       </c>
       <c r="B21" s="5" t="n">
-        <v>1350.5</v>
+        <v>1368.900024414062</v>
       </c>
       <c r="C21" s="5" t="n">
-        <v>-1.181723493619857</v>
+        <v>0.9476033422986196</v>
       </c>
       <c r="D21" s="5" t="n">
-        <v>1209.013247680664</v>
+        <v>1210.991748046875</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>11.70266352256768</v>
+        <v>13.03958318641451</v>
       </c>
       <c r="F21" s="5" t="n">
-        <v>1354.388002929687</v>
+        <v>1356.04400390625</v>
       </c>
       <c r="G21" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H21" s="5" t="n">
-        <v>51.88662703493427</v>
+        <v>57.38893887184976</v>
       </c>
       <c r="I21" s="5" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="J21" s="6" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22">
@@ -2994,31 +2994,31 @@
         </is>
       </c>
       <c r="B22" s="5" t="n">
-        <v>554.5499877929688</v>
+        <v>569.5</v>
       </c>
       <c r="C22" s="5" t="n">
-        <v>-3.815800965362248</v>
+        <v>0.494086418326356</v>
       </c>
       <c r="D22" s="5" t="n">
-        <v>481.7767500305176</v>
+        <v>482.8872500610352</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>15.10517843749028</v>
+        <v>17.93643338647216</v>
       </c>
       <c r="F22" s="5" t="n">
-        <v>565.2599987792969</v>
+        <v>565.2239990234375</v>
       </c>
       <c r="G22" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H22" s="5" t="n">
-        <v>49.31795284489768</v>
+        <v>55.66201839291925</v>
       </c>
       <c r="I22" s="5" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J22" s="6" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" hidden="1">
@@ -3028,31 +3028,31 @@
         </is>
       </c>
       <c r="B23" s="5" t="n">
-        <v>1501.099975585938</v>
+        <v>1506.949951171875</v>
       </c>
       <c r="C23" s="5" t="n">
-        <v>1.669546901640495</v>
+        <v>0.5739630744529212</v>
       </c>
       <c r="D23" s="5" t="n">
-        <v>1422.197501831055</v>
+        <v>1420.896751098633</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>5.54792661731561</v>
+        <v>6.056259894091958</v>
       </c>
       <c r="F23" s="5" t="n">
-        <v>1399.024990234375</v>
+        <v>1405.281987304687</v>
       </c>
       <c r="G23" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H23" s="5" t="n">
-        <v>73.32280324092426</v>
+        <v>73.60504057556201</v>
       </c>
       <c r="I23" s="5" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J23" s="6" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" hidden="1">
@@ -3062,31 +3062,31 @@
         </is>
       </c>
       <c r="B24" s="5" t="n">
-        <v>451.1499938964844</v>
+        <v>449.9500122070312</v>
       </c>
       <c r="C24" s="5" t="n">
-        <v>0.8832695844436689</v>
+        <v>-0.7827977492764648</v>
       </c>
       <c r="D24" s="5" t="n">
-        <v>403.8042501831055</v>
+        <v>404.9162503051758</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>11.72492456231204</v>
+        <v>11.12174724227902</v>
       </c>
       <c r="F24" s="5" t="n">
-        <v>458.05</v>
+        <v>457.29</v>
       </c>
       <c r="G24" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H24" s="5" t="n">
-        <v>53.00223928293671</v>
+        <v>51.29503284359539</v>
       </c>
       <c r="I24" s="5" t="n">
         <v>13</v>
       </c>
       <c r="J24" s="6" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" hidden="1">
@@ -3096,31 +3096,31 @@
         </is>
       </c>
       <c r="B25" s="5" t="n">
-        <v>1811.199951171875</v>
+        <v>1821.550048828125</v>
       </c>
       <c r="C25" s="5" t="n">
-        <v>0.1825281660075229</v>
+        <v>-0.1671559135493883</v>
       </c>
       <c r="D25" s="5" t="n">
-        <v>1829.403251342774</v>
+        <v>1828.267751464844</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>-0.9950403311865421</v>
+        <v>-0.36743538419558</v>
       </c>
       <c r="F25" s="5" t="n">
-        <v>1829.327993164062</v>
+        <v>1827.719995117187</v>
       </c>
       <c r="G25" s="5" t="n">
         <v>1</v>
       </c>
       <c r="H25" s="5" t="n">
-        <v>55.3269513780625</v>
+        <v>58.07465653425648</v>
       </c>
       <c r="I25" s="5" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="J25" s="6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" hidden="1">
@@ -3130,28 +3130,28 @@
         </is>
       </c>
       <c r="B26" s="5" t="n">
-        <v>581.25</v>
+        <v>580.7999877929688</v>
       </c>
       <c r="C26" s="5" t="n">
-        <v>-0.5475253897159083</v>
+        <v>-0.4456696112937419</v>
       </c>
       <c r="D26" s="5" t="n">
-        <v>520.5475012207031</v>
+        <v>521.4897512817383</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>11.66127944845519</v>
+        <v>11.37323147107979</v>
       </c>
       <c r="F26" s="5" t="n">
-        <v>556.97</v>
+        <v>558.9540002441406</v>
       </c>
       <c r="G26" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H26" s="5" t="n">
-        <v>59.4552173393257</v>
+        <v>58.26950960408997</v>
       </c>
       <c r="I26" s="5" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J26" s="6" t="n">
         <v>21</v>
@@ -3164,25 +3164,25 @@
         </is>
       </c>
       <c r="B27" s="5" t="n">
-        <v>332.1499938964844</v>
+        <v>336.5</v>
       </c>
       <c r="C27" s="5" t="n">
-        <v>-1.248702878197261</v>
+        <v>-0.4437869822485174</v>
       </c>
       <c r="D27" s="5" t="n">
-        <v>257.96049949646</v>
+        <v>258.7402494049072</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>28.76002122218037</v>
+        <v>30.05321003359055</v>
       </c>
       <c r="F27" s="5" t="n">
-        <v>310.8129992675781</v>
+        <v>312.8979992675781</v>
       </c>
       <c r="G27" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H27" s="5" t="n">
-        <v>66.16159840866175</v>
+        <v>67.92372102089455</v>
       </c>
       <c r="I27" s="5" t="n">
         <v>31</v>
@@ -3198,31 +3198,31 @@
         </is>
       </c>
       <c r="B28" s="5" t="n">
-        <v>22317.75</v>
+        <v>22477.69921875</v>
       </c>
       <c r="C28" s="5" t="n">
-        <v>0.8618374885802416</v>
+        <v>1.343106912627601</v>
       </c>
       <c r="D28" s="5" t="n">
-        <v>20803.42822265625</v>
+        <v>20830.39172851562</v>
       </c>
       <c r="E28" s="5" t="n">
-        <v>7.279193415316796</v>
+        <v>7.90819256643794</v>
       </c>
       <c r="F28" s="5" t="n">
-        <v>22399.977109375</v>
+        <v>22382.6480859375</v>
       </c>
       <c r="G28" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H28" s="5" t="n">
-        <v>55.60147301249906</v>
+        <v>58.57435559117977</v>
       </c>
       <c r="I28" s="5" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="J28" s="6" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" hidden="1">
@@ -3232,31 +3232,31 @@
         </is>
       </c>
       <c r="B29" s="5" t="n">
-        <v>1000.900024414062</v>
+        <v>1020.900024414062</v>
       </c>
       <c r="C29" s="5" t="n">
-        <v>0.04998000677707282</v>
+        <v>0.635813704905841</v>
       </c>
       <c r="D29" s="5" t="n">
-        <v>917.01125</v>
+        <v>918.3565002441406</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>9.14806382299699</v>
+        <v>11.16598228930281</v>
       </c>
       <c r="F29" s="5" t="n">
-        <v>964.5890026855469</v>
+        <v>966.5520031738281</v>
       </c>
       <c r="G29" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H29" s="5" t="n">
-        <v>62.67638759359586</v>
+        <v>68.60308024082187</v>
       </c>
       <c r="I29" s="5" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="J29" s="6" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" hidden="1">
@@ -3266,31 +3266,31 @@
         </is>
       </c>
       <c r="B30" s="5" t="n">
-        <v>40847.19921875</v>
+        <v>40036.3515625</v>
       </c>
       <c r="C30" s="5" t="n">
-        <v>-2.027584176692232</v>
+        <v>-0.4473277282193155</v>
       </c>
       <c r="D30" s="5" t="n">
-        <v>39973.39896484375</v>
+        <v>39906.5512109375</v>
       </c>
       <c r="E30" s="5" t="n">
-        <v>2.185954350979136</v>
+        <v>0.3252607595088972</v>
       </c>
       <c r="F30" s="5" t="n">
-        <v>38798.1759375</v>
+        <v>38926.349921875</v>
       </c>
       <c r="G30" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H30" s="5" t="n">
-        <v>55.83949325016842</v>
+        <v>49.38908192089843</v>
       </c>
       <c r="I30" s="5" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="J30" s="6" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31">
@@ -3300,28 +3300,28 @@
         </is>
       </c>
       <c r="B31" s="5" t="n">
-        <v>3841.699951171875</v>
+        <v>3849.199951171875</v>
       </c>
       <c r="C31" s="5" t="n">
-        <v>-0.1169985975021604</v>
+        <v>-0.01039449486243127</v>
       </c>
       <c r="D31" s="5" t="n">
-        <v>3931.816245117187</v>
+        <v>3926.043746337891</v>
       </c>
       <c r="E31" s="5" t="n">
-        <v>-2.291976235085385</v>
+        <v>-1.957283212590119</v>
       </c>
       <c r="F31" s="5" t="n">
-        <v>3876.42</v>
+        <v>3878.777998046875</v>
       </c>
       <c r="G31" s="5" t="n">
         <v>1</v>
       </c>
       <c r="H31" s="5" t="n">
-        <v>44.58942754718834</v>
+        <v>46.36292464227922</v>
       </c>
       <c r="I31" s="5" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J31" s="6" t="n">
         <v>2</v>
@@ -3334,31 +3334,31 @@
         </is>
       </c>
       <c r="B32" s="5" t="n">
-        <v>17099.30078125</v>
+        <v>17230.849609375</v>
       </c>
       <c r="C32" s="5" t="n">
-        <v>-1.387548970610486</v>
+        <v>-0.5262116997171273</v>
       </c>
       <c r="D32" s="5" t="n">
-        <v>14343.11224121094</v>
+        <v>14376.53099121094</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>19.21611219160596</v>
+        <v>19.85401499088372</v>
       </c>
       <c r="F32" s="5" t="n">
-        <v>15681.008984375</v>
+        <v>15786.58697265625</v>
       </c>
       <c r="G32" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H32" s="5" t="n">
-        <v>66.68597853815652</v>
+        <v>66.94954480416396</v>
       </c>
       <c r="I32" s="5" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J32" s="6" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33">
@@ -3368,31 +3368,31 @@
         </is>
       </c>
       <c r="B33" s="5" t="n">
-        <v>2487.25</v>
+        <v>2483.199951171875</v>
       </c>
       <c r="C33" s="5" t="n">
-        <v>-1.446260525012377</v>
+        <v>-0.2149885496082082</v>
       </c>
       <c r="D33" s="5" t="n">
-        <v>2506.085501708984</v>
+        <v>2504.114251708984</v>
       </c>
       <c r="E33" s="5" t="n">
-        <v>-0.7515905461381813</v>
+        <v>-0.8351975363279007</v>
       </c>
       <c r="F33" s="5" t="n">
-        <v>2574.075014648437</v>
+        <v>2569.924013671875</v>
       </c>
       <c r="G33" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H33" s="5" t="n">
-        <v>41.60982471634887</v>
+        <v>41.00398208361345</v>
       </c>
       <c r="I33" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J33" s="6" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" hidden="1">
@@ -3402,31 +3402,31 @@
         </is>
       </c>
       <c r="B34" s="5" t="n">
-        <v>7151.25</v>
+        <v>7262.10009765625</v>
       </c>
       <c r="C34" s="5" t="n">
-        <v>0.6481141054671458</v>
+        <v>-0.0694881040760098</v>
       </c>
       <c r="D34" s="5" t="n">
-        <v>6228.109750976562</v>
+        <v>6244.81375</v>
       </c>
       <c r="E34" s="5" t="n">
-        <v>14.82215770007409</v>
+        <v>16.29009908672216</v>
       </c>
       <c r="F34" s="5" t="n">
-        <v>7051.612998046875</v>
+        <v>7063.765</v>
       </c>
       <c r="G34" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H34" s="5" t="n">
-        <v>54.85444513763437</v>
+        <v>62.99002924189784</v>
       </c>
       <c r="I34" s="5" t="n">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="J34" s="6" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" hidden="1">
@@ -3436,31 +3436,31 @@
         </is>
       </c>
       <c r="B35" s="5" t="n">
-        <v>3580.800048828125</v>
+        <v>3560.050048828125</v>
       </c>
       <c r="C35" s="5" t="n">
-        <v>2.877340419010177</v>
+        <v>-0.2186204188693086</v>
       </c>
       <c r="D35" s="5" t="n">
-        <v>3323.950998535156</v>
+        <v>3325.741500244141</v>
       </c>
       <c r="E35" s="5" t="n">
-        <v>7.727221322039968</v>
+        <v>7.045302485679773</v>
       </c>
       <c r="F35" s="5" t="n">
-        <v>3408.159990234375</v>
+        <v>3418.1419921875</v>
       </c>
       <c r="G35" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H35" s="5" t="n">
-        <v>71.8845173562848</v>
+        <v>67.82911466459805</v>
       </c>
       <c r="I35" s="5" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J35" s="6" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" hidden="1">
@@ -3470,31 +3470,31 @@
         </is>
       </c>
       <c r="B36" s="5" t="n">
-        <v>3185.800048828125</v>
+        <v>3261.35009765625</v>
       </c>
       <c r="C36" s="5" t="n">
-        <v>-0.8558179934061605</v>
+        <v>-0.05668832873574337</v>
       </c>
       <c r="D36" s="5" t="n">
-        <v>2709.878250732422</v>
+        <v>2716.473001708984</v>
       </c>
       <c r="E36" s="5" t="n">
-        <v>17.56247897731464</v>
+        <v>20.05825552488368</v>
       </c>
       <c r="F36" s="5" t="n">
-        <v>3049.59900390625</v>
+        <v>3056.600004882812</v>
       </c>
       <c r="G36" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H36" s="5" t="n">
-        <v>67.57715800267991</v>
+        <v>74.51039025442756</v>
       </c>
       <c r="I36" s="5" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J36" s="6" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" hidden="1">
@@ -3504,31 +3504,31 @@
         </is>
       </c>
       <c r="B37" s="5" t="n">
-        <v>1686.400024414062</v>
+        <v>1650.75</v>
       </c>
       <c r="C37" s="5" t="n">
-        <v>-0.7737356380372429</v>
+        <v>1.341394515221839</v>
       </c>
       <c r="D37" s="5" t="n">
-        <v>1430.830001220703</v>
+        <v>1432.235001831055</v>
       </c>
       <c r="E37" s="5" t="n">
-        <v>17.86166232014437</v>
+        <v>15.25692347202678</v>
       </c>
       <c r="F37" s="5" t="n">
-        <v>1531.571003417969</v>
+        <v>1537.892001953125</v>
       </c>
       <c r="G37" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H37" s="5" t="n">
-        <v>77.34223862634666</v>
+        <v>59.57075461188062</v>
       </c>
       <c r="I37" s="5" t="n">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="J37" s="6" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38">
@@ -3538,31 +3538,31 @@
         </is>
       </c>
       <c r="B38" s="8" t="n">
-        <v>2438.85009765625</v>
+        <v>2453.300048828125</v>
       </c>
       <c r="C38" s="8" t="n">
-        <v>-1.444677870733924</v>
+        <v>0.09179739112532559</v>
       </c>
       <c r="D38" s="8" t="n">
-        <v>2475.305007324219</v>
+        <v>2473.843256835938</v>
       </c>
       <c r="E38" s="8" t="n">
-        <v>-1.472744149108973</v>
+        <v>-0.8304167190482193</v>
       </c>
       <c r="F38" s="8" t="n">
-        <v>2548.706000976562</v>
+        <v>2543.328002929688</v>
       </c>
       <c r="G38" s="8" t="n">
         <v>0</v>
       </c>
       <c r="H38" s="8" t="n">
-        <v>42.20490372005197</v>
+        <v>45.48869274494449</v>
       </c>
       <c r="I38" s="8" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J38" s="9" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3657,28 +3657,28 @@
         </is>
       </c>
       <c r="B2" s="5" t="n">
-        <v>50.86999893188477</v>
+        <v>52.13999938964844</v>
       </c>
       <c r="C2" s="5" t="n">
-        <v>-3.728238484129986</v>
+        <v>1.08568735694885</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>41.86109992980957</v>
+        <v>41.99289995193482</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>21.52093236245782</v>
+        <v>24.16384543417582</v>
       </c>
       <c r="F2" s="5" t="n">
-        <v>47.10440010070801</v>
+        <v>47.40960006713867</v>
       </c>
       <c r="G2" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="5" t="n">
-        <v>62.81478662515356</v>
+        <v>68.38651233236614</v>
       </c>
       <c r="I2" s="5" t="n">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="J2" s="6" t="n">
         <v>49</v>
@@ -3691,31 +3691,31 @@
         </is>
       </c>
       <c r="B3" s="5" t="n">
-        <v>51.43999862670898</v>
+        <v>51.2400016784668</v>
       </c>
       <c r="C3" s="5" t="n">
-        <v>-0.3487026518797509</v>
+        <v>-0.03901022965505652</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>50.92355003356933</v>
+        <v>50.97270002365112</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>1.014164552155538</v>
+        <v>0.5244016006443614</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>51.7683999633789</v>
+        <v>51.76779991149903</v>
       </c>
       <c r="G3" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H3" s="5" t="n">
-        <v>40.81777233500616</v>
+        <v>36.06937521766776</v>
       </c>
       <c r="I3" s="5" t="n">
         <v>1</v>
       </c>
       <c r="J3" s="6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -3725,31 +3725,31 @@
         </is>
       </c>
       <c r="B4" s="5" t="n">
-        <v>50.2400016784668</v>
+        <v>49.9900016784668</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>-0.2382822288133579</v>
+        <v>-0.1996375999530287</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>49.24334993362427</v>
+        <v>49.3095499420166</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>2.023931650031792</v>
+        <v>1.379959332929102</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>50.3821997833252</v>
+        <v>50.3597998046875</v>
       </c>
       <c r="G4" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H4" s="5" t="n">
-        <v>45.39499483101815</v>
+        <v>39.79465508529761</v>
       </c>
       <c r="I4" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="J4" s="6" t="n">
         <v>6</v>
-      </c>
-      <c r="J4" s="6" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -3759,28 +3759,28 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>269.0199890136719</v>
+        <v>269.3299865722656</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>-0.1262237735300098</v>
+        <v>0.3651874218225215</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>283.5652996826172</v>
+        <v>283.7542496490478</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>-5.129439563030201</v>
+        <v>-5.0833645996923</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>275.2933990478516</v>
+        <v>274.9625994873047</v>
       </c>
       <c r="G5" s="5" t="n">
         <v>1</v>
       </c>
       <c r="H5" s="5" t="n">
-        <v>43.57577194421625</v>
+        <v>44.95479787157078</v>
       </c>
       <c r="I5" s="5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J5" s="6" t="n">
         <v>1</v>
@@ -3793,31 +3793,31 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>14.5600004196167</v>
+        <v>14.53999996185303</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>-1.421801162075043</v>
+        <v>-0.4109617674589394</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>14.57535000801087</v>
+        <v>14.59530001163483</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>-0.1053119711412041</v>
+        <v>-0.3788894352134996</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>14.82040002822876</v>
+        <v>14.83380002975464</v>
       </c>
       <c r="G6" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H6" s="5" t="n">
-        <v>42.5012524493041</v>
+        <v>42.25048247858744</v>
       </c>
       <c r="I6" s="5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J6" s="6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -3827,31 +3827,31 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>53.22999954223633</v>
+        <v>53.7599983215332</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>-0.1875160048468771</v>
+        <v>0.392155158663976</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>53.31490003585815</v>
+        <v>53.32190002441406</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>-0.1592434639560833</v>
+        <v>0.8216104394602434</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>53.56480033874512</v>
+        <v>53.55660026550293</v>
       </c>
       <c r="G7" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>47.68402680269586</v>
+        <v>55.65239158334667</v>
       </c>
       <c r="I7" s="5" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="J7" s="6" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" hidden="1">
@@ -3861,31 +3861,31 @@
         </is>
       </c>
       <c r="B8" s="5" t="n">
-        <v>124.129997253418</v>
+        <v>123.879997253418</v>
       </c>
       <c r="C8" s="5" t="n">
-        <v>0.242263924676811</v>
+        <v>0.4703926904338296</v>
       </c>
       <c r="D8" s="5" t="n">
-        <v>109.5778790283203</v>
+        <v>109.7919190597534</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>13.28016051609894</v>
+        <v>12.8316166748094</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>122.8739999389648</v>
+        <v>122.9902000427246</v>
       </c>
       <c r="G8" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>56.4437594933483</v>
+        <v>54.69947450178652</v>
       </c>
       <c r="I8" s="5" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J8" s="6" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" hidden="1">
@@ -3895,28 +3895,28 @@
         </is>
       </c>
       <c r="B9" s="5" t="n">
-        <v>218.1900024414062</v>
+        <v>219.5200042724609</v>
       </c>
       <c r="C9" s="5" t="n">
-        <v>-0.287910091273802</v>
+        <v>0.228289649459601</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>200.7654002380371</v>
+        <v>200.9261502838135</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>8.679086228358921</v>
+        <v>9.254073679500225</v>
       </c>
       <c r="F9" s="5" t="n">
-        <v>213.2434008789062</v>
+        <v>213.5860012817383</v>
       </c>
       <c r="G9" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H9" s="5" t="n">
-        <v>69.60349263911688</v>
+        <v>72.8808700856095</v>
       </c>
       <c r="I9" s="5" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J9" s="6" t="n">
         <v>14</v>
@@ -3929,31 +3929,31 @@
         </is>
       </c>
       <c r="B10" s="5" t="n">
-        <v>15.60000038146973</v>
+        <v>15.59000015258789</v>
       </c>
       <c r="C10" s="5" t="n">
-        <v>0.4507446857833441</v>
+        <v>0.192800335232457</v>
       </c>
       <c r="D10" s="5" t="n">
-        <v>14.04794999599457</v>
+        <v>14.06789999961853</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>11.04823398373206</v>
+        <v>10.81966855757173</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>15.26900001525879</v>
+        <v>15.26200002670288</v>
       </c>
       <c r="G10" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H10" s="5" t="n">
-        <v>63.00722192859121</v>
+        <v>61.92270166370393</v>
       </c>
       <c r="I10" s="5" t="n">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="J10" s="6" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" hidden="1">
@@ -3963,28 +3963,28 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>165.1499938964844</v>
+        <v>165.3899993896484</v>
       </c>
       <c r="C11" s="5" t="n">
-        <v>0.04239887609240878</v>
+        <v>0.1513867027516103</v>
       </c>
       <c r="D11" s="5" t="n">
-        <v>148.9794498443603</v>
+        <v>149.1862998199463</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>10.85421114725386</v>
+        <v>10.86138579028937</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>161.4267999267578</v>
+        <v>161.7133999633789</v>
       </c>
       <c r="G11" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H11" s="5" t="n">
-        <v>70.19477817929319</v>
+        <v>71.14954703749706</v>
       </c>
       <c r="I11" s="5" t="n">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="J11" s="6" t="n">
         <v>25</v>
@@ -3997,28 +3997,28 @@
         </is>
       </c>
       <c r="B12" s="5" t="n">
-        <v>22.97999954223633</v>
+        <v>23.20999908447266</v>
       </c>
       <c r="C12" s="5" t="n">
-        <v>-2.461799392417152</v>
+        <v>0.7378392456171445</v>
       </c>
       <c r="D12" s="5" t="n">
-        <v>20.2271999835968</v>
+        <v>20.25599998474121</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>13.60939507629283</v>
+        <v>14.58332889986514</v>
       </c>
       <c r="F12" s="5" t="n">
-        <v>22.19059989929199</v>
+        <v>22.25299991607666</v>
       </c>
       <c r="G12" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H12" s="5" t="n">
-        <v>60.00504179778186</v>
+        <v>64.06753381379005</v>
       </c>
       <c r="I12" s="5" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J12" s="6" t="n">
         <v>35</v>
@@ -4031,31 +4031,31 @@
         </is>
       </c>
       <c r="B13" s="5" t="n">
-        <v>45.72999954223633</v>
+        <v>46.08000183105469</v>
       </c>
       <c r="C13" s="5" t="n">
-        <v>-2.119010386558162</v>
+        <v>1.386140940681679</v>
       </c>
       <c r="D13" s="5" t="n">
-        <v>39.9989500617981</v>
+        <v>40.04990007400513</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>14.32799978895396</v>
+        <v>15.05647141667519</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>43.85580001831055</v>
+        <v>43.98480010986328</v>
       </c>
       <c r="G13" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>61.08830243944911</v>
+        <v>62.76382012345815</v>
       </c>
       <c r="I13" s="5" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J13" s="6" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" hidden="1">
@@ -4065,28 +4065,28 @@
         </is>
       </c>
       <c r="B14" s="5" t="n">
-        <v>16.65999984741211</v>
+        <v>16.70999908447266</v>
       </c>
       <c r="C14" s="5" t="n">
-        <v>-0.4184082291664004</v>
+        <v>1.272721724076709</v>
       </c>
       <c r="D14" s="5" t="n">
-        <v>14.97239996910095</v>
+        <v>14.99219996452332</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>11.27140526431243</v>
+        <v>11.4579522952885</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>16.13519992828369</v>
+        <v>16.16339990615845</v>
       </c>
       <c r="G14" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>70.20729371129866</v>
+        <v>66.97495627020794</v>
       </c>
       <c r="I14" s="5" t="n">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="J14" s="6" t="n">
         <v>27</v>
@@ -4099,28 +4099,28 @@
         </is>
       </c>
       <c r="B15" s="5" t="n">
-        <v>219.0899963378906</v>
+        <v>220.3099975585938</v>
       </c>
       <c r="C15" s="5" t="n">
-        <v>0.009124486695388789</v>
+        <v>0.09540729180141927</v>
       </c>
       <c r="D15" s="5" t="n">
-        <v>200.9331999206543</v>
+        <v>201.1250499725342</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>9.036235139044321</v>
+        <v>9.538815572043104</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>214.0269995117187</v>
+        <v>214.3655996704101</v>
       </c>
       <c r="G15" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>73.31976448771834</v>
+        <v>76.19705131465869</v>
       </c>
       <c r="I15" s="5" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J15" s="6" t="n">
         <v>17</v>
@@ -4133,31 +4133,31 @@
         </is>
       </c>
       <c r="B16" s="5" t="n">
-        <v>208.2599945068359</v>
+        <v>209.3600006103516</v>
       </c>
       <c r="C16" s="5" t="n">
-        <v>0.00959902667334589</v>
+        <v>0.05256898941532473</v>
       </c>
       <c r="D16" s="5" t="n">
-        <v>191.0540502929688</v>
+        <v>191.2304002380371</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>9.005799242404443</v>
+        <v>9.480501191101073</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>203.4386004638672</v>
+        <v>203.7596005249023</v>
       </c>
       <c r="G16" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>73.36263976327271</v>
+        <v>76.07857218761765</v>
       </c>
       <c r="I16" s="5" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J16" s="6" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" hidden="1">
@@ -4167,31 +4167,31 @@
         </is>
       </c>
       <c r="B17" s="5" t="n">
-        <v>220.1900024414062</v>
+        <v>221.5299987792969</v>
       </c>
       <c r="C17" s="5" t="n">
-        <v>-0.08621582593543176</v>
+        <v>0.04516375686380858</v>
       </c>
       <c r="D17" s="5" t="n">
-        <v>202.0936995697022</v>
+        <v>202.2881494903564</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>8.954412191094892</v>
+        <v>9.512099120694042</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>215.2739993286133</v>
+        <v>215.6135992431641</v>
       </c>
       <c r="G17" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>72.16364712517912</v>
+        <v>75.32918376700046</v>
       </c>
       <c r="I17" s="5" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J17" s="6" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" hidden="1">
@@ -4201,21 +4201,31 @@
         </is>
       </c>
       <c r="B18" s="5" t="n">
-        <v>236.9499969482422</v>
-      </c>
-      <c r="C18" s="5" t="n"/>
-      <c r="D18" s="5" t="n"/>
-      <c r="E18" s="5" t="n"/>
-      <c r="F18" s="5" t="n"/>
+        <v>243.4100036621094</v>
+      </c>
+      <c r="C18" s="5" t="n">
+        <v/>
+      </c>
+      <c r="D18" s="5" t="n">
+        <v/>
+      </c>
+      <c r="E18" s="5" t="n">
+        <v/>
+      </c>
+      <c r="F18" s="5" t="n">
+        <v/>
+      </c>
       <c r="G18" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H18" s="5" t="n"/>
+      <c r="H18" s="5" t="n">
+        <v/>
+      </c>
       <c r="I18" s="5" t="n">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="J18" s="6" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" hidden="1">
@@ -4225,31 +4235,31 @@
         </is>
       </c>
       <c r="B19" s="5" t="n">
-        <v>34.29999923706055</v>
+        <v>34.81999969482422</v>
       </c>
       <c r="C19" s="5" t="n">
-        <v>-3.894646800597568</v>
+        <v>1.162119544328744</v>
       </c>
       <c r="D19" s="5" t="n">
-        <v>28.67755000114441</v>
+        <v>28.72789999961853</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>19.6057516618113</v>
+        <v>21.20621310742026</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>32.5669998550415</v>
+        <v>32.7217998123169</v>
       </c>
       <c r="G19" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H19" s="5" t="n">
-        <v>59.5918961217582</v>
+        <v>64.16636608314603</v>
       </c>
       <c r="I19" s="5" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="J19" s="6" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" hidden="1">
@@ -4259,31 +4269,31 @@
         </is>
       </c>
       <c r="B20" s="5" t="n">
-        <v>202.5</v>
+        <v>203.3000030517578</v>
       </c>
       <c r="C20" s="5" t="n">
-        <v>-0.5011813340448867</v>
+        <v>0.1872683255674579</v>
       </c>
       <c r="D20" s="5" t="n">
-        <v>182.7171007537842</v>
+        <v>182.9777008056641</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>10.82706498986856</v>
+        <v>11.10643655298607</v>
       </c>
       <c r="F20" s="5" t="n">
-        <v>198.9134008789063</v>
+        <v>199.2066009521484</v>
       </c>
       <c r="G20" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H20" s="5" t="n">
-        <v>63.59288613847825</v>
+        <v>66.05012495866339</v>
       </c>
       <c r="I20" s="5" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J20" s="6" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" hidden="1">
@@ -4293,31 +4303,31 @@
         </is>
       </c>
       <c r="B21" s="5" t="n">
-        <v>163.3600006103516</v>
+        <v>164.3399963378906</v>
       </c>
       <c r="C21" s="5" t="n">
-        <v>-1.874096105993228</v>
+        <v>0.9149463792023971</v>
       </c>
       <c r="D21" s="5" t="n">
-        <v>138.0492498397827</v>
+        <v>138.343099861145</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>18.33458044860369</v>
+        <v>18.79161049798558</v>
       </c>
       <c r="F21" s="5" t="n">
-        <v>156.1104000854492</v>
+        <v>156.7233999633789</v>
       </c>
       <c r="G21" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H21" s="5" t="n">
-        <v>64.49157717876878</v>
+        <v>65.98258205674995</v>
       </c>
       <c r="I21" s="5" t="n">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="J21" s="6" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" hidden="1">
@@ -4327,31 +4337,31 @@
         </is>
       </c>
       <c r="B22" s="5" t="n">
-        <v>463.8599853515625</v>
+        <v>468.5700073242188</v>
       </c>
       <c r="C22" s="5" t="n">
-        <v>-0.05386654196001261</v>
+        <v>0.2267325910572771</v>
       </c>
       <c r="D22" s="5" t="n">
-        <v>436.1437498474121</v>
+        <v>436.4725498962403</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>6.35483954862293</v>
+        <v>7.353831858523248</v>
       </c>
       <c r="F22" s="5" t="n">
-        <v>457.2451995849609</v>
+        <v>457.5223999023438</v>
       </c>
       <c r="G22" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H22" s="5" t="n">
-        <v>65.89269584015895</v>
+        <v>71.15325751039649</v>
       </c>
       <c r="I22" s="5" t="n">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="J22" s="6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" hidden="1">
@@ -4361,31 +4371,31 @@
         </is>
       </c>
       <c r="B23" s="5" t="n">
-        <v>459.75</v>
+        <v>465.6799926757812</v>
       </c>
       <c r="C23" s="5" t="n">
-        <v>-0.08692685032923864</v>
+        <v>0.3707218838651993</v>
       </c>
       <c r="D23" s="5" t="n">
-        <v>432.6044999694824</v>
+        <v>432.9366497802735</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>6.274900060547798</v>
+        <v>7.563079474127655</v>
       </c>
       <c r="F23" s="5" t="n">
-        <v>453.4222009277344</v>
+        <v>453.7424005126953</v>
       </c>
       <c r="G23" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H23" s="5" t="n">
-        <v>65.60238910188117</v>
+        <v>72.16029555650377</v>
       </c>
       <c r="I23" s="5" t="n">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="J23" s="6" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" hidden="1">
@@ -4395,28 +4405,28 @@
         </is>
       </c>
       <c r="B24" s="5" t="n">
-        <v>45.95000076293945</v>
+        <v>46.47000122070312</v>
       </c>
       <c r="C24" s="5" t="n">
-        <v>-0.02175439889550157</v>
+        <v>0.3238374932365673</v>
       </c>
       <c r="D24" s="5" t="n">
-        <v>42.95289999008179</v>
+        <v>43.00439998626709</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>6.977644754020616</v>
+        <v>8.058713144568305</v>
       </c>
       <c r="F24" s="5" t="n">
-        <v>44.93880004882813</v>
+        <v>45.03200012207031</v>
       </c>
       <c r="G24" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H24" s="5" t="n">
-        <v>66.39388640805581</v>
+        <v>71.85227256399563</v>
       </c>
       <c r="I24" s="5" t="n">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="J24" s="6" t="n">
         <v>11</v>
@@ -4435,13 +4445,13 @@
         <v>0</v>
       </c>
       <c r="D25" s="5" t="n">
-        <v>19.2981500339508</v>
+        <v>19.30095004081726</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>3.32596906427621</v>
+        <v>3.310979469346881</v>
       </c>
       <c r="F25" s="5" t="n">
-        <v>20.27160015106201</v>
+        <v>20.25660015106201</v>
       </c>
       <c r="G25" s="5" t="n">
         <v>0</v>
@@ -4450,7 +4460,7 @@
         <v>42.34592928411659</v>
       </c>
       <c r="I25" s="5" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J25" s="6" t="n">
         <v>7</v>
@@ -4463,31 +4473,31 @@
         </is>
       </c>
       <c r="B26" s="5" t="n">
-        <v>537.3099975585938</v>
+        <v>537.8400268554688</v>
       </c>
       <c r="C26" s="5" t="n">
-        <v>-0.04836761018703895</v>
+        <v>0.1284561872930912</v>
       </c>
       <c r="D26" s="5" t="n">
-        <v>494.9718016052246</v>
+        <v>495.8315518188476</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>8.553658171246067</v>
+        <v>8.472327927200757</v>
       </c>
       <c r="F26" s="5" t="n">
-        <v>539.747802734375</v>
+        <v>539.3072033691407</v>
       </c>
       <c r="G26" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H26" s="5" t="n">
-        <v>54.09588490416495</v>
+        <v>54.86353968388604</v>
       </c>
       <c r="I26" s="5" t="n">
         <v>9</v>
       </c>
       <c r="J26" s="6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" hidden="1">
@@ -4497,31 +4507,31 @@
         </is>
       </c>
       <c r="B27" s="5" t="n">
-        <v>98.5</v>
+        <v>98.80999755859375</v>
       </c>
       <c r="C27" s="5" t="n">
-        <v>0.1627045638273206</v>
+        <v>0.202816090664526</v>
       </c>
       <c r="D27" s="5" t="n">
-        <v>84.4305498123169</v>
+        <v>84.58464977264404</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>16.66393292351938</v>
+        <v>16.81788341523689</v>
       </c>
       <c r="F27" s="5" t="n">
-        <v>95.46759979248047</v>
+        <v>95.82439971923829</v>
       </c>
       <c r="G27" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H27" s="5" t="n">
-        <v>62.57528204590086</v>
+        <v>64.23674330983349</v>
       </c>
       <c r="I27" s="5" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J27" s="6" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" hidden="1">
@@ -4531,28 +4541,28 @@
         </is>
       </c>
       <c r="B28" s="5" t="n">
-        <v>9.819999694824219</v>
+        <v>9.869999885559082</v>
       </c>
       <c r="C28" s="5" t="n">
-        <v>-0.1017317289872977</v>
+        <v>0.3048753303454221</v>
       </c>
       <c r="D28" s="5" t="n">
-        <v>8.43174998998642</v>
+        <v>8.447199990749359</v>
       </c>
       <c r="E28" s="5" t="n">
-        <v>16.46455014067649</v>
+        <v>16.84344985756049</v>
       </c>
       <c r="F28" s="5" t="n">
-        <v>9.539200019836425</v>
+        <v>9.574200019836425</v>
       </c>
       <c r="G28" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H28" s="5" t="n">
-        <v>61.859562668431</v>
+        <v>64.70836077594873</v>
       </c>
       <c r="I28" s="5" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J28" s="6" t="n">
         <v>38</v>
@@ -4565,31 +4575,31 @@
         </is>
       </c>
       <c r="B29" s="5" t="n">
-        <v>93.13999938964844</v>
+        <v>93.54000091552734</v>
       </c>
       <c r="C29" s="5" t="n">
-        <v>-0.491452021337202</v>
+        <v>0.3109929389033095</v>
       </c>
       <c r="D29" s="5" t="n">
-        <v>84.56885005950927</v>
+        <v>84.63730007171631</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>10.13511396230152</v>
+        <v>10.51864938539798</v>
       </c>
       <c r="F29" s="5" t="n">
-        <v>91.12140014648438</v>
+        <v>91.27660018920898</v>
       </c>
       <c r="G29" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H29" s="5" t="n">
-        <v>66.97756540650994</v>
+        <v>69.73185336827612</v>
       </c>
       <c r="I29" s="5" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J29" s="6" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" hidden="1">
@@ -4599,28 +4609,28 @@
         </is>
       </c>
       <c r="B30" s="5" t="n">
-        <v>66.95999908447266</v>
+        <v>67.33999633789062</v>
       </c>
       <c r="C30" s="5" t="n">
-        <v>-0.8587530695773893</v>
+        <v>0.7179116409770758</v>
       </c>
       <c r="D30" s="5" t="n">
-        <v>57.4692000579834</v>
+        <v>57.56480005264282</v>
       </c>
       <c r="E30" s="5" t="n">
-        <v>16.51458349326863</v>
+        <v>16.98120427120118</v>
       </c>
       <c r="F30" s="5" t="n">
-        <v>63.0673999786377</v>
+        <v>63.32759994506836</v>
       </c>
       <c r="G30" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H30" s="5" t="n">
-        <v>72.29593808417265</v>
+        <v>73.47293458833873</v>
       </c>
       <c r="I30" s="5" t="n">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J30" s="6" t="n">
         <v>39</v>
@@ -4639,13 +4649,13 @@
         <v>0</v>
       </c>
       <c r="D31" s="5" t="n">
-        <v>87.50035007476806</v>
+        <v>87.5713000869751</v>
       </c>
       <c r="E31" s="5" t="n">
-        <v>12.4452637110312</v>
+        <v>12.35416088596183</v>
       </c>
       <c r="F31" s="5" t="n">
-        <v>96.61120010375977</v>
+        <v>96.72620010375977</v>
       </c>
       <c r="G31" s="5" t="n">
         <v>0</v>
@@ -4654,10 +4664,10 @@
         <v>67.83070521020178</v>
       </c>
       <c r="I31" s="5" t="n">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="J31" s="6" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" hidden="1">
@@ -4667,31 +4677,31 @@
         </is>
       </c>
       <c r="B32" s="5" t="n">
-        <v>34.22999954223633</v>
+        <v>34.29000091552734</v>
       </c>
       <c r="C32" s="5" t="n">
-        <v>0.6764692418715468</v>
+        <v>0.02917776133792849</v>
       </c>
       <c r="D32" s="5" t="n">
-        <v>30.60350004196167</v>
+        <v>30.63380003929138</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>11.84995015374784</v>
+        <v>11.93518555173195</v>
       </c>
       <c r="F32" s="5" t="n">
-        <v>32.05540004730224</v>
+        <v>32.18840003967285</v>
       </c>
       <c r="G32" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H32" s="5" t="n">
-        <v>80.77974827989659</v>
+        <v>81.26150867117445</v>
       </c>
       <c r="I32" s="5" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J32" s="6" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" hidden="1">
@@ -4701,31 +4711,31 @@
         </is>
       </c>
       <c r="B33" s="5" t="n">
-        <v>34.54000091552734</v>
+        <v>34.66999816894531</v>
       </c>
       <c r="C33" s="5" t="n">
-        <v>0.8467180015396814</v>
+        <v>0.4054427877141276</v>
       </c>
       <c r="D33" s="5" t="n">
-        <v>30.74835004806518</v>
+        <v>30.78040002822876</v>
       </c>
       <c r="E33" s="5" t="n">
-        <v>12.33123358337969</v>
+        <v>12.63660685744629</v>
       </c>
       <c r="F33" s="5" t="n">
-        <v>32.23000003814698</v>
+        <v>32.36759998321534</v>
       </c>
       <c r="G33" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H33" s="5" t="n">
-        <v>79.38897265362388</v>
+        <v>80.2093797295253</v>
       </c>
       <c r="I33" s="5" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J33" s="6" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" hidden="1">
@@ -4735,28 +4745,28 @@
         </is>
       </c>
       <c r="B34" s="5" t="n">
-        <v>34.68000030517578</v>
+        <v>34.72000122070312</v>
       </c>
       <c r="C34" s="5" t="n">
-        <v>1.166865636297754</v>
+        <v>0.3468287626422484</v>
       </c>
       <c r="D34" s="5" t="n">
-        <v>30.76385004043579</v>
+        <v>30.80950004577637</v>
       </c>
       <c r="E34" s="5" t="n">
-        <v>12.72971445249092</v>
+        <v>12.69251746739345</v>
       </c>
       <c r="F34" s="5" t="n">
-        <v>32.00599990844727</v>
+        <v>32.18739990234375</v>
       </c>
       <c r="G34" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H34" s="5" t="n">
-        <v>79.94937456359216</v>
+        <v>78.69531897069865</v>
       </c>
       <c r="I34" s="5" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J34" s="6" t="n">
         <v>32</v>
@@ -4769,28 +4779,28 @@
         </is>
       </c>
       <c r="B35" s="5" t="n">
-        <v>42.75</v>
+        <v>43.22000122070312</v>
       </c>
       <c r="C35" s="5" t="n">
-        <v>-2.907106097624368</v>
+        <v>0.910575234590949</v>
       </c>
       <c r="D35" s="5" t="n">
-        <v>35.38040000915527</v>
+        <v>35.47765003204346</v>
       </c>
       <c r="E35" s="5" t="n">
-        <v>20.829611844235</v>
+        <v>21.82317933027348</v>
       </c>
       <c r="F35" s="5" t="n">
-        <v>40.27800010681153</v>
+        <v>40.47600021362305</v>
       </c>
       <c r="G35" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H35" s="5" t="n">
-        <v>63.58221539515217</v>
+        <v>67.3455174950487</v>
       </c>
       <c r="I35" s="5" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J35" s="6" t="n">
         <v>47</v>
@@ -4803,31 +4813,31 @@
         </is>
       </c>
       <c r="B36" s="5" t="n">
-        <v>153.7200012207031</v>
+        <v>155.3099975585938</v>
       </c>
       <c r="C36" s="5" t="n">
-        <v>-2.838003478050866</v>
+        <v>0.9227358337625891</v>
       </c>
       <c r="D36" s="5" t="n">
-        <v>127.9649001312256</v>
+        <v>128.3001000976562</v>
       </c>
       <c r="E36" s="5" t="n">
-        <v>20.12669182179345</v>
+        <v>21.05212501033031</v>
       </c>
       <c r="F36" s="5" t="n">
-        <v>144.9462002563477</v>
+        <v>145.6436001586914</v>
       </c>
       <c r="G36" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H36" s="5" t="n">
-        <v>64.08794453878212</v>
+        <v>67.82267528169206</v>
       </c>
       <c r="I36" s="5" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J36" s="6" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" hidden="1">
@@ -4837,28 +4847,28 @@
         </is>
       </c>
       <c r="B37" s="5" t="n">
-        <v>153.8899993896484</v>
+        <v>155.7400054931641</v>
       </c>
       <c r="C37" s="5" t="n">
-        <v>-3.012541018754744</v>
+        <v>0.8156459091618107</v>
       </c>
       <c r="D37" s="5" t="n">
-        <v>126.8751497268677</v>
+        <v>127.2045497131348</v>
       </c>
       <c r="E37" s="5" t="n">
-        <v>21.29246721752634</v>
+        <v>22.43273204015187</v>
       </c>
       <c r="F37" s="5" t="n">
-        <v>143.859599609375</v>
+        <v>144.7119998168945</v>
       </c>
       <c r="G37" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H37" s="5" t="n">
-        <v>64.72322725382713</v>
+        <v>68.76644379739099</v>
       </c>
       <c r="I37" s="5" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J37" s="6" t="n">
         <v>48</v>
@@ -4877,25 +4887,25 @@
         <v>0</v>
       </c>
       <c r="D38" s="5" t="n">
-        <v>12.59039999485016</v>
+        <v>12.60504999160767</v>
       </c>
       <c r="E38" s="5" t="n">
-        <v>17.70872808557338</v>
+        <v>17.5719231949992</v>
       </c>
       <c r="F38" s="5" t="n">
-        <v>14.22359996795654</v>
+        <v>14.25079996109009</v>
       </c>
       <c r="G38" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H38" s="5" t="n">
-        <v>78.78026856837572</v>
+        <v>78.7802685683757</v>
       </c>
       <c r="I38" s="5" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J38" s="6" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" hidden="1">
@@ -4905,10 +4915,10 @@
         </is>
       </c>
       <c r="B39" s="5" t="n">
-        <v>193.5599975585938</v>
+        <v>194.6699981689453</v>
       </c>
       <c r="C39" s="5" t="n">
-        <v>-2.064360374243346</v>
+        <v>-1.652017900438751</v>
       </c>
       <c r="D39" s="5" t="n">
         <v/>
@@ -4917,19 +4927,19 @@
         <v/>
       </c>
       <c r="F39" s="5" t="n">
-        <v>183.1405993652344</v>
+        <v>184.0725991821289</v>
       </c>
       <c r="G39" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H39" s="5" t="n">
-        <v>63.63726910367807</v>
+        <v>60.99322380240922</v>
       </c>
       <c r="I39" s="5" t="n">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="J39" s="6" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" hidden="1">
@@ -4939,28 +4949,28 @@
         </is>
       </c>
       <c r="B40" s="5" t="n">
-        <v>48.15999984741211</v>
+        <v>48.58000183105469</v>
       </c>
       <c r="C40" s="5" t="n">
-        <v>-1.89448014317587</v>
+        <v>0.9769303985458722</v>
       </c>
       <c r="D40" s="5" t="n">
-        <v>43.97454996109009</v>
+        <v>44.00794998168945</v>
       </c>
       <c r="E40" s="5" t="n">
-        <v>9.517891348576441</v>
+        <v>10.38914980422298</v>
       </c>
       <c r="F40" s="5" t="n">
-        <v>47.05000015258789</v>
+        <v>47.13500022888184</v>
       </c>
       <c r="G40" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H40" s="5" t="n">
-        <v>59.88546309259989</v>
+        <v>63.79195186737026</v>
       </c>
       <c r="I40" s="5" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J40" s="6" t="n">
         <v>18</v>
@@ -4973,28 +4983,28 @@
         </is>
       </c>
       <c r="B41" s="5" t="n">
-        <v>47.11999893188477</v>
+        <v>47.4900016784668</v>
       </c>
       <c r="C41" s="5" t="n">
-        <v>-2.057787707144165</v>
+        <v>0.6997494319813891</v>
       </c>
       <c r="D41" s="5" t="n">
-        <v>42.97699996948242</v>
+        <v>43.00904996871948</v>
       </c>
       <c r="E41" s="5" t="n">
-        <v>9.640037613942926</v>
+        <v>10.418625180064</v>
       </c>
       <c r="F41" s="5" t="n">
-        <v>46.0639998626709</v>
+        <v>46.14299987792969</v>
       </c>
       <c r="G41" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H41" s="5" t="n">
-        <v>58.51073273134337</v>
+        <v>62.19185242664833</v>
       </c>
       <c r="I41" s="5" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J41" s="6" t="n">
         <v>19</v>
@@ -5007,31 +5017,31 @@
         </is>
       </c>
       <c r="B42" s="5" t="n">
-        <v>483.6600036621094</v>
+        <v>488.510009765625</v>
       </c>
       <c r="C42" s="5" t="n">
-        <v>-2.136699755677829</v>
+        <v>0.6572987705563804</v>
       </c>
       <c r="D42" s="5" t="n">
-        <v>440.8230992126465</v>
+        <v>441.1625993347168</v>
       </c>
       <c r="E42" s="5" t="n">
-        <v>9.717481803012102</v>
+        <v>10.73241714105166</v>
       </c>
       <c r="F42" s="5" t="n">
-        <v>472.8767993164063</v>
+        <v>473.7187994384765</v>
       </c>
       <c r="G42" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H42" s="5" t="n">
-        <v>58.0028551022317</v>
+        <v>62.51669398835828</v>
       </c>
       <c r="I42" s="5" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J42" s="6" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" hidden="1">
@@ -5041,28 +5051,28 @@
         </is>
       </c>
       <c r="B43" s="5" t="n">
-        <v>15.5600004196167</v>
+        <v>15.72999954223633</v>
       </c>
       <c r="C43" s="5" t="n">
-        <v>0.1931789257008987</v>
+        <v>0.1910811040487292</v>
       </c>
       <c r="D43" s="5" t="n">
-        <v>13.17944999694824</v>
+        <v>13.20004999637604</v>
       </c>
       <c r="E43" s="5" t="n">
-        <v>18.06259307649168</v>
+        <v>19.16621184431019</v>
       </c>
       <c r="F43" s="5" t="n">
-        <v>14.79560001373291</v>
+        <v>14.89559999465942</v>
       </c>
       <c r="G43" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H43" s="5" t="n">
-        <v>62.30922504453024</v>
+        <v>67.32553551401077</v>
       </c>
       <c r="I43" s="5" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="J43" s="6" t="n">
         <v>43</v>
@@ -5075,31 +5085,31 @@
         </is>
       </c>
       <c r="B44" s="5" t="n">
-        <v>235.0299987792969</v>
+        <v>237.5299987792969</v>
       </c>
       <c r="C44" s="5" t="n">
-        <v>-0.3307742620637044</v>
+        <v>0.4950068395346285</v>
       </c>
       <c r="D44" s="5" t="n">
-        <v>218.0058499145508</v>
+        <v>218.2100498962402</v>
       </c>
       <c r="E44" s="5" t="n">
-        <v>7.809033047241089</v>
+        <v>8.853830926780574</v>
       </c>
       <c r="F44" s="5" t="n">
-        <v>230.5819998168945</v>
+        <v>230.8891998291016</v>
       </c>
       <c r="G44" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H44" s="5" t="n">
-        <v>63.75040401314051</v>
+        <v>69.30413231016833</v>
       </c>
       <c r="I44" s="5" t="n">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J44" s="6" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" hidden="1">
@@ -5109,31 +5119,31 @@
         </is>
       </c>
       <c r="B45" s="5" t="n">
-        <v>465.3299865722656</v>
+        <v>499.2200012207031</v>
       </c>
       <c r="C45" s="5" t="n">
-        <v>-3.777919623793236</v>
+        <v>1.740443603243613</v>
       </c>
       <c r="D45" s="5" t="n">
-        <v>411.4979006958008</v>
+        <v>412.4296507263184</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>13.08198311229298</v>
+        <v>21.04367383420195</v>
       </c>
       <c r="F45" s="5" t="n">
-        <v>452.2630017089843</v>
+        <v>454.7182019042968</v>
       </c>
       <c r="G45" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H45" s="5" t="n">
-        <v>54.93039620892432</v>
+        <v>68.68529380269804</v>
       </c>
       <c r="I45" s="5" t="n">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="J45" s="6" t="n">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" hidden="1">
@@ -5143,10 +5153,10 @@
         </is>
       </c>
       <c r="B46" s="5" t="n">
-        <v>120.4700012207031</v>
+        <v>122.879997253418</v>
       </c>
       <c r="C46" s="5" t="n">
-        <v>-3.361144166787644</v>
+        <v>1.027707003392919</v>
       </c>
       <c r="D46" s="5" t="n">
         <v/>
@@ -5155,19 +5165,19 @@
         <v/>
       </c>
       <c r="F46" s="5" t="n">
-        <v>114.3030001831055</v>
+        <v>114.9191999816895</v>
       </c>
       <c r="G46" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H46" s="5" t="n">
-        <v>59.57019743913033</v>
+        <v>66.61557146608445</v>
       </c>
       <c r="I46" s="5" t="n">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="J46" s="6" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47">
@@ -5183,13 +5193,13 @@
         <v>0</v>
       </c>
       <c r="D47" s="5" t="n">
-        <v>30.03185002326966</v>
+        <v>30.036100025177</v>
       </c>
       <c r="E47" s="5" t="n">
-        <v>4.888643142506288</v>
+        <v>4.873801770522538</v>
       </c>
       <c r="F47" s="5" t="n">
-        <v>31.45800003051758</v>
+        <v>31.46440002441406</v>
       </c>
       <c r="G47" s="5" t="n">
         <v>0</v>
@@ -5198,7 +5208,7 @@
         <v>52.1854555994307</v>
       </c>
       <c r="I47" s="5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J47" s="6" t="n">
         <v>8</v>
@@ -5211,31 +5221,31 @@
         </is>
       </c>
       <c r="B48" s="5" t="n">
-        <v>117.2200012207031</v>
+        <v>117.870002746582</v>
       </c>
       <c r="C48" s="5" t="n">
-        <v>0.2137300140129916</v>
+        <v>0.2636995529314845</v>
       </c>
       <c r="D48" s="5" t="n">
-        <v>106.4151002120972</v>
+        <v>106.5627502059937</v>
       </c>
       <c r="E48" s="5" t="n">
-        <v>10.15354116762619</v>
+        <v>10.61088656095176</v>
       </c>
       <c r="F48" s="5" t="n">
-        <v>113.2583999633789</v>
+        <v>113.5013999938965</v>
       </c>
       <c r="G48" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H48" s="5" t="n">
-        <v>71.887236003504</v>
+        <v>74.24266694545454</v>
       </c>
       <c r="I48" s="5" t="n">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="J48" s="6" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" hidden="1">
@@ -5245,31 +5255,31 @@
         </is>
       </c>
       <c r="B49" s="5" t="n">
-        <v>114.9800033569336</v>
+        <v>115.8099975585938</v>
       </c>
       <c r="C49" s="5" t="n">
-        <v>0.05221474847230123</v>
+        <v>0.3118238370443338</v>
       </c>
       <c r="D49" s="5" t="n">
-        <v>104.4231497192383</v>
+        <v>104.5684996795654</v>
       </c>
       <c r="E49" s="5" t="n">
-        <v>10.10968704361001</v>
+        <v>10.7503673797331</v>
       </c>
       <c r="F49" s="5" t="n">
-        <v>111.001199798584</v>
+        <v>111.2393997192383</v>
       </c>
       <c r="G49" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H49" s="5" t="n">
-        <v>70.33065969955925</v>
+        <v>73.26865055250909</v>
       </c>
       <c r="I49" s="5" t="n">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="J49" s="6" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50">
@@ -5279,31 +5289,31 @@
         </is>
       </c>
       <c r="B50" s="5" t="n">
-        <v>64.51999664306641</v>
+        <v>64.37999725341797</v>
       </c>
       <c r="C50" s="5" t="n">
-        <v>0.4202282382356426</v>
+        <v>0.5937457084655762</v>
       </c>
       <c r="D50" s="5" t="n">
-        <v>51.51269989013672</v>
+        <v>51.77009986877442</v>
       </c>
       <c r="E50" s="5" t="n">
-        <v>25.25066009095018</v>
+        <v>24.35749093899145</v>
       </c>
       <c r="F50" s="5" t="n">
-        <v>63.92179969787598</v>
+        <v>63.93619956970215</v>
       </c>
       <c r="G50" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H50" s="5" t="n">
-        <v>56.72277818966567</v>
+        <v>55.15049739176025</v>
       </c>
       <c r="I50" s="5" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J50" s="6" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" hidden="1">
@@ -5313,31 +5323,31 @@
         </is>
       </c>
       <c r="B51" s="5" t="n">
-        <v>33.22000122070312</v>
+        <v>33.02000045776367</v>
       </c>
       <c r="C51" s="5" t="n">
-        <v>0.1205573091001666</v>
+        <v>-0.3320271862515267</v>
       </c>
       <c r="D51" s="5" t="n">
-        <v>29.11525007247925</v>
+        <v>29.17820008277893</v>
       </c>
       <c r="E51" s="5" t="n">
-        <v>14.09828573687516</v>
+        <v>13.16668048092585</v>
       </c>
       <c r="F51" s="5" t="n">
-        <v>32.51939998626709</v>
+        <v>32.56779998779297</v>
       </c>
       <c r="G51" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H51" s="5" t="n">
-        <v>60.62896237027272</v>
+        <v>55.84490922597161</v>
       </c>
       <c r="I51" s="5" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="J51" s="6" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" hidden="1">
@@ -5347,31 +5357,31 @@
         </is>
       </c>
       <c r="B52" s="5" t="n">
-        <v>29.34000015258789</v>
+        <v>29.51000022888184</v>
       </c>
       <c r="C52" s="5" t="n">
-        <v>-0.9787344461443692</v>
+        <v>0.30591486184397</v>
       </c>
       <c r="D52" s="5" t="n">
-        <v>26.30885004043579</v>
+        <v>26.34090003967285</v>
       </c>
       <c r="E52" s="5" t="n">
-        <v>11.5214086039235</v>
+        <v>12.0311006246404</v>
       </c>
       <c r="F52" s="5" t="n">
-        <v>28.41060005187988</v>
+        <v>28.47740005493164</v>
       </c>
       <c r="G52" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H52" s="5" t="n">
-        <v>67.4393493653851</v>
+        <v>70.21969875175114</v>
       </c>
       <c r="I52" s="5" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J52" s="6" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" hidden="1">
@@ -5381,28 +5391,28 @@
         </is>
       </c>
       <c r="B53" s="5" t="n">
-        <v>121.6100006103516</v>
+        <v>122.0400009155273</v>
       </c>
       <c r="C53" s="5" t="n">
-        <v>-2.913940175339635</v>
+        <v>0.8511683010610449</v>
       </c>
       <c r="D53" s="5" t="n">
-        <v>103.4592500686645</v>
+        <v>103.6453500747681</v>
       </c>
       <c r="E53" s="5" t="n">
-        <v>17.54386440037078</v>
+        <v>17.74768557150869</v>
       </c>
       <c r="F53" s="5" t="n">
-        <v>115.1714002990723</v>
+        <v>115.595400390625</v>
       </c>
       <c r="G53" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H53" s="5" t="n">
-        <v>63.93814718873109</v>
+        <v>64.05616642827904</v>
       </c>
       <c r="I53" s="5" t="n">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="J53" s="6" t="n">
         <v>41</v>
@@ -5415,31 +5425,31 @@
         </is>
       </c>
       <c r="B54" s="5" t="n">
-        <v>73.01000213623047</v>
+        <v>71.87000274658203</v>
       </c>
       <c r="C54" s="5" t="n">
-        <v>-0.1777375642641466</v>
+        <v>-1.128077682326678</v>
       </c>
       <c r="D54" s="5" t="n">
-        <v>70.78464979171753</v>
+        <v>70.91014982223511</v>
       </c>
       <c r="E54" s="5" t="n">
-        <v>3.143834646439586</v>
+        <v>1.353618525349583</v>
       </c>
       <c r="F54" s="5" t="n">
-        <v>73.61039978027344</v>
+        <v>73.56539993286133</v>
       </c>
       <c r="G54" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H54" s="5" t="n">
-        <v>43.39906505995343</v>
+        <v>36.68410111835272</v>
       </c>
       <c r="I54" s="5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J54" s="6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" hidden="1">
@@ -5449,16 +5459,26 @@
         </is>
       </c>
       <c r="B55" s="8" t="n">
-        <v>71.18000030517578</v>
-      </c>
-      <c r="C55" s="8" t="n"/>
-      <c r="D55" s="8" t="n"/>
-      <c r="E55" s="8" t="n"/>
-      <c r="F55" s="8" t="n"/>
+        <v>69.22000122070312</v>
+      </c>
+      <c r="C55" s="8" t="n">
+        <v/>
+      </c>
+      <c r="D55" s="8" t="n">
+        <v/>
+      </c>
+      <c r="E55" s="8" t="n">
+        <v/>
+      </c>
+      <c r="F55" s="8" t="n">
+        <v/>
+      </c>
       <c r="G55" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="H55" s="8" t="n"/>
+      <c r="H55" s="8" t="n">
+        <v/>
+      </c>
       <c r="I55" s="8" t="n">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
Commit for adding requirements.txt
</commit_message>
<xml_diff>
--- a/buy_low.xlsx
+++ b/buy_low.xlsx
@@ -3657,28 +3657,28 @@
         </is>
       </c>
       <c r="B2" s="5" t="n">
-        <v>52.13999938964844</v>
+        <v>51.58000183105469</v>
       </c>
       <c r="C2" s="5" t="n">
-        <v>1.08568735694885</v>
+        <v>1.395720295022262</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>41.99289995193482</v>
+        <v>41.92599994659424</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>24.16384543417582</v>
+        <v>23.02628892991894</v>
       </c>
       <c r="F2" s="5" t="n">
-        <v>47.40960006713867</v>
+        <v>47.25300010681153</v>
       </c>
       <c r="G2" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="5" t="n">
-        <v>68.38651233236614</v>
+        <v>66.05016344223489</v>
       </c>
       <c r="I2" s="5" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J2" s="6" t="n">
         <v>49</v>
@@ -3691,31 +3691,31 @@
         </is>
       </c>
       <c r="B3" s="5" t="n">
-        <v>51.2400016784668</v>
+        <v>51.2599983215332</v>
       </c>
       <c r="C3" s="5" t="n">
-        <v>-0.03901022965505652</v>
+        <v>-0.3499228421097178</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>50.97270002365112</v>
+        <v>50.94760002136231</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>0.5244016006443614</v>
+        <v>0.6131756943210463</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>51.76779991149903</v>
+        <v>51.77059989929199</v>
       </c>
       <c r="G3" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H3" s="5" t="n">
-        <v>36.06937521766776</v>
+        <v>36.52337919510731</v>
       </c>
       <c r="I3" s="5" t="n">
         <v>1</v>
       </c>
       <c r="J3" s="6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -3759,28 +3759,28 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>269.3299865722656</v>
+        <v>268.3500061035156</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>0.3651874218225215</v>
+        <v>-0.2490457726255446</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>283.7542496490478</v>
+        <v>283.6553997039795</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>-5.0833645996923</v>
+        <v>-5.395770225575269</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>274.9625994873047</v>
+        <v>275.0931994628907</v>
       </c>
       <c r="G5" s="5" t="n">
         <v>1</v>
       </c>
       <c r="H5" s="5" t="n">
-        <v>44.95479787157078</v>
+        <v>42.18255649838467</v>
       </c>
       <c r="I5" s="5" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J5" s="6" t="n">
         <v>1</v>
@@ -3793,28 +3793,28 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>14.53999996185303</v>
+        <v>14.60000038146973</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>-0.4109617674589394</v>
+        <v>0.2747250048093175</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>14.59530001163483</v>
+        <v>14.58445001125336</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>-0.3788894352134996</v>
+        <v>0.1066229457015533</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>14.83380002975464</v>
+        <v>14.82640003204346</v>
       </c>
       <c r="G6" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H6" s="5" t="n">
-        <v>42.25048247858744</v>
+        <v>43.84222986630397</v>
       </c>
       <c r="I6" s="5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J6" s="6" t="n">
         <v>2</v>
@@ -3827,31 +3827,31 @@
         </is>
       </c>
       <c r="B7" s="5" t="n">
-        <v>53.7599983215332</v>
+        <v>53.54999923706055</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>0.392155158663976</v>
+        <v>0.601164188570591</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>53.32190002441406</v>
+        <v>53.31775003433228</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.8216104394602434</v>
+        <v>0.4355945301118664</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>53.55660026550293</v>
+        <v>53.55920028686523</v>
       </c>
       <c r="G7" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>55.65239158334667</v>
+        <v>52.66710461578787</v>
       </c>
       <c r="I7" s="5" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J7" s="6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" hidden="1">
@@ -3861,31 +3861,31 @@
         </is>
       </c>
       <c r="B8" s="5" t="n">
-        <v>123.879997253418</v>
+        <v>123.3000030517578</v>
       </c>
       <c r="C8" s="5" t="n">
-        <v>0.4703926904338296</v>
+        <v>-0.6686491742730616</v>
       </c>
       <c r="D8" s="5" t="n">
-        <v>109.7919190597534</v>
+        <v>109.6834490585327</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>12.8316166748094</v>
+        <v>12.41441084329743</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>122.9902000427246</v>
+        <v>122.9224000549316</v>
       </c>
       <c r="G8" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>54.69947450178652</v>
+        <v>52.03925239240116</v>
       </c>
       <c r="I8" s="5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J8" s="6" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" hidden="1">
@@ -3895,25 +3895,25 @@
         </is>
       </c>
       <c r="B9" s="5" t="n">
-        <v>219.5200042724609</v>
+        <v>219.0200042724609</v>
       </c>
       <c r="C9" s="5" t="n">
-        <v>0.228289649459601</v>
+        <v>0.3804032365220644</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>200.9261502838135</v>
+        <v>200.8452002716064</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>9.254073679500225</v>
+        <v>9.049160236976732</v>
       </c>
       <c r="F9" s="5" t="n">
-        <v>213.5860012817383</v>
+        <v>213.4142010498047</v>
       </c>
       <c r="G9" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H9" s="5" t="n">
-        <v>72.8808700856095</v>
+        <v>71.67936020370283</v>
       </c>
       <c r="I9" s="5" t="n">
         <v>42</v>
@@ -3929,31 +3929,31 @@
         </is>
       </c>
       <c r="B10" s="5" t="n">
-        <v>15.59000015258789</v>
+        <v>15.5600004196167</v>
       </c>
       <c r="C10" s="5" t="n">
-        <v>0.192800335232457</v>
+        <v>-0.2564100056083429</v>
       </c>
       <c r="D10" s="5" t="n">
-        <v>14.06789999961853</v>
+        <v>14.0580999994278</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>10.81966855757173</v>
+        <v>10.68352352202669</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>15.26200002670288</v>
+        <v>15.25200002670288</v>
       </c>
       <c r="G10" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H10" s="5" t="n">
-        <v>61.92270166370393</v>
+        <v>60.88856038271267</v>
       </c>
       <c r="I10" s="5" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="J10" s="6" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" hidden="1">
@@ -3963,31 +3963,31 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>165.3899993896484</v>
+        <v>165.1399993896484</v>
       </c>
       <c r="C11" s="5" t="n">
-        <v>0.1513867027516103</v>
+        <v>-0.006051775480053756</v>
       </c>
       <c r="D11" s="5" t="n">
-        <v>149.1862998199463</v>
+        <v>149.0829498291016</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>10.86138579028937</v>
+        <v>10.77054725503727</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>161.7133999633789</v>
+        <v>161.5844000244141</v>
       </c>
       <c r="G11" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H11" s="5" t="n">
-        <v>71.14954703749706</v>
+        <v>70.09998023185538</v>
       </c>
       <c r="I11" s="5" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J11" s="6" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" hidden="1">
@@ -3997,28 +3997,28 @@
         </is>
       </c>
       <c r="B12" s="5" t="n">
-        <v>23.20999908447266</v>
+        <v>23.04000091552734</v>
       </c>
       <c r="C12" s="5" t="n">
-        <v>0.7378392456171445</v>
+        <v>0.2611025869723616</v>
       </c>
       <c r="D12" s="5" t="n">
-        <v>20.25599998474121</v>
+        <v>20.24144998550415</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>14.58332889986514</v>
+        <v>13.82584218041379</v>
       </c>
       <c r="F12" s="5" t="n">
-        <v>22.25299991607666</v>
+        <v>22.22159992218018</v>
       </c>
       <c r="G12" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H12" s="5" t="n">
-        <v>64.06753381379005</v>
+        <v>61.09090509274157</v>
       </c>
       <c r="I12" s="5" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J12" s="6" t="n">
         <v>35</v>
@@ -4052,7 +4052,7 @@
         <v>62.76382012345815</v>
       </c>
       <c r="I13" s="5" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="J13" s="6" t="n">
         <v>36</v>
@@ -4065,31 +4065,31 @@
         </is>
       </c>
       <c r="B14" s="5" t="n">
-        <v>16.70999908447266</v>
+        <v>16.5</v>
       </c>
       <c r="C14" s="5" t="n">
-        <v>1.272721724076709</v>
+        <v>-0.9603832465638562</v>
       </c>
       <c r="D14" s="5" t="n">
-        <v>14.99219996452332</v>
+        <v>14.9818999671936</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>11.4579522952885</v>
+        <v>10.13289393288324</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>16.16339990615845</v>
+        <v>16.14939992904663</v>
       </c>
       <c r="G14" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>66.97495627020794</v>
+        <v>60.56196194919459</v>
       </c>
       <c r="I14" s="5" t="n">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="J14" s="6" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" hidden="1">
@@ -4099,28 +4099,28 @@
         </is>
       </c>
       <c r="B15" s="5" t="n">
-        <v>220.3099975585938</v>
+        <v>220.1000061035156</v>
       </c>
       <c r="C15" s="5" t="n">
-        <v>0.09540729180141927</v>
+        <v>0.4610022285395976</v>
       </c>
       <c r="D15" s="5" t="n">
-        <v>201.1250499725342</v>
+        <v>201.0297999572754</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>9.538815572043104</v>
+        <v>9.486258331000275</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>214.3655996704101</v>
+        <v>214.1979995727539</v>
       </c>
       <c r="G15" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>76.19705131465869</v>
+        <v>75.71798930902504</v>
       </c>
       <c r="I15" s="5" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J15" s="6" t="n">
         <v>17</v>
@@ -4133,31 +4133,31 @@
         </is>
       </c>
       <c r="B16" s="5" t="n">
-        <v>209.3600006103516</v>
+        <v>209.25</v>
       </c>
       <c r="C16" s="5" t="n">
-        <v>0.05256898941532473</v>
+        <v>0.4753699794856958</v>
       </c>
       <c r="D16" s="5" t="n">
-        <v>191.2304002380371</v>
+        <v>191.1424502563476</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>9.480501191101073</v>
+        <v>9.473327206681564</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>203.7596005249023</v>
+        <v>203.6002005004883</v>
       </c>
       <c r="G16" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>76.07857218761765</v>
+        <v>75.81504231762028</v>
       </c>
       <c r="I16" s="5" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="J16" s="6" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" hidden="1">
@@ -4167,31 +4167,31 @@
         </is>
       </c>
       <c r="B17" s="5" t="n">
-        <v>221.5299987792969</v>
+        <v>221.4299926757812</v>
       </c>
       <c r="C17" s="5" t="n">
-        <v>0.04516375686380858</v>
+        <v>0.5631455654781403</v>
       </c>
       <c r="D17" s="5" t="n">
-        <v>202.2881494903564</v>
+        <v>202.1922495269775</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>9.512099120694042</v>
+        <v>9.514579907889546</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>215.6135992431641</v>
+        <v>215.441399230957</v>
       </c>
       <c r="G17" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>75.32918376700046</v>
+        <v>75.10292531955281</v>
       </c>
       <c r="I17" s="5" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J17" s="6" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" hidden="1">
@@ -4203,24 +4203,14 @@
       <c r="B18" s="5" t="n">
         <v>243.4100036621094</v>
       </c>
-      <c r="C18" s="5" t="n">
-        <v/>
-      </c>
-      <c r="D18" s="5" t="n">
-        <v/>
-      </c>
-      <c r="E18" s="5" t="n">
-        <v/>
-      </c>
-      <c r="F18" s="5" t="n">
-        <v/>
-      </c>
+      <c r="C18" s="5" t="n"/>
+      <c r="D18" s="5" t="n"/>
+      <c r="E18" s="5" t="n"/>
+      <c r="F18" s="5" t="n"/>
       <c r="G18" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H18" s="5" t="n">
-        <v/>
-      </c>
+      <c r="H18" s="5" t="n"/>
       <c r="I18" s="5" t="n">
         <v>47</v>
       </c>
@@ -4235,31 +4225,31 @@
         </is>
       </c>
       <c r="B19" s="5" t="n">
-        <v>34.81999969482422</v>
+        <v>34.41999816894531</v>
       </c>
       <c r="C19" s="5" t="n">
-        <v>1.162119544328744</v>
+        <v>0.3498511211484479</v>
       </c>
       <c r="D19" s="5" t="n">
-        <v>28.72789999961853</v>
+        <v>28.70234999656677</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>21.20621310742026</v>
+        <v>19.92048794981057</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>32.7217998123169</v>
+        <v>32.64379981994629</v>
       </c>
       <c r="G19" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H19" s="5" t="n">
-        <v>64.16636608314603</v>
+        <v>60.68537726206829</v>
       </c>
       <c r="I19" s="5" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="J19" s="6" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" hidden="1">
@@ -4269,31 +4259,31 @@
         </is>
       </c>
       <c r="B20" s="5" t="n">
-        <v>203.3000030517578</v>
+        <v>202.9199981689453</v>
       </c>
       <c r="C20" s="5" t="n">
-        <v>0.1872683255674579</v>
+        <v>0.207406503182872</v>
       </c>
       <c r="D20" s="5" t="n">
-        <v>182.9777008056641</v>
+        <v>182.84580078125</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>11.10643655298607</v>
+        <v>10.97875767555162</v>
       </c>
       <c r="F20" s="5" t="n">
-        <v>199.2066009521484</v>
+        <v>199.0752008056641</v>
       </c>
       <c r="G20" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H20" s="5" t="n">
-        <v>66.05012495866339</v>
+        <v>64.88033430859353</v>
       </c>
       <c r="I20" s="5" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J20" s="6" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" hidden="1">
@@ -4324,7 +4314,7 @@
         <v>65.98258205674995</v>
       </c>
       <c r="I21" s="5" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J21" s="6" t="n">
         <v>42</v>
@@ -4337,28 +4327,28 @@
         </is>
       </c>
       <c r="B22" s="5" t="n">
-        <v>468.5700073242188</v>
+        <v>467.510009765625</v>
       </c>
       <c r="C22" s="5" t="n">
-        <v>0.2267325910572771</v>
+        <v>0.7868806384099036</v>
       </c>
       <c r="D22" s="5" t="n">
-        <v>436.4725498962403</v>
+        <v>436.3054998779297</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>7.353831858523248</v>
+        <v>7.151986371115146</v>
       </c>
       <c r="F22" s="5" t="n">
-        <v>457.5223999023438</v>
+        <v>457.3507995605469</v>
       </c>
       <c r="G22" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H22" s="5" t="n">
-        <v>71.15325751039649</v>
+        <v>70.05285192165391</v>
       </c>
       <c r="I22" s="5" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J22" s="6" t="n">
         <v>9</v>
@@ -4371,28 +4361,28 @@
         </is>
       </c>
       <c r="B23" s="5" t="n">
-        <v>465.6799926757812</v>
+        <v>463.9599914550781</v>
       </c>
       <c r="C23" s="5" t="n">
-        <v>0.3707218838651993</v>
+        <v>0.9157132039321558</v>
       </c>
       <c r="D23" s="5" t="n">
-        <v>432.9366497802735</v>
+        <v>432.7659498596191</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>7.563079474127655</v>
+        <v>7.208062835252576</v>
       </c>
       <c r="F23" s="5" t="n">
-        <v>453.7424005126953</v>
+        <v>453.5490008544922</v>
       </c>
       <c r="G23" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H23" s="5" t="n">
-        <v>72.16029555650377</v>
+        <v>70.43825664160977</v>
       </c>
       <c r="I23" s="5" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J23" s="6" t="n">
         <v>10</v>
@@ -4426,7 +4416,7 @@
         <v>71.85227256399563</v>
       </c>
       <c r="I24" s="5" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="J24" s="6" t="n">
         <v>11</v>
@@ -4473,31 +4463,31 @@
         </is>
       </c>
       <c r="B26" s="5" t="n">
-        <v>537.8400268554688</v>
+        <v>537.1500244140625</v>
       </c>
       <c r="C26" s="5" t="n">
-        <v>0.1284561872930912</v>
+        <v>-0.02977297002813017</v>
       </c>
       <c r="D26" s="5" t="n">
-        <v>495.8315518188476</v>
+        <v>495.3964517211914</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>8.472327927200757</v>
+        <v>8.4283148471903</v>
       </c>
       <c r="F26" s="5" t="n">
-        <v>539.3072033691407</v>
+        <v>539.6252026367188</v>
       </c>
       <c r="G26" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H26" s="5" t="n">
-        <v>54.86353968388604</v>
+        <v>53.82894065531436</v>
       </c>
       <c r="I26" s="5" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J26" s="6" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" hidden="1">
@@ -4507,31 +4497,31 @@
         </is>
       </c>
       <c r="B27" s="5" t="n">
-        <v>98.80999755859375</v>
+        <v>98.61000061035156</v>
       </c>
       <c r="C27" s="5" t="n">
-        <v>0.202816090664526</v>
+        <v>0.1116757465497997</v>
       </c>
       <c r="D27" s="5" t="n">
-        <v>84.58464977264404</v>
+        <v>84.50744979858399</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>16.81788341523689</v>
+        <v>16.68793798106528</v>
       </c>
       <c r="F27" s="5" t="n">
-        <v>95.82439971923829</v>
+        <v>95.65279983520507</v>
       </c>
       <c r="G27" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H27" s="5" t="n">
-        <v>64.23674330983349</v>
+        <v>63.15397140557052</v>
       </c>
       <c r="I27" s="5" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J27" s="6" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" hidden="1">
@@ -4541,25 +4531,25 @@
         </is>
       </c>
       <c r="B28" s="5" t="n">
-        <v>9.869999885559082</v>
+        <v>9.840000152587891</v>
       </c>
       <c r="C28" s="5" t="n">
-        <v>0.3048753303454221</v>
+        <v>0.2036706556540313</v>
       </c>
       <c r="D28" s="5" t="n">
-        <v>8.447199990749359</v>
+        <v>8.439499990940094</v>
       </c>
       <c r="E28" s="5" t="n">
-        <v>16.84344985756049</v>
+        <v>16.59458692044849</v>
       </c>
       <c r="F28" s="5" t="n">
-        <v>9.574200019836425</v>
+        <v>9.55700002670288</v>
       </c>
       <c r="G28" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H28" s="5" t="n">
-        <v>64.70836077594873</v>
+        <v>63.00151186028023</v>
       </c>
       <c r="I28" s="5" t="n">
         <v>23</v>
@@ -4596,10 +4586,10 @@
         <v>69.73185336827612</v>
       </c>
       <c r="I29" s="5" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J29" s="6" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" hidden="1">
@@ -4609,31 +4599,31 @@
         </is>
       </c>
       <c r="B30" s="5" t="n">
-        <v>67.33999633789062</v>
+        <v>66.86000061035156</v>
       </c>
       <c r="C30" s="5" t="n">
-        <v>0.7179116409770758</v>
+        <v>-0.1493406145285925</v>
       </c>
       <c r="D30" s="5" t="n">
-        <v>57.56480005264282</v>
+        <v>57.51675006866455</v>
       </c>
       <c r="E30" s="5" t="n">
-        <v>16.98120427120118</v>
+        <v>16.2443992933065</v>
       </c>
       <c r="F30" s="5" t="n">
-        <v>63.32759994506836</v>
+        <v>63.19180000305176</v>
       </c>
       <c r="G30" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H30" s="5" t="n">
-        <v>73.47293458833873</v>
+        <v>70.98338556558251</v>
       </c>
       <c r="I30" s="5" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J30" s="6" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" hidden="1">
@@ -4664,10 +4654,10 @@
         <v>67.83070521020178</v>
       </c>
       <c r="I31" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="J31" s="6" t="n">
         <v>31</v>
-      </c>
-      <c r="J31" s="6" t="n">
-        <v>30</v>
       </c>
     </row>
     <row r="32" hidden="1">
@@ -4677,31 +4667,31 @@
         </is>
       </c>
       <c r="B32" s="5" t="n">
-        <v>34.29000091552734</v>
+        <v>34.27999877929688</v>
       </c>
       <c r="C32" s="5" t="n">
-        <v>0.02917776133792849</v>
+        <v>0.1460684713093574</v>
       </c>
       <c r="D32" s="5" t="n">
-        <v>30.63380003929138</v>
+        <v>30.61905003547669</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>11.93518555173195</v>
+        <v>11.95644129905546</v>
       </c>
       <c r="F32" s="5" t="n">
-        <v>32.18840003967285</v>
+        <v>32.12300003051758</v>
       </c>
       <c r="G32" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H32" s="5" t="n">
-        <v>81.26150867117445</v>
+        <v>81.17788617325215</v>
       </c>
       <c r="I32" s="5" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J32" s="6" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" hidden="1">
@@ -4711,31 +4701,31 @@
         </is>
       </c>
       <c r="B33" s="5" t="n">
-        <v>34.66999816894531</v>
+        <v>34.52999877929688</v>
       </c>
       <c r="C33" s="5" t="n">
-        <v>0.4054427877141276</v>
+        <v>-0.02895812381398244</v>
       </c>
       <c r="D33" s="5" t="n">
-        <v>30.78040002822876</v>
+        <v>30.76455003738403</v>
       </c>
       <c r="E33" s="5" t="n">
-        <v>12.63660685744629</v>
+        <v>12.23957034098401</v>
       </c>
       <c r="F33" s="5" t="n">
-        <v>32.36759998321534</v>
+        <v>32.29800003051758</v>
       </c>
       <c r="G33" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H33" s="5" t="n">
-        <v>80.2093797295253</v>
+        <v>79.09147129946832</v>
       </c>
       <c r="I33" s="5" t="n">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J33" s="6" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" hidden="1">
@@ -4766,10 +4756,10 @@
         <v>78.69531897069865</v>
       </c>
       <c r="I34" s="5" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J34" s="6" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" hidden="1">
@@ -4779,28 +4769,28 @@
         </is>
       </c>
       <c r="B35" s="5" t="n">
-        <v>43.22000122070312</v>
+        <v>42.83000183105469</v>
       </c>
       <c r="C35" s="5" t="n">
-        <v>0.910575234590949</v>
+        <v>0.1871387860928442</v>
       </c>
       <c r="D35" s="5" t="n">
-        <v>35.47765003204346</v>
+        <v>35.42875001907348</v>
       </c>
       <c r="E35" s="5" t="n">
-        <v>21.82317933027348</v>
+        <v>20.89052480823245</v>
       </c>
       <c r="F35" s="5" t="n">
-        <v>40.47600021362305</v>
+        <v>40.37620018005371</v>
       </c>
       <c r="G35" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H35" s="5" t="n">
-        <v>67.3455174950487</v>
+        <v>64.24159173426844</v>
       </c>
       <c r="I35" s="5" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J35" s="6" t="n">
         <v>47</v>
@@ -4813,31 +4803,31 @@
         </is>
       </c>
       <c r="B36" s="5" t="n">
-        <v>155.3099975585938</v>
+        <v>153.8899993896484</v>
       </c>
       <c r="C36" s="5" t="n">
-        <v>0.9227358337625891</v>
+        <v>0.1105894923206785</v>
       </c>
       <c r="D36" s="5" t="n">
-        <v>128.3001000976562</v>
+        <v>128.1314501190186</v>
       </c>
       <c r="E36" s="5" t="n">
-        <v>21.05212501033031</v>
+        <v>20.10322153281128</v>
       </c>
       <c r="F36" s="5" t="n">
-        <v>145.6436001586914</v>
+        <v>145.2892001342773</v>
       </c>
       <c r="G36" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H36" s="5" t="n">
-        <v>67.82267528169206</v>
+        <v>64.50016406644946</v>
       </c>
       <c r="I36" s="5" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J36" s="6" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" hidden="1">
@@ -4868,7 +4858,7 @@
         <v>68.76644379739099</v>
       </c>
       <c r="I37" s="5" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J37" s="6" t="n">
         <v>48</v>
@@ -4902,10 +4892,10 @@
         <v>78.7802685683757</v>
       </c>
       <c r="I38" s="5" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J38" s="6" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" hidden="1">
@@ -4936,10 +4926,10 @@
         <v>60.99322380240922</v>
       </c>
       <c r="I39" s="5" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J39" s="6" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" hidden="1">
@@ -4949,31 +4939,31 @@
         </is>
       </c>
       <c r="B40" s="5" t="n">
-        <v>48.58000183105469</v>
+        <v>48.11000061035156</v>
       </c>
       <c r="C40" s="5" t="n">
-        <v>0.9769303985458722</v>
+        <v>-0.103819014158979</v>
       </c>
       <c r="D40" s="5" t="n">
-        <v>44.00794998168945</v>
+        <v>43.99054996490479</v>
       </c>
       <c r="E40" s="5" t="n">
-        <v>10.38914980422298</v>
+        <v>9.364399055554504</v>
       </c>
       <c r="F40" s="5" t="n">
-        <v>47.13500022888184</v>
+        <v>47.08660018920899</v>
       </c>
       <c r="G40" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H40" s="5" t="n">
-        <v>63.79195186737026</v>
+        <v>59.12258739279579</v>
       </c>
       <c r="I40" s="5" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J40" s="6" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" hidden="1">
@@ -4983,28 +4973,28 @@
         </is>
       </c>
       <c r="B41" s="5" t="n">
-        <v>47.4900016784668</v>
+        <v>47.15999984741211</v>
       </c>
       <c r="C41" s="5" t="n">
-        <v>0.6997494319813891</v>
+        <v>0.08489158835756072</v>
       </c>
       <c r="D41" s="5" t="n">
-        <v>43.00904996871948</v>
+        <v>42.99249996185303</v>
       </c>
       <c r="E41" s="5" t="n">
-        <v>10.418625180064</v>
+        <v>9.693550943203762</v>
       </c>
       <c r="F41" s="5" t="n">
-        <v>46.14299987792969</v>
+        <v>46.10299987792969</v>
       </c>
       <c r="G41" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H41" s="5" t="n">
-        <v>62.19185242664833</v>
+        <v>58.91542077760771</v>
       </c>
       <c r="I41" s="5" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J41" s="6" t="n">
         <v>19</v>
@@ -5017,31 +5007,31 @@
         </is>
       </c>
       <c r="B42" s="5" t="n">
-        <v>488.510009765625</v>
+        <v>485.3200073242188</v>
       </c>
       <c r="C42" s="5" t="n">
-        <v>0.6572987705563804</v>
+        <v>0.3432170635447207</v>
       </c>
       <c r="D42" s="5" t="n">
-        <v>441.1625993347168</v>
+        <v>440.9880493164063</v>
       </c>
       <c r="E42" s="5" t="n">
-        <v>10.73241714105166</v>
+        <v>10.0528706110139</v>
       </c>
       <c r="F42" s="5" t="n">
-        <v>473.7187994384765</v>
+        <v>473.3061993408203</v>
       </c>
       <c r="G42" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H42" s="5" t="n">
-        <v>62.51669398835828</v>
+        <v>59.58828479368986</v>
       </c>
       <c r="I42" s="5" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J42" s="6" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" hidden="1">
@@ -5072,10 +5062,10 @@
         <v>67.32553551401077</v>
       </c>
       <c r="I43" s="5" t="n">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="J43" s="6" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" hidden="1">
@@ -5085,31 +5075,31 @@
         </is>
       </c>
       <c r="B44" s="5" t="n">
-        <v>237.5299987792969</v>
+        <v>236.3600006103516</v>
       </c>
       <c r="C44" s="5" t="n">
-        <v>0.4950068395346285</v>
+        <v>0.5658859881557676</v>
       </c>
       <c r="D44" s="5" t="n">
-        <v>218.2100498962402</v>
+        <v>218.1072998809815</v>
       </c>
       <c r="E44" s="5" t="n">
-        <v>8.853830926780574</v>
+        <v>8.368679424911676</v>
       </c>
       <c r="F44" s="5" t="n">
-        <v>230.8891998291016</v>
+        <v>230.7265997314453</v>
       </c>
       <c r="G44" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H44" s="5" t="n">
-        <v>69.30413231016833</v>
+        <v>66.83200518208352</v>
       </c>
       <c r="I44" s="5" t="n">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J44" s="6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" hidden="1">
@@ -5119,31 +5109,31 @@
         </is>
       </c>
       <c r="B45" s="5" t="n">
-        <v>499.2200012207031</v>
+        <v>490.6799926757812</v>
       </c>
       <c r="C45" s="5" t="n">
-        <v>1.740443603243613</v>
+        <v>5.447748229219007</v>
       </c>
       <c r="D45" s="5" t="n">
-        <v>412.4296507263184</v>
+        <v>411.9460006713867</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>21.04367383420195</v>
+        <v>19.11269726519359</v>
       </c>
       <c r="F45" s="5" t="n">
-        <v>454.7182019042968</v>
+        <v>453.4668017578125</v>
       </c>
       <c r="G45" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H45" s="5" t="n">
-        <v>68.68529380269804</v>
+        <v>65.91607934705254</v>
       </c>
       <c r="I45" s="5" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J45" s="6" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" hidden="1">
@@ -5153,10 +5143,10 @@
         </is>
       </c>
       <c r="B46" s="5" t="n">
-        <v>122.879997253418</v>
+        <v>121.629997253418</v>
       </c>
       <c r="C46" s="5" t="n">
-        <v>1.027707003392919</v>
+        <v>0.9628920237078065</v>
       </c>
       <c r="D46" s="5" t="n">
         <v/>
@@ -5165,19 +5155,19 @@
         <v/>
       </c>
       <c r="F46" s="5" t="n">
-        <v>114.9191999816895</v>
+        <v>114.6076000976562</v>
       </c>
       <c r="G46" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H46" s="5" t="n">
-        <v>66.61557146608445</v>
+        <v>63.16798148434177</v>
       </c>
       <c r="I46" s="5" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J46" s="6" t="n">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47">
@@ -5208,7 +5198,7 @@
         <v>52.1854555994307</v>
       </c>
       <c r="I47" s="5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J47" s="6" t="n">
         <v>8</v>
@@ -5221,31 +5211,31 @@
         </is>
       </c>
       <c r="B48" s="5" t="n">
-        <v>117.870002746582</v>
+        <v>117.5599975585938</v>
       </c>
       <c r="C48" s="5" t="n">
-        <v>0.2636995529314845</v>
+        <v>0.2900497648438582</v>
       </c>
       <c r="D48" s="5" t="n">
-        <v>106.5627502059937</v>
+        <v>106.4894501876831</v>
       </c>
       <c r="E48" s="5" t="n">
-        <v>10.61088656095176</v>
+        <v>10.39590997173831</v>
       </c>
       <c r="F48" s="5" t="n">
-        <v>113.5013999938965</v>
+        <v>113.3879998779297</v>
       </c>
       <c r="G48" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H48" s="5" t="n">
-        <v>74.24266694545454</v>
+        <v>73.12716062295928</v>
       </c>
       <c r="I48" s="5" t="n">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J48" s="6" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" hidden="1">
@@ -5255,28 +5245,28 @@
         </is>
       </c>
       <c r="B49" s="5" t="n">
-        <v>115.8099975585938</v>
+        <v>115.4499969482422</v>
       </c>
       <c r="C49" s="5" t="n">
-        <v>0.3118238370443338</v>
+        <v>0.4087611563635019</v>
       </c>
       <c r="D49" s="5" t="n">
-        <v>104.5684996795654</v>
+        <v>104.4957497024536</v>
       </c>
       <c r="E49" s="5" t="n">
-        <v>10.7503673797331</v>
+        <v>10.48295961986994</v>
       </c>
       <c r="F49" s="5" t="n">
-        <v>111.2393997192383</v>
+        <v>111.1285997009277</v>
       </c>
       <c r="G49" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H49" s="5" t="n">
-        <v>73.26865055250909</v>
+        <v>72.01605518024627</v>
       </c>
       <c r="I49" s="5" t="n">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="J49" s="6" t="n">
         <v>23</v>
@@ -5289,31 +5279,31 @@
         </is>
       </c>
       <c r="B50" s="5" t="n">
-        <v>64.37999725341797</v>
+        <v>64</v>
       </c>
       <c r="C50" s="5" t="n">
-        <v>0.5937457084655762</v>
+        <v>-0.8059464818994</v>
       </c>
       <c r="D50" s="5" t="n">
-        <v>51.77009986877442</v>
+        <v>51.64069988250733</v>
       </c>
       <c r="E50" s="5" t="n">
-        <v>24.35749093899145</v>
+        <v>23.93325447875899</v>
       </c>
       <c r="F50" s="5" t="n">
-        <v>63.93619956970215</v>
+        <v>63.92519966125488</v>
       </c>
       <c r="G50" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H50" s="5" t="n">
-        <v>55.15049739176025</v>
+        <v>52.56055502176282</v>
       </c>
       <c r="I50" s="5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J50" s="6" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" hidden="1">
@@ -5323,25 +5313,25 @@
         </is>
       </c>
       <c r="B51" s="5" t="n">
-        <v>33.02000045776367</v>
+        <v>33.13000106811523</v>
       </c>
       <c r="C51" s="5" t="n">
-        <v>-0.3320271862515267</v>
+        <v>-0.2709215812183752</v>
       </c>
       <c r="D51" s="5" t="n">
-        <v>29.17820008277893</v>
+        <v>29.14725008010864</v>
       </c>
       <c r="E51" s="5" t="n">
-        <v>13.16668048092585</v>
+        <v>13.66424268862536</v>
       </c>
       <c r="F51" s="5" t="n">
-        <v>32.56779998779297</v>
+        <v>32.54319999694824</v>
       </c>
       <c r="G51" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H51" s="5" t="n">
-        <v>55.84490922597161</v>
+        <v>58.46656451703969</v>
       </c>
       <c r="I51" s="5" t="n">
         <v>12</v>
@@ -5357,31 +5347,31 @@
         </is>
       </c>
       <c r="B52" s="5" t="n">
-        <v>29.51000022888184</v>
+        <v>29.42000007629395</v>
       </c>
       <c r="C52" s="5" t="n">
-        <v>0.30591486184397</v>
+        <v>0.2726650418882093</v>
       </c>
       <c r="D52" s="5" t="n">
-        <v>26.34090003967285</v>
+        <v>26.32480004310608</v>
       </c>
       <c r="E52" s="5" t="n">
-        <v>12.0311006246404</v>
+        <v>11.75773425864419</v>
       </c>
       <c r="F52" s="5" t="n">
-        <v>28.47740005493164</v>
+        <v>28.44360004425049</v>
       </c>
       <c r="G52" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H52" s="5" t="n">
-        <v>70.21969875175114</v>
+        <v>68.75824544257117</v>
       </c>
       <c r="I52" s="5" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J52" s="6" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="53" hidden="1">
@@ -5391,31 +5381,31 @@
         </is>
       </c>
       <c r="B53" s="5" t="n">
-        <v>122.0400009155273</v>
+        <v>121.0100021362305</v>
       </c>
       <c r="C53" s="5" t="n">
-        <v>0.8511683010610449</v>
+        <v>-0.4933792213713928</v>
       </c>
       <c r="D53" s="5" t="n">
-        <v>103.6453500747681</v>
+        <v>103.554400062561</v>
       </c>
       <c r="E53" s="5" t="n">
-        <v>17.74768557150869</v>
+        <v>16.85645618450193</v>
       </c>
       <c r="F53" s="5" t="n">
-        <v>115.595400390625</v>
+        <v>115.3786003112793</v>
       </c>
       <c r="G53" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H53" s="5" t="n">
-        <v>64.05616642827904</v>
+        <v>60.93413773859091</v>
       </c>
       <c r="I53" s="5" t="n">
         <v>19</v>
       </c>
       <c r="J53" s="6" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="54">
@@ -5461,24 +5451,14 @@
       <c r="B55" s="8" t="n">
         <v>69.22000122070312</v>
       </c>
-      <c r="C55" s="8" t="n">
-        <v/>
-      </c>
-      <c r="D55" s="8" t="n">
-        <v/>
-      </c>
-      <c r="E55" s="8" t="n">
-        <v/>
-      </c>
-      <c r="F55" s="8" t="n">
-        <v/>
-      </c>
+      <c r="C55" s="8" t="n"/>
+      <c r="D55" s="8" t="n"/>
+      <c r="E55" s="8" t="n"/>
+      <c r="F55" s="8" t="n"/>
       <c r="G55" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="H55" s="8" t="n">
-        <v/>
-      </c>
+      <c r="H55" s="8" t="n"/>
       <c r="I55" s="8" t="n">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
Commit for Updating the code .
</commit_message>
<xml_diff>
--- a/buy_low.xlsx
+++ b/buy_low.xlsx
@@ -1475,7 +1475,7 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.140625" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="11.42578125" customWidth="1" min="3" max="3"/>
@@ -2241,7 +2241,7 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="12.28515625" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="12" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -3586,7 +3586,7 @@
       <selection activeCell="A1" sqref="A1:J55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="11.42578125" customWidth="1" min="3" max="3"/>
@@ -4910,12 +4910,8 @@
       <c r="C39" s="5" t="n">
         <v>-1.652017900438751</v>
       </c>
-      <c r="D39" s="5" t="n">
-        <v/>
-      </c>
-      <c r="E39" s="5" t="n">
-        <v/>
-      </c>
+      <c r="D39" s="5" t="n"/>
+      <c r="E39" s="5" t="n"/>
       <c r="F39" s="5" t="n">
         <v>184.0725991821289</v>
       </c>
@@ -5148,12 +5144,8 @@
       <c r="C46" s="5" t="n">
         <v>1.027707003392919</v>
       </c>
-      <c r="D46" s="5" t="n">
-        <v/>
-      </c>
-      <c r="E46" s="5" t="n">
-        <v/>
-      </c>
+      <c r="D46" s="5" t="n"/>
+      <c r="E46" s="5" t="n"/>
       <c r="F46" s="5" t="n">
         <v>114.9191999816895</v>
       </c>

</xml_diff>

<commit_message>
Commit to merge in main.
</commit_message>
<xml_diff>
--- a/buy_low.xlsx
+++ b/buy_low.xlsx
@@ -1475,7 +1475,7 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.140625" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="11.42578125" customWidth="1" min="3" max="3"/>
@@ -2241,7 +2241,7 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="12.28515625" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="12" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -3586,7 +3586,7 @@
       <selection activeCell="A1" sqref="A1:J55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="15.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="11.42578125" customWidth="1" min="3" max="3"/>
@@ -4910,8 +4910,12 @@
       <c r="C39" s="5" t="n">
         <v>-1.652017900438751</v>
       </c>
-      <c r="D39" s="5" t="n"/>
-      <c r="E39" s="5" t="n"/>
+      <c r="D39" s="5" t="n">
+        <v/>
+      </c>
+      <c r="E39" s="5" t="n">
+        <v/>
+      </c>
       <c r="F39" s="5" t="n">
         <v>184.0725991821289</v>
       </c>
@@ -5144,8 +5148,12 @@
       <c r="C46" s="5" t="n">
         <v>1.027707003392919</v>
       </c>
-      <c r="D46" s="5" t="n"/>
-      <c r="E46" s="5" t="n"/>
+      <c r="D46" s="5" t="n">
+        <v/>
+      </c>
+      <c r="E46" s="5" t="n">
+        <v/>
+      </c>
       <c r="F46" s="5" t="n">
         <v>114.9191999816895</v>
       </c>

</xml_diff>